<commit_message>
dpv: added Applicability concepts
</commit_message>
<xml_diff>
--- a/code/vocab_csv/context_status.xlsx
+++ b/code/vocab_csv/context_status.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="333">
   <si>
     <t>Term</t>
   </si>
@@ -356,6 +356,54 @@
   </si>
   <si>
     <t>Indication that the specified context has a subsequent occurence or that it applies after the initial occurnece or not at the beginning</t>
+  </si>
+  <si>
+    <t>Applicability</t>
+  </si>
+  <si>
+    <t>Concept provided to represent indication of cases where the information or context is not applicable (N/A) or not available or this is not known or determined yet. If the information is applicable and available, this concept should not be used.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These concepts are useful in closed-world interpretations, for example in forms where a field must have a value to explicitly denote it is not applicable or the information is not available yet. </t>
+  </si>
+  <si>
+    <t>UnknownApplicability</t>
+  </si>
+  <si>
+    <t>Unknown Applicability</t>
+  </si>
+  <si>
+    <t>Concept indicating information or context availability is unknown i.e. it is not known if the information exists or is applicable and therefore statements about its availability cannot be made (yet)</t>
+  </si>
+  <si>
+    <t>dpv:Applicability</t>
+  </si>
+  <si>
+    <t>This concept is useful when describing situations where it cannot be stated whether the context applies or whether the information is not available yet. For example, if a form field asks about whether a process X was completed and it is not yet known whether X applies or not and therefore it is also unclear whether X was completed or not. Using UnknownApplicability is a signal that the applicability of X should be assessed, and if applicable, then information about X should be identified and used here.</t>
+  </si>
+  <si>
+    <t>NotApplicable</t>
+  </si>
+  <si>
+    <t>Not Applicable</t>
+  </si>
+  <si>
+    <t>Concept indicating the information or context is not applicable</t>
+  </si>
+  <si>
+    <t>This concept is useful when describing situations where information must be provided to indicate the context does not apply and leaving a blank field or having no value or triple is not an option. For example, if in a form a field asks about whether a process X was completed and the response to that would be "not applicable (N/A)" - then this is represented using the concept NotApplicable. If instead the value was left blank the open-world interpretation creates an ambiguity as to whether the information was not available or was it not provided as it is not applicable.</t>
+  </si>
+  <si>
+    <t>NotAvailable</t>
+  </si>
+  <si>
+    <t>Not Available</t>
+  </si>
+  <si>
+    <t>Concept indicating the information or context is applicable but information is not yet available</t>
+  </si>
+  <si>
+    <t>This concept is useful when describing situations where information is required but is not available (yet). For example, if in a form a field asks about whether a process X was completed, and it is correct to interpret that process X is applicable and must be completed, but the information is not yet available as to whether this was done - then NotAvailable is useful to represent this.</t>
   </si>
   <si>
     <t>domain</t>
@@ -504,7 +552,7 @@
     <t>is applicable for</t>
   </si>
   <si>
-    <t>Indicates applicability for specified context or criteria</t>
+    <t>Indicates the concept or information is applicable for specified context</t>
   </si>
   <si>
     <t>Harshvardhan J Pandit, Beatriz Esteves, Georg P Krog, Paul Ryan</t>
@@ -516,7 +564,7 @@
     <t>is not applicable for</t>
   </si>
   <si>
-    <t>Indicates non-applicability for specified context or criteria</t>
+    <t>Indicates the concept or information is not applicable for specified context</t>
   </si>
   <si>
     <t>hasImportance</t>
@@ -535,6 +583,15 @@
   </si>
   <si>
     <t>Indicates the necessity for specified context or criteria</t>
+  </si>
+  <si>
+    <t>hasApplicability</t>
+  </si>
+  <si>
+    <t>has applicability</t>
+  </si>
+  <si>
+    <t>Indicates situations where the context is not applicable, information is not available, or this is unknown. An appropriate instance of dpv:Applicability should be used with this relation to express the situation</t>
   </si>
   <si>
     <t>The status or state of something</t>
@@ -1157,7 +1214,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1297,9 +1354,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -3124,16 +3178,204 @@
       <c r="B37" s="20"/>
     </row>
     <row r="38">
-      <c r="B38" s="20"/>
+      <c r="A38" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="J38" s="11"/>
+      <c r="K38" s="17">
+        <v>45162.0</v>
+      </c>
+      <c r="L38" s="11"/>
+      <c r="M38" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N38" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="O38" s="11"/>
+      <c r="P38" s="11"/>
+      <c r="Q38" s="11"/>
+      <c r="R38" s="11"/>
+      <c r="S38" s="11"/>
+      <c r="T38" s="11"/>
+      <c r="U38" s="11"/>
+      <c r="V38" s="11"/>
+      <c r="W38" s="11"/>
+      <c r="X38" s="11"/>
+      <c r="Y38" s="11"/>
+      <c r="Z38" s="11"/>
+      <c r="AA38" s="11"/>
+      <c r="AB38" s="11"/>
+      <c r="AC38" s="11"/>
+      <c r="AD38" s="11"/>
     </row>
     <row r="39">
-      <c r="B39" s="20"/>
+      <c r="A39" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="J39" s="11"/>
+      <c r="K39" s="17">
+        <v>45162.0</v>
+      </c>
+      <c r="L39" s="11"/>
+      <c r="M39" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N39" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="O39" s="11"/>
+      <c r="P39" s="11"/>
+      <c r="Q39" s="11"/>
+      <c r="R39" s="11"/>
+      <c r="S39" s="11"/>
+      <c r="T39" s="11"/>
+      <c r="U39" s="11"/>
+      <c r="V39" s="11"/>
+      <c r="W39" s="11"/>
+      <c r="X39" s="11"/>
+      <c r="Y39" s="11"/>
+      <c r="Z39" s="11"/>
+      <c r="AA39" s="11"/>
+      <c r="AB39" s="11"/>
+      <c r="AC39" s="11"/>
+      <c r="AD39" s="11"/>
     </row>
     <row r="40">
-      <c r="B40" s="20"/>
+      <c r="A40" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J40" s="11"/>
+      <c r="K40" s="17">
+        <v>45162.0</v>
+      </c>
+      <c r="L40" s="11"/>
+      <c r="M40" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N40" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="O40" s="11"/>
+      <c r="P40" s="11"/>
+      <c r="Q40" s="11"/>
+      <c r="R40" s="11"/>
+      <c r="S40" s="11"/>
+      <c r="T40" s="11"/>
+      <c r="U40" s="11"/>
+      <c r="V40" s="11"/>
+      <c r="W40" s="11"/>
+      <c r="X40" s="11"/>
+      <c r="Y40" s="11"/>
+      <c r="Z40" s="11"/>
+      <c r="AA40" s="11"/>
+      <c r="AB40" s="11"/>
+      <c r="AC40" s="11"/>
+      <c r="AD40" s="11"/>
     </row>
     <row r="41">
-      <c r="B41" s="20"/>
+      <c r="A41" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="J41" s="11"/>
+      <c r="K41" s="17">
+        <v>45162.0</v>
+      </c>
+      <c r="L41" s="11"/>
+      <c r="M41" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N41" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="O41" s="11"/>
+      <c r="P41" s="11"/>
+      <c r="Q41" s="11"/>
+      <c r="R41" s="11"/>
+      <c r="S41" s="11"/>
+      <c r="T41" s="11"/>
+      <c r="U41" s="11"/>
+      <c r="V41" s="11"/>
+      <c r="W41" s="11"/>
+      <c r="X41" s="11"/>
+      <c r="Y41" s="11"/>
+      <c r="Z41" s="11"/>
+      <c r="AA41" s="11"/>
+      <c r="AB41" s="11"/>
+      <c r="AC41" s="11"/>
+      <c r="AD41" s="11"/>
     </row>
     <row r="42">
       <c r="B42" s="20"/>
@@ -5742,13 +5984,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="G1" s="21" t="s">
         <v>6</v>
@@ -5763,7 +6005,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="L1" s="26" t="s">
         <v>11</v>
@@ -5780,13 +6022,13 @@
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>17</v>
@@ -5795,7 +6037,7 @@
         <v>25</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
@@ -5830,13 +6072,13 @@
     </row>
     <row r="3">
       <c r="A3" s="28" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="D3" s="28" t="s">
         <v>17</v>
@@ -5845,13 +6087,13 @@
         <v>75</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="G3" s="30"/>
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
       <c r="J3" s="31" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="K3" s="32">
         <v>43560.0</v>
@@ -5861,7 +6103,7 @@
         <v>20</v>
       </c>
       <c r="N3" s="34" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
       <c r="O3" s="35" t="s">
         <v>22</v>
@@ -5884,13 +6126,13 @@
     </row>
     <row r="4">
       <c r="A4" s="36" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="D4" s="38" t="s">
         <v>17</v>
@@ -5899,7 +6141,7 @@
         <v>17</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="G4" s="39"/>
       <c r="H4" s="39"/>
@@ -5913,10 +6155,10 @@
         <v>20</v>
       </c>
       <c r="N4" s="36" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="O4" s="42" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="P4" s="43"/>
       <c r="Q4" s="43"/>
@@ -5936,13 +6178,13 @@
     </row>
     <row r="5">
       <c r="A5" s="12" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>17</v>
@@ -5951,7 +6193,7 @@
         <v>60</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -5968,7 +6210,7 @@
         <v>50</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
@@ -5988,13 +6230,13 @@
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="D6" s="44" t="s">
         <v>17</v>
@@ -6003,7 +6245,7 @@
         <v>17</v>
       </c>
       <c r="F6" s="44" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
@@ -6017,10 +6259,10 @@
         <v>20</v>
       </c>
       <c r="N6" s="12" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
       <c r="P6" s="11"/>
       <c r="Q6" s="11"/>
@@ -6040,13 +6282,13 @@
     </row>
     <row r="7">
       <c r="A7" s="12" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="D7" s="44" t="s">
         <v>17</v>
@@ -6055,7 +6297,7 @@
         <v>17</v>
       </c>
       <c r="F7" s="44" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -6069,10 +6311,10 @@
         <v>20</v>
       </c>
       <c r="N7" s="19" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
@@ -6092,22 +6334,22 @@
     </row>
     <row r="8">
       <c r="A8" s="12" t="s">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>145</v>
+        <v>161</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
@@ -6144,22 +6386,22 @@
     </row>
     <row r="9">
       <c r="A9" s="12" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
@@ -6196,13 +6438,13 @@
     </row>
     <row r="10">
       <c r="A10" s="12" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>154</v>
+        <v>170</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>17</v>
@@ -6211,7 +6453,7 @@
         <v>17</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
@@ -6228,7 +6470,7 @@
         <v>50</v>
       </c>
       <c r="O10" s="45" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="P10" s="11"/>
       <c r="Q10" s="11"/>
@@ -6248,34 +6490,36 @@
     </row>
     <row r="11">
       <c r="A11" s="12" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="C11" s="46" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
+      <c r="K11" s="17">
+        <v>45395.0</v>
+      </c>
       <c r="L11" s="11"/>
       <c r="M11" s="12" t="s">
-        <v>95</v>
+        <v>20</v>
       </c>
       <c r="N11" s="12" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="O11" s="11"/>
       <c r="P11" s="11"/>
@@ -6296,34 +6540,36 @@
     </row>
     <row r="12">
       <c r="A12" s="12" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="C12" s="46" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
+      <c r="K12" s="17">
+        <v>45395.0</v>
+      </c>
       <c r="L12" s="11"/>
       <c r="M12" s="12" t="s">
-        <v>95</v>
+        <v>20</v>
       </c>
       <c r="N12" s="12" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="O12" s="11"/>
       <c r="P12" s="11"/>
@@ -6344,13 +6590,13 @@
     </row>
     <row r="13">
       <c r="A13" s="12" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>17</v>
@@ -6359,18 +6605,22 @@
         <v>33</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
+      <c r="K13" s="17">
+        <v>45395.0</v>
+      </c>
       <c r="L13" s="11"/>
       <c r="M13" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="N13" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="N13" s="12" t="s">
+        <v>50</v>
+      </c>
       <c r="O13" s="11"/>
       <c r="P13" s="11"/>
       <c r="Q13" s="11"/>
@@ -6390,13 +6640,13 @@
     </row>
     <row r="14">
       <c r="A14" s="47" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>17</v>
@@ -6405,18 +6655,22 @@
         <v>42</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
+      <c r="K14" s="17">
+        <v>45395.0</v>
+      </c>
       <c r="L14" s="11"/>
       <c r="M14" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="N14" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="N14" s="12" t="s">
+        <v>50</v>
+      </c>
       <c r="O14" s="11"/>
       <c r="P14" s="11"/>
       <c r="Q14" s="11"/>
@@ -6435,8 +6689,54 @@
       <c r="AD14" s="11"/>
     </row>
     <row r="15">
-      <c r="A15" s="48"/>
-      <c r="B15" s="20"/>
+      <c r="A15" s="47" t="s">
+        <v>185</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="17">
+        <v>45162.0</v>
+      </c>
+      <c r="L15" s="11"/>
+      <c r="M15" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N15" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+      <c r="X15" s="11"/>
+      <c r="Y15" s="11"/>
+      <c r="Z15" s="11"/>
+      <c r="AA15" s="11"/>
+      <c r="AB15" s="11"/>
+      <c r="AC15" s="11"/>
+      <c r="AD15" s="11"/>
     </row>
     <row r="16">
       <c r="B16" s="20"/>
@@ -9425,7 +9725,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>169</v>
+        <v>188</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>25</v>
@@ -9449,7 +9749,7 @@
         <v>50</v>
       </c>
       <c r="O2" s="45" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
@@ -9481,16 +9781,16 @@
     </row>
     <row r="4">
       <c r="A4" s="15" t="s">
-        <v>170</v>
+        <v>189</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>171</v>
+        <v>190</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>173</v>
+        <v>192</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>26</v>
@@ -9511,7 +9811,7 @@
         <v>50</v>
       </c>
       <c r="O4" s="45" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
@@ -9531,17 +9831,17 @@
     </row>
     <row r="5">
       <c r="A5" s="12" t="s">
-        <v>174</v>
+        <v>193</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>175</v>
+        <v>194</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>176</v>
+        <v>195</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="12" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
@@ -9559,7 +9859,7 @@
         <v>50</v>
       </c>
       <c r="O5" s="45" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
@@ -9579,17 +9879,17 @@
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>179</v>
+        <v>198</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="12" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
@@ -9607,7 +9907,7 @@
         <v>50</v>
       </c>
       <c r="O6" s="45" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="P6" s="11"/>
       <c r="Q6" s="11"/>
@@ -9627,23 +9927,23 @@
     </row>
     <row r="7">
       <c r="A7" s="12" t="s">
-        <v>181</v>
+        <v>200</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>182</v>
+        <v>201</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>183</v>
+        <v>202</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="12" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
-      <c r="J7" s="49"/>
+      <c r="J7" s="48"/>
       <c r="K7" s="17">
         <v>44699.0</v>
       </c>
@@ -9655,7 +9955,7 @@
         <v>50</v>
       </c>
       <c r="O7" s="45" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
@@ -9674,23 +9974,23 @@
       <c r="AD7" s="11"/>
     </row>
     <row r="8">
-      <c r="A8" s="50" t="s">
-        <v>184</v>
-      </c>
-      <c r="B8" s="51" t="s">
-        <v>185</v>
-      </c>
-      <c r="C8" s="50" t="s">
-        <v>186</v>
+      <c r="A8" s="49" t="s">
+        <v>203</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>204</v>
+      </c>
+      <c r="C8" s="49" t="s">
+        <v>205</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="52"/>
+        <v>196</v>
+      </c>
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
       <c r="J8" s="11"/>
       <c r="K8" s="17">
         <v>44699.0</v>
@@ -9703,43 +10003,43 @@
         <v>50</v>
       </c>
       <c r="O8" s="45" t="s">
-        <v>155</v>
-      </c>
-      <c r="P8" s="52"/>
-      <c r="Q8" s="52"/>
-      <c r="R8" s="52"/>
-      <c r="S8" s="52"/>
-      <c r="T8" s="52"/>
-      <c r="U8" s="52"/>
-      <c r="V8" s="52"/>
-      <c r="W8" s="52"/>
-      <c r="X8" s="52"/>
-      <c r="Y8" s="52"/>
-      <c r="Z8" s="52"/>
-      <c r="AA8" s="52"/>
-      <c r="AB8" s="52"/>
+        <v>171</v>
+      </c>
+      <c r="P8" s="51"/>
+      <c r="Q8" s="51"/>
+      <c r="R8" s="51"/>
+      <c r="S8" s="51"/>
+      <c r="T8" s="51"/>
+      <c r="U8" s="51"/>
+      <c r="V8" s="51"/>
+      <c r="W8" s="51"/>
+      <c r="X8" s="51"/>
+      <c r="Y8" s="51"/>
+      <c r="Z8" s="51"/>
+      <c r="AA8" s="51"/>
+      <c r="AB8" s="51"/>
       <c r="AC8" s="11"/>
       <c r="AD8" s="11"/>
     </row>
     <row r="9">
       <c r="A9" s="12" t="s">
-        <v>187</v>
+        <v>206</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>188</v>
+        <v>207</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>189</v>
+        <v>208</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="19" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="12" t="s">
-        <v>190</v>
+        <v>209</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="14">
@@ -9783,16 +10083,16 @@
     </row>
     <row r="11">
       <c r="A11" s="15" t="s">
-        <v>191</v>
+        <v>210</v>
       </c>
       <c r="B11" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="D11" s="44" t="s">
         <v>192</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="D11" s="44" t="s">
-        <v>173</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>26</v>
@@ -9813,7 +10113,7 @@
         <v>50</v>
       </c>
       <c r="O11" s="45" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="P11" s="11"/>
       <c r="Q11" s="11"/>
@@ -9833,17 +10133,17 @@
     </row>
     <row r="12">
       <c r="A12" s="12" t="s">
-        <v>194</v>
+        <v>213</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>194</v>
+        <v>213</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>195</v>
+        <v>214</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="12" t="s">
-        <v>196</v>
+        <v>215</v>
       </c>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
@@ -9861,7 +10161,7 @@
         <v>50</v>
       </c>
       <c r="O12" s="45" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="P12" s="11"/>
       <c r="Q12" s="11"/>
@@ -9881,23 +10181,23 @@
     </row>
     <row r="13">
       <c r="A13" s="12" t="s">
-        <v>197</v>
+        <v>216</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>197</v>
+        <v>216</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>198</v>
+        <v>217</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="12" t="s">
-        <v>196</v>
+        <v>215</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="12" t="s">
-        <v>199</v>
+        <v>218</v>
       </c>
       <c r="J13" s="11"/>
       <c r="K13" s="17">
@@ -9905,13 +10205,13 @@
       </c>
       <c r="L13" s="11"/>
       <c r="M13" s="12" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="N13" s="12" t="s">
         <v>50</v>
       </c>
       <c r="O13" s="45" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="P13" s="11"/>
       <c r="Q13" s="11"/>
@@ -9931,17 +10231,17 @@
     </row>
     <row r="14">
       <c r="A14" s="12" t="s">
-        <v>201</v>
+        <v>220</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>202</v>
+        <v>221</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>203</v>
+        <v>222</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="12" t="s">
-        <v>196</v>
+        <v>215</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
@@ -9959,7 +10259,7 @@
         <v>50</v>
       </c>
       <c r="O14" s="45" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="P14" s="11"/>
       <c r="Q14" s="11"/>
@@ -9979,23 +10279,23 @@
     </row>
     <row r="15">
       <c r="A15" s="12" t="s">
-        <v>204</v>
+        <v>223</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>205</v>
+        <v>224</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>206</v>
+        <v>225</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="12" t="s">
-        <v>196</v>
+        <v>215</v>
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
       <c r="I15" s="12" t="s">
-        <v>207</v>
+        <v>226</v>
       </c>
       <c r="J15" s="11"/>
       <c r="K15" s="17">
@@ -10011,7 +10311,7 @@
         <v>50</v>
       </c>
       <c r="O15" s="45" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="P15" s="11"/>
       <c r="Q15" s="11"/>
@@ -10031,23 +10331,23 @@
     </row>
     <row r="16">
       <c r="A16" s="12" t="s">
-        <v>208</v>
+        <v>227</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>209</v>
+        <v>228</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>210</v>
+        <v>229</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="12" t="s">
-        <v>196</v>
+        <v>215</v>
       </c>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
       <c r="I16" s="12" t="s">
-        <v>211</v>
+        <v>230</v>
       </c>
       <c r="J16" s="11"/>
       <c r="K16" s="17">
@@ -10063,7 +10363,7 @@
         <v>50</v>
       </c>
       <c r="O16" s="45" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="P16" s="11"/>
       <c r="Q16" s="11"/>
@@ -10083,17 +10383,17 @@
     </row>
     <row r="17">
       <c r="A17" s="12" t="s">
-        <v>212</v>
+        <v>231</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>213</v>
+        <v>232</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>214</v>
+        <v>233</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="12" t="s">
-        <v>196</v>
+        <v>215</v>
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
@@ -10129,17 +10429,17 @@
     </row>
     <row r="18">
       <c r="A18" s="12" t="s">
-        <v>215</v>
+        <v>234</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>216</v>
+        <v>235</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>217</v>
+        <v>236</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="12" t="s">
-        <v>196</v>
+        <v>215</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
@@ -10182,16 +10482,16 @@
     </row>
     <row r="20">
       <c r="A20" s="15" t="s">
-        <v>218</v>
+        <v>237</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>218</v>
+        <v>237</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>196</v>
+        <v>215</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>26</v>
@@ -10212,7 +10512,7 @@
         <v>50</v>
       </c>
       <c r="O20" s="16" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="P20" s="11"/>
       <c r="Q20" s="11"/>
@@ -10232,17 +10532,17 @@
     </row>
     <row r="21">
       <c r="A21" s="12" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>222</v>
+        <v>241</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="12" t="s">
-        <v>223</v>
+        <v>242</v>
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
@@ -10260,7 +10560,7 @@
         <v>50</v>
       </c>
       <c r="O21" s="16" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="P21" s="11"/>
       <c r="Q21" s="11"/>
@@ -10280,17 +10580,17 @@
     </row>
     <row r="22">
       <c r="A22" s="12" t="s">
-        <v>224</v>
+        <v>243</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>224</v>
+        <v>243</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>225</v>
+        <v>244</v>
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="12" t="s">
-        <v>223</v>
+        <v>242</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
@@ -10308,7 +10608,7 @@
         <v>50</v>
       </c>
       <c r="O22" s="16" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="P22" s="11"/>
       <c r="Q22" s="11"/>
@@ -10328,17 +10628,17 @@
     </row>
     <row r="23">
       <c r="A23" s="13" t="s">
-        <v>226</v>
+        <v>245</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>227</v>
+        <v>246</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>228</v>
+        <v>247</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="12" t="s">
-        <v>223</v>
+        <v>242</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
@@ -10356,7 +10656,7 @@
         <v>50</v>
       </c>
       <c r="O23" s="16" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="P23" s="11"/>
       <c r="Q23" s="11"/>
@@ -10379,16 +10679,16 @@
     </row>
     <row r="25">
       <c r="A25" s="15" t="s">
-        <v>229</v>
+        <v>248</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>230</v>
+        <v>249</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>231</v>
+        <v>250</v>
       </c>
       <c r="D25" s="44" t="s">
-        <v>173</v>
+        <v>192</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>26</v>
@@ -10409,7 +10709,7 @@
         <v>50</v>
       </c>
       <c r="O25" s="45" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="P25" s="11"/>
       <c r="Q25" s="11"/>
@@ -10429,17 +10729,17 @@
     </row>
     <row r="26">
       <c r="A26" s="12" t="s">
-        <v>232</v>
+        <v>251</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>233</v>
+        <v>252</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>234</v>
+        <v>253</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="12" t="s">
-        <v>235</v>
+        <v>254</v>
       </c>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
@@ -10457,7 +10757,7 @@
         <v>50</v>
       </c>
       <c r="O26" s="45" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="P26" s="11"/>
       <c r="Q26" s="11"/>
@@ -10477,23 +10777,23 @@
     </row>
     <row r="27">
       <c r="A27" s="12" t="s">
-        <v>236</v>
+        <v>255</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>237</v>
+        <v>256</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>238</v>
+        <v>257</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="12" t="s">
-        <v>235</v>
+        <v>254</v>
       </c>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
       <c r="I27" s="12" t="s">
-        <v>239</v>
+        <v>258</v>
       </c>
       <c r="J27" s="11"/>
       <c r="K27" s="17">
@@ -10504,10 +10804,10 @@
         <v>20</v>
       </c>
       <c r="N27" s="12" t="s">
-        <v>240</v>
+        <v>259</v>
       </c>
       <c r="O27" s="45" t="s">
-        <v>241</v>
+        <v>260</v>
       </c>
       <c r="P27" s="11"/>
       <c r="Q27" s="11"/>
@@ -10527,17 +10827,17 @@
     </row>
     <row r="28">
       <c r="A28" s="12" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>243</v>
+        <v>262</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>244</v>
+        <v>263</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="12" t="s">
-        <v>235</v>
+        <v>254</v>
       </c>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
@@ -10555,7 +10855,7 @@
         <v>50</v>
       </c>
       <c r="O28" s="45" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="P28" s="11"/>
       <c r="Q28" s="11"/>
@@ -10575,17 +10875,17 @@
     </row>
     <row r="29">
       <c r="A29" s="12" t="s">
-        <v>245</v>
+        <v>264</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>246</v>
+        <v>265</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>247</v>
+        <v>266</v>
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="12" t="s">
-        <v>235</v>
+        <v>254</v>
       </c>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
@@ -10603,7 +10903,7 @@
         <v>50</v>
       </c>
       <c r="O29" s="45" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="P29" s="11"/>
       <c r="Q29" s="11"/>
@@ -10623,17 +10923,17 @@
     </row>
     <row r="30">
       <c r="A30" s="12" t="s">
-        <v>248</v>
+        <v>267</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>249</v>
+        <v>268</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>250</v>
+        <v>269</v>
       </c>
       <c r="D30" s="11"/>
       <c r="E30" s="12" t="s">
-        <v>235</v>
+        <v>254</v>
       </c>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
@@ -10651,7 +10951,7 @@
         <v>50</v>
       </c>
       <c r="O30" s="45" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="P30" s="11"/>
       <c r="Q30" s="11"/>
@@ -10671,17 +10971,17 @@
     </row>
     <row r="31">
       <c r="A31" s="12" t="s">
-        <v>251</v>
+        <v>270</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>252</v>
+        <v>271</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>253</v>
+        <v>272</v>
       </c>
       <c r="D31" s="11"/>
       <c r="E31" s="12" t="s">
-        <v>235</v>
+        <v>254</v>
       </c>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
@@ -10699,7 +10999,7 @@
         <v>50</v>
       </c>
       <c r="O31" s="45" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="P31" s="11"/>
       <c r="Q31" s="11"/>
@@ -10722,16 +11022,16 @@
     </row>
     <row r="33">
       <c r="A33" s="15" t="s">
-        <v>254</v>
+        <v>273</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>255</v>
+        <v>274</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>256</v>
+        <v>275</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>173</v>
+        <v>192</v>
       </c>
       <c r="E33" s="12" t="s">
         <v>26</v>
@@ -10770,17 +11070,17 @@
     </row>
     <row r="34">
       <c r="A34" s="12" t="s">
-        <v>257</v>
+        <v>276</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>257</v>
+        <v>276</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>258</v>
+        <v>277</v>
       </c>
       <c r="D34" s="11"/>
       <c r="E34" s="12" t="s">
-        <v>259</v>
+        <v>278</v>
       </c>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
@@ -10816,17 +11116,17 @@
     </row>
     <row r="35">
       <c r="A35" s="12" t="s">
-        <v>260</v>
+        <v>279</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>260</v>
+        <v>279</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>261</v>
+        <v>280</v>
       </c>
       <c r="D35" s="11"/>
       <c r="E35" s="12" t="s">
-        <v>259</v>
+        <v>278</v>
       </c>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
@@ -10865,16 +11165,16 @@
     </row>
     <row r="37">
       <c r="A37" s="15" t="s">
-        <v>262</v>
+        <v>281</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>263</v>
+        <v>282</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>173</v>
+        <v>192</v>
       </c>
       <c r="E37" s="12" t="s">
         <v>26</v>
@@ -10913,17 +11213,17 @@
     </row>
     <row r="38">
       <c r="A38" s="12" t="s">
-        <v>265</v>
+        <v>284</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>267</v>
+        <v>286</v>
       </c>
       <c r="D38" s="11"/>
       <c r="E38" s="12" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
@@ -10959,17 +11259,17 @@
     </row>
     <row r="39">
       <c r="A39" s="12" t="s">
-        <v>269</v>
+        <v>288</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>270</v>
+        <v>289</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>271</v>
+        <v>290</v>
       </c>
       <c r="D39" s="11"/>
       <c r="E39" s="12" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
       <c r="F39" s="11"/>
       <c r="G39" s="11"/>
@@ -11005,17 +11305,17 @@
     </row>
     <row r="40">
       <c r="A40" s="12" t="s">
-        <v>272</v>
+        <v>291</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>273</v>
+        <v>292</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>274</v>
+        <v>293</v>
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="12" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
@@ -11051,17 +11351,17 @@
     </row>
     <row r="41">
       <c r="A41" s="12" t="s">
-        <v>275</v>
+        <v>294</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>276</v>
+        <v>295</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>277</v>
+        <v>296</v>
       </c>
       <c r="D41" s="11"/>
       <c r="E41" s="12" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
       <c r="F41" s="11"/>
       <c r="G41" s="11"/>
@@ -11097,17 +11397,17 @@
     </row>
     <row r="42">
       <c r="A42" s="12" t="s">
-        <v>278</v>
+        <v>297</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>279</v>
+        <v>298</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>280</v>
+        <v>299</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="12" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
@@ -11143,17 +11443,17 @@
     </row>
     <row r="43">
       <c r="A43" s="12" t="s">
-        <v>281</v>
+        <v>300</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>282</v>
+        <v>301</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>283</v>
+        <v>302</v>
       </c>
       <c r="D43" s="11"/>
       <c r="E43" s="12" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
       <c r="F43" s="11"/>
       <c r="G43" s="11"/>
@@ -11189,17 +11489,17 @@
     </row>
     <row r="44">
       <c r="A44" s="12" t="s">
-        <v>284</v>
+        <v>303</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>285</v>
+        <v>304</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>286</v>
+        <v>305</v>
       </c>
       <c r="D44" s="11"/>
       <c r="E44" s="12" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
       <c r="F44" s="11"/>
       <c r="G44" s="11"/>
@@ -11235,17 +11535,17 @@
     </row>
     <row r="45">
       <c r="A45" s="12" t="s">
-        <v>287</v>
+        <v>306</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>288</v>
+        <v>307</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>289</v>
+        <v>308</v>
       </c>
       <c r="D45" s="11"/>
       <c r="E45" s="12" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
@@ -11281,17 +11581,17 @@
     </row>
     <row r="46">
       <c r="A46" s="12" t="s">
-        <v>290</v>
+        <v>309</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>291</v>
+        <v>310</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>292</v>
+        <v>311</v>
       </c>
       <c r="D46" s="11"/>
       <c r="E46" s="12" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
       <c r="F46" s="11"/>
       <c r="G46" s="11"/>
@@ -11327,17 +11627,17 @@
     </row>
     <row r="47">
       <c r="A47" s="19" t="s">
-        <v>293</v>
+        <v>312</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>294</v>
+        <v>313</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>295</v>
+        <v>314</v>
       </c>
       <c r="D47" s="11"/>
       <c r="E47" s="12" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
       <c r="F47" s="11"/>
       <c r="G47" s="11"/>
@@ -13921,13 +14221,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="G1" s="21" t="s">
         <v>6</v>
@@ -13942,7 +14242,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="L1" s="26" t="s">
         <v>11</v>
@@ -13959,22 +14259,22 @@
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>296</v>
+        <v>315</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>297</v>
+        <v>316</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>298</v>
+        <v>317</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>173</v>
+        <v>192</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
@@ -13991,7 +14291,7 @@
         <v>50</v>
       </c>
       <c r="O2" s="16" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
@@ -14009,22 +14309,22 @@
     </row>
     <row r="3">
       <c r="A3" s="12" t="s">
-        <v>299</v>
+        <v>318</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>300</v>
+        <v>319</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>301</v>
+        <v>320</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>196</v>
+        <v>215</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>302</v>
+        <v>321</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -14041,7 +14341,7 @@
         <v>50</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="P3" s="11"/>
       <c r="Q3" s="11"/>
@@ -14059,22 +14359,22 @@
     </row>
     <row r="4">
       <c r="A4" s="12" t="s">
-        <v>303</v>
+        <v>322</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>304</v>
+        <v>323</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>302</v>
+        <v>321</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
@@ -14091,7 +14391,7 @@
         <v>50</v>
       </c>
       <c r="O4" s="16" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
@@ -14109,22 +14409,22 @@
     </row>
     <row r="5">
       <c r="A5" s="12" t="s">
-        <v>306</v>
+        <v>325</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>307</v>
+        <v>326</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>308</v>
+        <v>327</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>235</v>
+        <v>254</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>302</v>
+        <v>321</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -14141,7 +14441,7 @@
         <v>50</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>309</v>
+        <v>328</v>
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
@@ -14159,22 +14459,22 @@
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>310</v>
+        <v>329</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>311</v>
+        <v>330</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>312</v>
+        <v>331</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>223</v>
+        <v>242</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>313</v>
+        <v>332</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>

</xml_diff>

<commit_message>
fix missing contributors, fix inconsistent names
In 300.py HTML output - fixed error where only one contributor was added
and the rest were not.

In CSVs and other outputs - fixed inconsisten names for contributors
e.g. Harsh, Harshvardhan Pandit --> Harshvardhan J. Pandit
This was done for all contributors that were identified in concept docs.
</commit_message>
<xml_diff>
--- a/code/vocab_csv/context_status.xlsx
+++ b/code/vocab_csv/context_status.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="386">
   <si>
     <t>Term</t>
   </si>
@@ -79,7 +79,7 @@
     <t>accepted</t>
   </si>
   <si>
-    <t>Harshvardhan J. Pandit, Javier Fernandez, Axel Polleres, Elmar Kiesling, Fajar Ekaputra, Simon Steyskal</t>
+    <t>Harshvardhan J. Pandit, Javier Fernández, Axel Polleres, Elmar Kiesling, Fajar Ekaputra, Simon Steyskal</t>
   </si>
   <si>
     <t>https://www.w3.org/2019/04/05-dpvcg-minutes.html</t>
@@ -100,7 +100,7 @@
     <t>Importance can be used to express importance, desirability, relevance, or significance as a context.</t>
   </si>
   <si>
-    <t>Harshvardhan J. Pandit, Paul Ryan, Georg P Krog, Julian Flake, Beatriz Esteves</t>
+    <t>Harshvardhan J. Pandit, Paul Ryan, Georg P. Krog, Julian Flake, Beatriz Esteves</t>
   </si>
   <si>
     <t>https://www.w3.org/2022/02/09-dpvcg-minutes.html</t>
@@ -404,6 +404,165 @@
   </si>
   <si>
     <t>This concept is useful when describing situations where information is required but is not available (yet). For example, if in a form a field asks about whether a process X was completed, and it is correct to interpret that process X is applicable and must be completed, but the information is not yet available as to whether this was done - then NotAvailable is useful to represent this.</t>
+  </si>
+  <si>
+    <t>EntityInformedStatus</t>
+  </si>
+  <si>
+    <t>Entity Informed Status</t>
+  </si>
+  <si>
+    <t>Status indicating whether an entity is informed or uninformed about specified context</t>
+  </si>
+  <si>
+    <t>EntityInformed</t>
+  </si>
+  <si>
+    <t>Entity Informed</t>
+  </si>
+  <si>
+    <t>Status indicating entity has been informed about specified context</t>
+  </si>
+  <si>
+    <t>dpv:EntityInformedStatus</t>
+  </si>
+  <si>
+    <t>DataSubjectInformed</t>
+  </si>
+  <si>
+    <t>DataSubject Informed</t>
+  </si>
+  <si>
+    <t>Status indicating DataSubject has been informed about the specified context</t>
+  </si>
+  <si>
+    <t>dpv:EntityInformed</t>
+  </si>
+  <si>
+    <t>ControllerInformed</t>
+  </si>
+  <si>
+    <t>Controller Informed</t>
+  </si>
+  <si>
+    <t>Status indicating Controller has been informed about the specified context</t>
+  </si>
+  <si>
+    <t>RecipientInformed</t>
+  </si>
+  <si>
+    <t>Recipient Informed</t>
+  </si>
+  <si>
+    <t>Status indicating Recipient has been informed about the specified context</t>
+  </si>
+  <si>
+    <t>AuthorityInformed</t>
+  </si>
+  <si>
+    <t>Authority Informed</t>
+  </si>
+  <si>
+    <t>Status indicating Authority has been informed about the specified context</t>
+  </si>
+  <si>
+    <t>EntityUninformed</t>
+  </si>
+  <si>
+    <t>Entity Uninformed</t>
+  </si>
+  <si>
+    <t>Status indicating entity is uninformed i.e. has been not been informed about specified context</t>
+  </si>
+  <si>
+    <t>DataSubjectUninformed</t>
+  </si>
+  <si>
+    <t>DataSubject Uninformed</t>
+  </si>
+  <si>
+    <t>Status indicating DataSubject is uninformed i.e. has not been informed about the specified context</t>
+  </si>
+  <si>
+    <t>dpv:EntityUninformed</t>
+  </si>
+  <si>
+    <t>ControllerUninformed</t>
+  </si>
+  <si>
+    <t>Controller Uninformed</t>
+  </si>
+  <si>
+    <t>Status indicating Controller is uninformed i.e. has not been informed about the specified context</t>
+  </si>
+  <si>
+    <t>RecipientUninformed</t>
+  </si>
+  <si>
+    <t>Recipient Uninformed</t>
+  </si>
+  <si>
+    <t>Status indicating Recipient is uninformed i.e. has not been informed about the specified context</t>
+  </si>
+  <si>
+    <t>AuthorityUninformed</t>
+  </si>
+  <si>
+    <t>Authority Uninformed</t>
+  </si>
+  <si>
+    <t>Status indicating Authority is uninformed i.e. has not been informed about the specified context</t>
+  </si>
+  <si>
+    <t>IntentionStatus</t>
+  </si>
+  <si>
+    <t>Intention Status</t>
+  </si>
+  <si>
+    <t>Status indicating whether the specified context was intended or unintended</t>
+  </si>
+  <si>
+    <t>Intention is associated with the goal or purpose for what is about to happen i.e. an ex-ante indication of whether the specified context is/was planned or intended. Intention and Expectation are closely related terms. We recommend using Intention when the entity has the ability to control the implementation and Expectation for when the entity does not have control or for what happens after or beyond the exercise of control.</t>
+  </si>
+  <si>
+    <t>Intended</t>
+  </si>
+  <si>
+    <t>Status indicating the specified context was intended</t>
+  </si>
+  <si>
+    <t>dpv:IntentionStatus</t>
+  </si>
+  <si>
+    <t>Unintended</t>
+  </si>
+  <si>
+    <t>Status indicating the specified context was unintended i.e. not intended</t>
+  </si>
+  <si>
+    <t>ExpectationStatus</t>
+  </si>
+  <si>
+    <t>Expectation Status</t>
+  </si>
+  <si>
+    <t>Expectation is associated with the outcome of a goal or purpose for what is expected to happen i.e. an ex-post indication of what was expected to happen in the specified context. Intention and Expectation are closely related terms. We recommend using Intention when the entity has the ability to control the implementation and Expectation for when the entity does not have control or for what happens after or beyond the exercise of control.</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
+  <si>
+    <t>Status indicating the specified context was expected</t>
+  </si>
+  <si>
+    <t>dpv:ExpectationStatus</t>
+  </si>
+  <si>
+    <t>Unexpected</t>
+  </si>
+  <si>
+    <t>Status indicating the specified context was unexpected i.e. not expected</t>
   </si>
   <si>
     <t>domain</t>
@@ -468,7 +627,7 @@
     <t>Indicates an identifier associated for identification or reference</t>
   </si>
   <si>
-    <t>Harshvardhan J.Pandit, Georg P Krog, Paul Ryan, Beatriz Esteves</t>
+    <t>Harshvardhan J. Pandit, Georg P. Krog, Paul Ryan, Beatriz Esteves</t>
   </si>
   <si>
     <t>https://www.w3.org/2020/11/25-dpvcg-minutes.html</t>
@@ -555,7 +714,7 @@
     <t>Indicates the concept or information is applicable for specified context</t>
   </si>
   <si>
-    <t>Harshvardhan J Pandit, Beatriz Esteves, Georg P Krog, Paul Ryan</t>
+    <t>Harshvardhan J. Pandit, Beatriz Esteves, Georg P. Krog, Paul Ryan</t>
   </si>
   <si>
     <t>isNotApplicableFor</t>
@@ -1214,7 +1373,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1336,6 +1495,9 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="14" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -3178,7 +3340,7 @@
       <c r="B37" s="20"/>
     </row>
     <row r="38">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="15" t="s">
         <v>114</v>
       </c>
       <c r="B38" s="12" t="s">
@@ -3381,67 +3543,729 @@
       <c r="B42" s="20"/>
     </row>
     <row r="43">
-      <c r="B43" s="20"/>
+      <c r="A43" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="11"/>
+      <c r="M43" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="N43" s="11"/>
+      <c r="O43" s="11"/>
+      <c r="P43" s="11"/>
+      <c r="Q43" s="11"/>
+      <c r="R43" s="11"/>
+      <c r="S43" s="11"/>
+      <c r="T43" s="11"/>
+      <c r="U43" s="11"/>
+      <c r="V43" s="11"/>
+      <c r="W43" s="11"/>
+      <c r="X43" s="11"/>
+      <c r="Y43" s="11"/>
+      <c r="Z43" s="11"/>
+      <c r="AA43" s="11"/>
+      <c r="AB43" s="11"/>
     </row>
     <row r="44">
-      <c r="B44" s="20"/>
+      <c r="A44" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="N44" s="11"/>
+      <c r="O44" s="11"/>
+      <c r="P44" s="11"/>
+      <c r="Q44" s="11"/>
+      <c r="R44" s="11"/>
+      <c r="S44" s="11"/>
+      <c r="T44" s="11"/>
+      <c r="U44" s="11"/>
+      <c r="V44" s="11"/>
+      <c r="W44" s="11"/>
+      <c r="X44" s="11"/>
+      <c r="Y44" s="11"/>
+      <c r="Z44" s="11"/>
+      <c r="AA44" s="11"/>
+      <c r="AB44" s="11"/>
     </row>
     <row r="45">
-      <c r="B45" s="20"/>
+      <c r="A45" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11"/>
+      <c r="M45" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="N45" s="11"/>
+      <c r="O45" s="11"/>
+      <c r="P45" s="11"/>
+      <c r="Q45" s="11"/>
+      <c r="R45" s="11"/>
+      <c r="S45" s="11"/>
+      <c r="T45" s="11"/>
+      <c r="U45" s="11"/>
+      <c r="V45" s="11"/>
+      <c r="W45" s="11"/>
+      <c r="X45" s="11"/>
+      <c r="Y45" s="11"/>
+      <c r="Z45" s="11"/>
+      <c r="AA45" s="11"/>
+      <c r="AB45" s="11"/>
     </row>
     <row r="46">
-      <c r="B46" s="20"/>
+      <c r="A46" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="11"/>
+      <c r="K46" s="11"/>
+      <c r="L46" s="11"/>
+      <c r="M46" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="N46" s="11"/>
+      <c r="O46" s="11"/>
+      <c r="P46" s="11"/>
+      <c r="Q46" s="11"/>
+      <c r="R46" s="11"/>
+      <c r="S46" s="11"/>
+      <c r="T46" s="11"/>
+      <c r="U46" s="11"/>
+      <c r="V46" s="11"/>
+      <c r="W46" s="11"/>
+      <c r="X46" s="11"/>
+      <c r="Y46" s="11"/>
+      <c r="Z46" s="11"/>
+      <c r="AA46" s="11"/>
+      <c r="AB46" s="11"/>
     </row>
     <row r="47">
-      <c r="B47" s="20"/>
+      <c r="A47" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="11"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="11"/>
+      <c r="M47" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="N47" s="11"/>
+      <c r="O47" s="11"/>
+      <c r="P47" s="11"/>
+      <c r="Q47" s="11"/>
+      <c r="R47" s="11"/>
+      <c r="S47" s="11"/>
+      <c r="T47" s="11"/>
+      <c r="U47" s="11"/>
+      <c r="V47" s="11"/>
+      <c r="W47" s="11"/>
+      <c r="X47" s="11"/>
+      <c r="Y47" s="11"/>
+      <c r="Z47" s="11"/>
+      <c r="AA47" s="11"/>
+      <c r="AB47" s="11"/>
     </row>
     <row r="48">
-      <c r="B48" s="20"/>
+      <c r="A48" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="11"/>
+      <c r="M48" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="N48" s="11"/>
+      <c r="O48" s="11"/>
+      <c r="P48" s="11"/>
+      <c r="Q48" s="11"/>
+      <c r="R48" s="11"/>
+      <c r="S48" s="11"/>
+      <c r="T48" s="11"/>
+      <c r="U48" s="11"/>
+      <c r="V48" s="11"/>
+      <c r="W48" s="11"/>
+      <c r="X48" s="11"/>
+      <c r="Y48" s="11"/>
+      <c r="Z48" s="11"/>
+      <c r="AA48" s="11"/>
+      <c r="AB48" s="11"/>
     </row>
     <row r="49">
-      <c r="B49" s="20"/>
+      <c r="A49" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="11"/>
+      <c r="K49" s="11"/>
+      <c r="L49" s="11"/>
+      <c r="M49" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="N49" s="11"/>
+      <c r="O49" s="11"/>
+      <c r="P49" s="11"/>
+      <c r="Q49" s="11"/>
+      <c r="R49" s="11"/>
+      <c r="S49" s="11"/>
+      <c r="T49" s="11"/>
+      <c r="U49" s="11"/>
+      <c r="V49" s="11"/>
+      <c r="W49" s="11"/>
+      <c r="X49" s="11"/>
+      <c r="Y49" s="11"/>
+      <c r="Z49" s="11"/>
+      <c r="AA49" s="11"/>
+      <c r="AB49" s="11"/>
     </row>
     <row r="50">
-      <c r="B50" s="20"/>
+      <c r="A50" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="11"/>
+      <c r="L50" s="11"/>
+      <c r="M50" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="N50" s="11"/>
+      <c r="O50" s="11"/>
+      <c r="P50" s="11"/>
+      <c r="Q50" s="11"/>
+      <c r="R50" s="11"/>
+      <c r="S50" s="11"/>
+      <c r="T50" s="11"/>
+      <c r="U50" s="11"/>
+      <c r="V50" s="11"/>
+      <c r="W50" s="11"/>
+      <c r="X50" s="11"/>
+      <c r="Y50" s="11"/>
+      <c r="Z50" s="11"/>
+      <c r="AA50" s="11"/>
+      <c r="AB50" s="11"/>
     </row>
     <row r="51">
-      <c r="B51" s="20"/>
+      <c r="A51" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="11"/>
+      <c r="L51" s="11"/>
+      <c r="M51" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="N51" s="11"/>
+      <c r="O51" s="11"/>
+      <c r="P51" s="11"/>
+      <c r="Q51" s="11"/>
+      <c r="R51" s="11"/>
+      <c r="S51" s="11"/>
+      <c r="T51" s="11"/>
+      <c r="U51" s="11"/>
+      <c r="V51" s="11"/>
+      <c r="W51" s="11"/>
+      <c r="X51" s="11"/>
+      <c r="Y51" s="11"/>
+      <c r="Z51" s="11"/>
+      <c r="AA51" s="11"/>
+      <c r="AB51" s="11"/>
     </row>
     <row r="52">
-      <c r="B52" s="20"/>
+      <c r="A52" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="11"/>
+      <c r="K52" s="11"/>
+      <c r="L52" s="11"/>
+      <c r="M52" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="N52" s="11"/>
+      <c r="O52" s="11"/>
+      <c r="P52" s="11"/>
+      <c r="Q52" s="11"/>
+      <c r="R52" s="11"/>
+      <c r="S52" s="11"/>
+      <c r="T52" s="11"/>
+      <c r="U52" s="11"/>
+      <c r="V52" s="11"/>
+      <c r="W52" s="11"/>
+      <c r="X52" s="11"/>
+      <c r="Y52" s="11"/>
+      <c r="Z52" s="11"/>
+      <c r="AA52" s="11"/>
+      <c r="AB52" s="11"/>
     </row>
     <row r="53">
-      <c r="B53" s="20"/>
+      <c r="A53" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="11"/>
+      <c r="K53" s="11"/>
+      <c r="L53" s="11"/>
+      <c r="M53" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="N53" s="11"/>
+      <c r="O53" s="11"/>
+      <c r="P53" s="11"/>
+      <c r="Q53" s="11"/>
+      <c r="R53" s="11"/>
+      <c r="S53" s="11"/>
+      <c r="T53" s="11"/>
+      <c r="U53" s="11"/>
+      <c r="V53" s="11"/>
+      <c r="W53" s="11"/>
+      <c r="X53" s="11"/>
+      <c r="Y53" s="11"/>
+      <c r="Z53" s="11"/>
+      <c r="AA53" s="11"/>
+      <c r="AB53" s="11"/>
     </row>
     <row r="54">
       <c r="B54" s="20"/>
     </row>
     <row r="55">
-      <c r="B55" s="20"/>
+      <c r="A55" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="J55" s="11"/>
+      <c r="K55" s="11"/>
+      <c r="L55" s="11"/>
+      <c r="M55" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="N55" s="11"/>
+      <c r="O55" s="11"/>
+      <c r="P55" s="11"/>
+      <c r="Q55" s="11"/>
+      <c r="R55" s="11"/>
+      <c r="S55" s="11"/>
+      <c r="T55" s="11"/>
+      <c r="U55" s="11"/>
+      <c r="V55" s="11"/>
+      <c r="W55" s="11"/>
+      <c r="X55" s="11"/>
+      <c r="Y55" s="11"/>
+      <c r="Z55" s="11"/>
+      <c r="AA55" s="11"/>
+      <c r="AB55" s="11"/>
     </row>
     <row r="56">
-      <c r="B56" s="20"/>
+      <c r="A56" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
+      <c r="J56" s="11"/>
+      <c r="K56" s="11"/>
+      <c r="L56" s="11"/>
+      <c r="M56" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="N56" s="11"/>
+      <c r="O56" s="11"/>
+      <c r="P56" s="11"/>
+      <c r="Q56" s="11"/>
+      <c r="R56" s="11"/>
+      <c r="S56" s="11"/>
+      <c r="T56" s="11"/>
+      <c r="U56" s="11"/>
+      <c r="V56" s="11"/>
+      <c r="W56" s="11"/>
+      <c r="X56" s="11"/>
+      <c r="Y56" s="11"/>
+      <c r="Z56" s="11"/>
+      <c r="AA56" s="11"/>
+      <c r="AB56" s="11"/>
     </row>
     <row r="57">
-      <c r="B57" s="20"/>
+      <c r="A57" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="E57" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="11"/>
+      <c r="J57" s="11"/>
+      <c r="K57" s="11"/>
+      <c r="L57" s="11"/>
+      <c r="M57" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="N57" s="11"/>
+      <c r="O57" s="11"/>
+      <c r="P57" s="11"/>
+      <c r="Q57" s="11"/>
+      <c r="R57" s="11"/>
+      <c r="S57" s="11"/>
+      <c r="T57" s="11"/>
+      <c r="U57" s="11"/>
+      <c r="V57" s="11"/>
+      <c r="W57" s="11"/>
+      <c r="X57" s="11"/>
+      <c r="Y57" s="11"/>
+      <c r="Z57" s="11"/>
+      <c r="AA57" s="11"/>
+      <c r="AB57" s="11"/>
     </row>
     <row r="58">
       <c r="B58" s="20"/>
     </row>
     <row r="59">
-      <c r="B59" s="20"/>
+      <c r="A59" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
+      <c r="I59" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="J59" s="11"/>
+      <c r="K59" s="11"/>
+      <c r="L59" s="11"/>
+      <c r="M59" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="N59" s="11"/>
+      <c r="O59" s="11"/>
+      <c r="P59" s="11"/>
+      <c r="Q59" s="11"/>
+      <c r="R59" s="11"/>
+      <c r="S59" s="11"/>
+      <c r="T59" s="11"/>
+      <c r="U59" s="11"/>
+      <c r="V59" s="11"/>
+      <c r="W59" s="11"/>
+      <c r="X59" s="11"/>
+      <c r="Y59" s="11"/>
+      <c r="Z59" s="11"/>
+      <c r="AA59" s="11"/>
+      <c r="AB59" s="11"/>
     </row>
     <row r="60">
-      <c r="B60" s="20"/>
+      <c r="A60" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="E60" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11"/>
+      <c r="I60" s="11"/>
+      <c r="J60" s="11"/>
+      <c r="K60" s="11"/>
+      <c r="L60" s="11"/>
+      <c r="M60" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="N60" s="11"/>
+      <c r="O60" s="11"/>
+      <c r="P60" s="11"/>
+      <c r="Q60" s="11"/>
+      <c r="R60" s="11"/>
+      <c r="S60" s="11"/>
+      <c r="T60" s="11"/>
+      <c r="U60" s="11"/>
+      <c r="V60" s="11"/>
+      <c r="W60" s="11"/>
+      <c r="X60" s="11"/>
+      <c r="Y60" s="11"/>
+      <c r="Z60" s="11"/>
+      <c r="AA60" s="11"/>
+      <c r="AB60" s="11"/>
     </row>
     <row r="61">
-      <c r="B61" s="20"/>
+      <c r="A61" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="B61" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="E61" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="11"/>
+      <c r="I61" s="11"/>
+      <c r="J61" s="11"/>
+      <c r="K61" s="11"/>
+      <c r="L61" s="11"/>
+      <c r="M61" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="N61" s="11"/>
+      <c r="O61" s="11"/>
+      <c r="P61" s="11"/>
+      <c r="Q61" s="11"/>
+      <c r="R61" s="11"/>
+      <c r="S61" s="11"/>
+      <c r="T61" s="11"/>
+      <c r="U61" s="11"/>
+      <c r="V61" s="11"/>
+      <c r="W61" s="11"/>
+      <c r="X61" s="11"/>
+      <c r="Y61" s="11"/>
+      <c r="Z61" s="11"/>
+      <c r="AA61" s="11"/>
+      <c r="AB61" s="11"/>
     </row>
     <row r="62">
       <c r="B62" s="20"/>
-    </row>
-    <row r="63">
-      <c r="B63" s="20"/>
     </row>
     <row r="64">
       <c r="B64" s="20"/>
@@ -5984,13 +6808,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>130</v>
+        <v>183</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>131</v>
+        <v>184</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>132</v>
+        <v>185</v>
       </c>
       <c r="G1" s="21" t="s">
         <v>6</v>
@@ -6005,7 +6829,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>133</v>
+        <v>186</v>
       </c>
       <c r="L1" s="26" t="s">
         <v>11</v>
@@ -6022,13 +6846,13 @@
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>134</v>
+        <v>187</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>135</v>
+        <v>188</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>136</v>
+        <v>189</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>17</v>
@@ -6037,7 +6861,7 @@
         <v>25</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>137</v>
+        <v>190</v>
       </c>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
@@ -6072,13 +6896,13 @@
     </row>
     <row r="3">
       <c r="A3" s="28" t="s">
-        <v>138</v>
+        <v>191</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>139</v>
+        <v>192</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>140</v>
+        <v>193</v>
       </c>
       <c r="D3" s="28" t="s">
         <v>17</v>
@@ -6087,13 +6911,13 @@
         <v>75</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>137</v>
+        <v>190</v>
       </c>
       <c r="G3" s="30"/>
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
       <c r="J3" s="31" t="s">
-        <v>141</v>
+        <v>194</v>
       </c>
       <c r="K3" s="32">
         <v>43560.0</v>
@@ -6103,7 +6927,7 @@
         <v>20</v>
       </c>
       <c r="N3" s="34" t="s">
-        <v>142</v>
+        <v>195</v>
       </c>
       <c r="O3" s="35" t="s">
         <v>22</v>
@@ -6126,13 +6950,13 @@
     </row>
     <row r="4">
       <c r="A4" s="36" t="s">
-        <v>143</v>
+        <v>196</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>144</v>
+        <v>197</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>145</v>
+        <v>198</v>
       </c>
       <c r="D4" s="38" t="s">
         <v>17</v>
@@ -6141,7 +6965,7 @@
         <v>17</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>137</v>
+        <v>190</v>
       </c>
       <c r="G4" s="39"/>
       <c r="H4" s="39"/>
@@ -6154,14 +6978,14 @@
       <c r="M4" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="N4" s="36" t="s">
-        <v>146</v>
-      </c>
-      <c r="O4" s="42" t="s">
-        <v>147</v>
-      </c>
-      <c r="P4" s="43"/>
-      <c r="Q4" s="43"/>
+      <c r="N4" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="O4" s="43" t="s">
+        <v>200</v>
+      </c>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="44"/>
       <c r="R4" s="39"/>
       <c r="S4" s="39"/>
       <c r="T4" s="39"/>
@@ -6178,13 +7002,13 @@
     </row>
     <row r="5">
       <c r="A5" s="12" t="s">
-        <v>148</v>
+        <v>201</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>149</v>
+        <v>202</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>150</v>
+        <v>203</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>17</v>
@@ -6193,7 +7017,7 @@
         <v>60</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>137</v>
+        <v>190</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -6210,7 +7034,7 @@
         <v>50</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>151</v>
+        <v>204</v>
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
@@ -6230,22 +7054,22 @@
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>152</v>
+        <v>205</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>153</v>
+        <v>206</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="D6" s="44" t="s">
+        <v>207</v>
+      </c>
+      <c r="D6" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="44" t="s">
+      <c r="E6" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="44" t="s">
-        <v>137</v>
+      <c r="F6" s="45" t="s">
+        <v>190</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
@@ -6259,10 +7083,10 @@
         <v>20</v>
       </c>
       <c r="N6" s="12" t="s">
-        <v>155</v>
+        <v>208</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>156</v>
+        <v>209</v>
       </c>
       <c r="P6" s="11"/>
       <c r="Q6" s="11"/>
@@ -6282,22 +7106,22 @@
     </row>
     <row r="7">
       <c r="A7" s="12" t="s">
-        <v>157</v>
+        <v>210</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>158</v>
+        <v>211</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="D7" s="44" t="s">
+        <v>212</v>
+      </c>
+      <c r="D7" s="45" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="44" t="s">
-        <v>137</v>
+      <c r="F7" s="45" t="s">
+        <v>190</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -6311,10 +7135,10 @@
         <v>20</v>
       </c>
       <c r="N7" s="19" t="s">
-        <v>155</v>
+        <v>208</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>156</v>
+        <v>209</v>
       </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
@@ -6334,22 +7158,22 @@
     </row>
     <row r="8">
       <c r="A8" s="12" t="s">
-        <v>160</v>
+        <v>213</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>161</v>
+        <v>214</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>162</v>
+        <v>215</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>137</v>
+        <v>190</v>
       </c>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
@@ -6386,22 +7210,22 @@
     </row>
     <row r="9">
       <c r="A9" s="12" t="s">
-        <v>164</v>
+        <v>217</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>165</v>
+        <v>218</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>166</v>
+        <v>219</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>167</v>
+        <v>220</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>137</v>
+        <v>190</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
@@ -6438,13 +7262,13 @@
     </row>
     <row r="10">
       <c r="A10" s="12" t="s">
-        <v>168</v>
+        <v>221</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>170</v>
+        <v>223</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>17</v>
@@ -6453,7 +7277,7 @@
         <v>17</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>137</v>
+        <v>190</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
@@ -6469,8 +7293,8 @@
       <c r="N10" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O10" s="45" t="s">
-        <v>171</v>
+      <c r="O10" s="46" t="s">
+        <v>224</v>
       </c>
       <c r="P10" s="11"/>
       <c r="Q10" s="11"/>
@@ -6490,22 +7314,22 @@
     </row>
     <row r="11">
       <c r="A11" s="12" t="s">
-        <v>172</v>
+        <v>225</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="C11" s="46" t="s">
-        <v>174</v>
+        <v>226</v>
+      </c>
+      <c r="C11" s="47" t="s">
+        <v>227</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>137</v>
+        <v>190</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -6519,7 +7343,7 @@
         <v>20</v>
       </c>
       <c r="N11" s="12" t="s">
-        <v>175</v>
+        <v>228</v>
       </c>
       <c r="O11" s="11"/>
       <c r="P11" s="11"/>
@@ -6540,22 +7364,22 @@
     </row>
     <row r="12">
       <c r="A12" s="12" t="s">
-        <v>176</v>
+        <v>229</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="C12" s="46" t="s">
-        <v>178</v>
+        <v>230</v>
+      </c>
+      <c r="C12" s="47" t="s">
+        <v>231</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>137</v>
+        <v>190</v>
       </c>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
@@ -6569,7 +7393,7 @@
         <v>20</v>
       </c>
       <c r="N12" s="12" t="s">
-        <v>175</v>
+        <v>228</v>
       </c>
       <c r="O12" s="11"/>
       <c r="P12" s="11"/>
@@ -6590,13 +7414,13 @@
     </row>
     <row r="13">
       <c r="A13" s="12" t="s">
-        <v>179</v>
+        <v>232</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>180</v>
+        <v>233</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>181</v>
+        <v>234</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>17</v>
@@ -6605,7 +7429,7 @@
         <v>33</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>137</v>
+        <v>190</v>
       </c>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
@@ -6639,14 +7463,14 @@
       <c r="AD13" s="11"/>
     </row>
     <row r="14">
-      <c r="A14" s="47" t="s">
-        <v>182</v>
+      <c r="A14" s="48" t="s">
+        <v>235</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>183</v>
+        <v>236</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>184</v>
+        <v>237</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>17</v>
@@ -6655,7 +7479,7 @@
         <v>42</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>137</v>
+        <v>190</v>
       </c>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
@@ -6689,14 +7513,14 @@
       <c r="AD14" s="11"/>
     </row>
     <row r="15">
-      <c r="A15" s="47" t="s">
-        <v>185</v>
+      <c r="A15" s="48" t="s">
+        <v>238</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>186</v>
+        <v>239</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>187</v>
+        <v>240</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>17</v>
@@ -6705,7 +7529,7 @@
         <v>120</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>137</v>
+        <v>190</v>
       </c>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
@@ -9725,7 +10549,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>188</v>
+        <v>241</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>25</v>
@@ -9748,8 +10572,8 @@
       <c r="N2" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O2" s="45" t="s">
-        <v>171</v>
+      <c r="O2" s="46" t="s">
+        <v>224</v>
       </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
@@ -9781,16 +10605,16 @@
     </row>
     <row r="4">
       <c r="A4" s="15" t="s">
-        <v>189</v>
+        <v>242</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>190</v>
+        <v>243</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>191</v>
+        <v>244</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>192</v>
+        <v>245</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>26</v>
@@ -9810,8 +10634,8 @@
       <c r="N4" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O4" s="45" t="s">
-        <v>171</v>
+      <c r="O4" s="46" t="s">
+        <v>224</v>
       </c>
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
@@ -9831,17 +10655,17 @@
     </row>
     <row r="5">
       <c r="A5" s="12" t="s">
-        <v>193</v>
+        <v>246</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>194</v>
+        <v>247</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>195</v>
+        <v>248</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="12" t="s">
-        <v>196</v>
+        <v>249</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
@@ -9858,8 +10682,8 @@
       <c r="N5" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O5" s="45" t="s">
-        <v>171</v>
+      <c r="O5" s="46" t="s">
+        <v>224</v>
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
@@ -9879,17 +10703,17 @@
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>197</v>
+        <v>250</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>198</v>
+        <v>251</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>199</v>
+        <v>252</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="12" t="s">
-        <v>196</v>
+        <v>249</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
@@ -9906,8 +10730,8 @@
       <c r="N6" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O6" s="45" t="s">
-        <v>171</v>
+      <c r="O6" s="46" t="s">
+        <v>224</v>
       </c>
       <c r="P6" s="11"/>
       <c r="Q6" s="11"/>
@@ -9927,23 +10751,23 @@
     </row>
     <row r="7">
       <c r="A7" s="12" t="s">
-        <v>200</v>
+        <v>253</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>201</v>
+        <v>254</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>202</v>
+        <v>255</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="12" t="s">
-        <v>196</v>
+        <v>249</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
-      <c r="J7" s="48"/>
+      <c r="J7" s="49"/>
       <c r="K7" s="17">
         <v>44699.0</v>
       </c>
@@ -9954,8 +10778,8 @@
       <c r="N7" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O7" s="45" t="s">
-        <v>171</v>
+      <c r="O7" s="46" t="s">
+        <v>224</v>
       </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
@@ -9974,23 +10798,23 @@
       <c r="AD7" s="11"/>
     </row>
     <row r="8">
-      <c r="A8" s="49" t="s">
-        <v>203</v>
-      </c>
-      <c r="B8" s="50" t="s">
-        <v>204</v>
-      </c>
-      <c r="C8" s="49" t="s">
-        <v>205</v>
+      <c r="A8" s="50" t="s">
+        <v>256</v>
+      </c>
+      <c r="B8" s="51" t="s">
+        <v>257</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>258</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="51"/>
+        <v>249</v>
+      </c>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
       <c r="J8" s="11"/>
       <c r="K8" s="17">
         <v>44699.0</v>
@@ -10002,44 +10826,44 @@
       <c r="N8" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O8" s="45" t="s">
-        <v>171</v>
-      </c>
-      <c r="P8" s="51"/>
-      <c r="Q8" s="51"/>
-      <c r="R8" s="51"/>
-      <c r="S8" s="51"/>
-      <c r="T8" s="51"/>
-      <c r="U8" s="51"/>
-      <c r="V8" s="51"/>
-      <c r="W8" s="51"/>
-      <c r="X8" s="51"/>
-      <c r="Y8" s="51"/>
-      <c r="Z8" s="51"/>
-      <c r="AA8" s="51"/>
-      <c r="AB8" s="51"/>
+      <c r="O8" s="46" t="s">
+        <v>224</v>
+      </c>
+      <c r="P8" s="52"/>
+      <c r="Q8" s="52"/>
+      <c r="R8" s="52"/>
+      <c r="S8" s="52"/>
+      <c r="T8" s="52"/>
+      <c r="U8" s="52"/>
+      <c r="V8" s="52"/>
+      <c r="W8" s="52"/>
+      <c r="X8" s="52"/>
+      <c r="Y8" s="52"/>
+      <c r="Z8" s="52"/>
+      <c r="AA8" s="52"/>
+      <c r="AB8" s="52"/>
       <c r="AC8" s="11"/>
       <c r="AD8" s="11"/>
     </row>
     <row r="9">
       <c r="A9" s="12" t="s">
-        <v>206</v>
+        <v>259</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>207</v>
+        <v>260</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>208</v>
+        <v>261</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="19" t="s">
-        <v>196</v>
+        <v>249</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="12" t="s">
-        <v>209</v>
+        <v>262</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="14">
@@ -10073,7 +10897,7 @@
       <c r="A10" s="12"/>
       <c r="B10" s="13"/>
       <c r="C10" s="12"/>
-      <c r="D10" s="44"/>
+      <c r="D10" s="45"/>
       <c r="E10" s="12"/>
       <c r="K10" s="17"/>
       <c r="L10" s="17"/>
@@ -10083,16 +10907,16 @@
     </row>
     <row r="11">
       <c r="A11" s="15" t="s">
-        <v>210</v>
+        <v>263</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>211</v>
+        <v>264</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="D11" s="44" t="s">
-        <v>192</v>
+        <v>265</v>
+      </c>
+      <c r="D11" s="45" t="s">
+        <v>245</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>26</v>
@@ -10112,8 +10936,8 @@
       <c r="N11" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O11" s="45" t="s">
-        <v>171</v>
+      <c r="O11" s="46" t="s">
+        <v>224</v>
       </c>
       <c r="P11" s="11"/>
       <c r="Q11" s="11"/>
@@ -10133,17 +10957,17 @@
     </row>
     <row r="12">
       <c r="A12" s="12" t="s">
-        <v>213</v>
+        <v>266</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>213</v>
+        <v>266</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>214</v>
+        <v>267</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="12" t="s">
-        <v>215</v>
+        <v>268</v>
       </c>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
@@ -10160,8 +10984,8 @@
       <c r="N12" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O12" s="45" t="s">
-        <v>171</v>
+      <c r="O12" s="46" t="s">
+        <v>224</v>
       </c>
       <c r="P12" s="11"/>
       <c r="Q12" s="11"/>
@@ -10181,23 +11005,23 @@
     </row>
     <row r="13">
       <c r="A13" s="12" t="s">
-        <v>216</v>
+        <v>269</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>216</v>
+        <v>269</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>217</v>
+        <v>270</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="12" t="s">
-        <v>215</v>
+        <v>268</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="12" t="s">
-        <v>218</v>
+        <v>271</v>
       </c>
       <c r="J13" s="11"/>
       <c r="K13" s="17">
@@ -10205,13 +11029,13 @@
       </c>
       <c r="L13" s="11"/>
       <c r="M13" s="12" t="s">
-        <v>219</v>
+        <v>272</v>
       </c>
       <c r="N13" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O13" s="45" t="s">
-        <v>171</v>
+      <c r="O13" s="46" t="s">
+        <v>224</v>
       </c>
       <c r="P13" s="11"/>
       <c r="Q13" s="11"/>
@@ -10231,17 +11055,17 @@
     </row>
     <row r="14">
       <c r="A14" s="12" t="s">
-        <v>220</v>
+        <v>273</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>221</v>
+        <v>274</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>222</v>
+        <v>275</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="12" t="s">
-        <v>215</v>
+        <v>268</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
@@ -10258,8 +11082,8 @@
       <c r="N14" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O14" s="45" t="s">
-        <v>171</v>
+      <c r="O14" s="46" t="s">
+        <v>224</v>
       </c>
       <c r="P14" s="11"/>
       <c r="Q14" s="11"/>
@@ -10279,23 +11103,23 @@
     </row>
     <row r="15">
       <c r="A15" s="12" t="s">
-        <v>223</v>
+        <v>276</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>224</v>
+        <v>277</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>225</v>
+        <v>278</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="12" t="s">
-        <v>215</v>
+        <v>268</v>
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
       <c r="I15" s="12" t="s">
-        <v>226</v>
+        <v>279</v>
       </c>
       <c r="J15" s="11"/>
       <c r="K15" s="17">
@@ -10310,8 +11134,8 @@
       <c r="N15" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O15" s="45" t="s">
-        <v>171</v>
+      <c r="O15" s="46" t="s">
+        <v>224</v>
       </c>
       <c r="P15" s="11"/>
       <c r="Q15" s="11"/>
@@ -10331,23 +11155,23 @@
     </row>
     <row r="16">
       <c r="A16" s="12" t="s">
-        <v>227</v>
+        <v>280</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>228</v>
+        <v>281</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>229</v>
+        <v>282</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="12" t="s">
-        <v>215</v>
+        <v>268</v>
       </c>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
       <c r="I16" s="12" t="s">
-        <v>230</v>
+        <v>283</v>
       </c>
       <c r="J16" s="11"/>
       <c r="K16" s="17">
@@ -10362,8 +11186,8 @@
       <c r="N16" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O16" s="45" t="s">
-        <v>171</v>
+      <c r="O16" s="46" t="s">
+        <v>224</v>
       </c>
       <c r="P16" s="11"/>
       <c r="Q16" s="11"/>
@@ -10383,17 +11207,17 @@
     </row>
     <row r="17">
       <c r="A17" s="12" t="s">
-        <v>231</v>
+        <v>284</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>232</v>
+        <v>285</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>233</v>
+        <v>286</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="12" t="s">
-        <v>215</v>
+        <v>268</v>
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
@@ -10429,17 +11253,17 @@
     </row>
     <row r="18">
       <c r="A18" s="12" t="s">
-        <v>234</v>
+        <v>287</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>235</v>
+        <v>288</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>236</v>
+        <v>289</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="12" t="s">
-        <v>215</v>
+        <v>268</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
@@ -10482,16 +11306,16 @@
     </row>
     <row r="20">
       <c r="A20" s="15" t="s">
-        <v>237</v>
+        <v>290</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>237</v>
+        <v>290</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>238</v>
+        <v>291</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>215</v>
+        <v>268</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>26</v>
@@ -10512,7 +11336,7 @@
         <v>50</v>
       </c>
       <c r="O20" s="16" t="s">
-        <v>239</v>
+        <v>292</v>
       </c>
       <c r="P20" s="11"/>
       <c r="Q20" s="11"/>
@@ -10532,17 +11356,17 @@
     </row>
     <row r="21">
       <c r="A21" s="12" t="s">
-        <v>240</v>
+        <v>293</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>240</v>
+        <v>293</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>241</v>
+        <v>294</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="12" t="s">
-        <v>242</v>
+        <v>295</v>
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
@@ -10560,7 +11384,7 @@
         <v>50</v>
       </c>
       <c r="O21" s="16" t="s">
-        <v>239</v>
+        <v>292</v>
       </c>
       <c r="P21" s="11"/>
       <c r="Q21" s="11"/>
@@ -10580,17 +11404,17 @@
     </row>
     <row r="22">
       <c r="A22" s="12" t="s">
-        <v>243</v>
+        <v>296</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>243</v>
+        <v>296</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>244</v>
+        <v>297</v>
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="12" t="s">
-        <v>242</v>
+        <v>295</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
@@ -10608,7 +11432,7 @@
         <v>50</v>
       </c>
       <c r="O22" s="16" t="s">
-        <v>239</v>
+        <v>292</v>
       </c>
       <c r="P22" s="11"/>
       <c r="Q22" s="11"/>
@@ -10628,17 +11452,17 @@
     </row>
     <row r="23">
       <c r="A23" s="13" t="s">
-        <v>245</v>
+        <v>298</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>246</v>
+        <v>299</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>247</v>
+        <v>300</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="12" t="s">
-        <v>242</v>
+        <v>295</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
@@ -10656,7 +11480,7 @@
         <v>50</v>
       </c>
       <c r="O23" s="16" t="s">
-        <v>239</v>
+        <v>292</v>
       </c>
       <c r="P23" s="11"/>
       <c r="Q23" s="11"/>
@@ -10679,16 +11503,16 @@
     </row>
     <row r="25">
       <c r="A25" s="15" t="s">
-        <v>248</v>
+        <v>301</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>249</v>
+        <v>302</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="D25" s="44" t="s">
-        <v>192</v>
+        <v>303</v>
+      </c>
+      <c r="D25" s="45" t="s">
+        <v>245</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>26</v>
@@ -10708,8 +11532,8 @@
       <c r="N25" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O25" s="45" t="s">
-        <v>171</v>
+      <c r="O25" s="46" t="s">
+        <v>224</v>
       </c>
       <c r="P25" s="11"/>
       <c r="Q25" s="11"/>
@@ -10729,17 +11553,17 @@
     </row>
     <row r="26">
       <c r="A26" s="12" t="s">
-        <v>251</v>
+        <v>304</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>252</v>
+        <v>305</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>253</v>
+        <v>306</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="12" t="s">
-        <v>254</v>
+        <v>307</v>
       </c>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
@@ -10756,8 +11580,8 @@
       <c r="N26" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O26" s="45" t="s">
-        <v>171</v>
+      <c r="O26" s="46" t="s">
+        <v>224</v>
       </c>
       <c r="P26" s="11"/>
       <c r="Q26" s="11"/>
@@ -10777,23 +11601,23 @@
     </row>
     <row r="27">
       <c r="A27" s="12" t="s">
-        <v>255</v>
+        <v>308</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>256</v>
+        <v>309</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>257</v>
+        <v>310</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="12" t="s">
-        <v>254</v>
+        <v>307</v>
       </c>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
       <c r="I27" s="12" t="s">
-        <v>258</v>
+        <v>311</v>
       </c>
       <c r="J27" s="11"/>
       <c r="K27" s="17">
@@ -10804,10 +11628,10 @@
         <v>20</v>
       </c>
       <c r="N27" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="O27" s="45" t="s">
-        <v>260</v>
+        <v>312</v>
+      </c>
+      <c r="O27" s="46" t="s">
+        <v>313</v>
       </c>
       <c r="P27" s="11"/>
       <c r="Q27" s="11"/>
@@ -10827,17 +11651,17 @@
     </row>
     <row r="28">
       <c r="A28" s="12" t="s">
-        <v>261</v>
+        <v>314</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>262</v>
+        <v>315</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>263</v>
+        <v>316</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="12" t="s">
-        <v>254</v>
+        <v>307</v>
       </c>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
@@ -10854,8 +11678,8 @@
       <c r="N28" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O28" s="45" t="s">
-        <v>171</v>
+      <c r="O28" s="46" t="s">
+        <v>224</v>
       </c>
       <c r="P28" s="11"/>
       <c r="Q28" s="11"/>
@@ -10875,17 +11699,17 @@
     </row>
     <row r="29">
       <c r="A29" s="12" t="s">
-        <v>264</v>
+        <v>317</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>265</v>
+        <v>318</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>266</v>
+        <v>319</v>
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="12" t="s">
-        <v>254</v>
+        <v>307</v>
       </c>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
@@ -10902,8 +11726,8 @@
       <c r="N29" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O29" s="45" t="s">
-        <v>171</v>
+      <c r="O29" s="46" t="s">
+        <v>224</v>
       </c>
       <c r="P29" s="11"/>
       <c r="Q29" s="11"/>
@@ -10923,17 +11747,17 @@
     </row>
     <row r="30">
       <c r="A30" s="12" t="s">
-        <v>267</v>
+        <v>320</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>268</v>
+        <v>321</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>269</v>
+        <v>322</v>
       </c>
       <c r="D30" s="11"/>
       <c r="E30" s="12" t="s">
-        <v>254</v>
+        <v>307</v>
       </c>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
@@ -10950,8 +11774,8 @@
       <c r="N30" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O30" s="45" t="s">
-        <v>171</v>
+      <c r="O30" s="46" t="s">
+        <v>224</v>
       </c>
       <c r="P30" s="11"/>
       <c r="Q30" s="11"/>
@@ -10971,17 +11795,17 @@
     </row>
     <row r="31">
       <c r="A31" s="12" t="s">
-        <v>270</v>
+        <v>323</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>271</v>
+        <v>324</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>272</v>
+        <v>325</v>
       </c>
       <c r="D31" s="11"/>
       <c r="E31" s="12" t="s">
-        <v>254</v>
+        <v>307</v>
       </c>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
@@ -10998,8 +11822,8 @@
       <c r="N31" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O31" s="45" t="s">
-        <v>171</v>
+      <c r="O31" s="46" t="s">
+        <v>224</v>
       </c>
       <c r="P31" s="11"/>
       <c r="Q31" s="11"/>
@@ -11022,16 +11846,16 @@
     </row>
     <row r="33">
       <c r="A33" s="15" t="s">
-        <v>273</v>
+        <v>326</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>274</v>
+        <v>327</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>275</v>
+        <v>328</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>192</v>
+        <v>245</v>
       </c>
       <c r="E33" s="12" t="s">
         <v>26</v>
@@ -11070,17 +11894,17 @@
     </row>
     <row r="34">
       <c r="A34" s="12" t="s">
-        <v>276</v>
+        <v>329</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>276</v>
+        <v>329</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>277</v>
+        <v>330</v>
       </c>
       <c r="D34" s="11"/>
       <c r="E34" s="12" t="s">
-        <v>278</v>
+        <v>331</v>
       </c>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
@@ -11116,17 +11940,17 @@
     </row>
     <row r="35">
       <c r="A35" s="12" t="s">
-        <v>279</v>
+        <v>332</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>279</v>
+        <v>332</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>280</v>
+        <v>333</v>
       </c>
       <c r="D35" s="11"/>
       <c r="E35" s="12" t="s">
-        <v>278</v>
+        <v>331</v>
       </c>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
@@ -11165,16 +11989,16 @@
     </row>
     <row r="37">
       <c r="A37" s="15" t="s">
-        <v>281</v>
+        <v>334</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>282</v>
+        <v>335</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>283</v>
+        <v>336</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>192</v>
+        <v>245</v>
       </c>
       <c r="E37" s="12" t="s">
         <v>26</v>
@@ -11213,17 +12037,17 @@
     </row>
     <row r="38">
       <c r="A38" s="12" t="s">
-        <v>284</v>
+        <v>337</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>285</v>
+        <v>338</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>286</v>
+        <v>339</v>
       </c>
       <c r="D38" s="11"/>
       <c r="E38" s="12" t="s">
-        <v>287</v>
+        <v>340</v>
       </c>
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
@@ -11259,17 +12083,17 @@
     </row>
     <row r="39">
       <c r="A39" s="12" t="s">
-        <v>288</v>
+        <v>341</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>289</v>
+        <v>342</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>290</v>
+        <v>343</v>
       </c>
       <c r="D39" s="11"/>
       <c r="E39" s="12" t="s">
-        <v>287</v>
+        <v>340</v>
       </c>
       <c r="F39" s="11"/>
       <c r="G39" s="11"/>
@@ -11305,17 +12129,17 @@
     </row>
     <row r="40">
       <c r="A40" s="12" t="s">
-        <v>291</v>
+        <v>344</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>292</v>
+        <v>345</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>293</v>
+        <v>346</v>
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="12" t="s">
-        <v>287</v>
+        <v>340</v>
       </c>
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
@@ -11351,17 +12175,17 @@
     </row>
     <row r="41">
       <c r="A41" s="12" t="s">
-        <v>294</v>
+        <v>347</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>295</v>
+        <v>348</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>296</v>
+        <v>349</v>
       </c>
       <c r="D41" s="11"/>
       <c r="E41" s="12" t="s">
-        <v>287</v>
+        <v>340</v>
       </c>
       <c r="F41" s="11"/>
       <c r="G41" s="11"/>
@@ -11397,17 +12221,17 @@
     </row>
     <row r="42">
       <c r="A42" s="12" t="s">
-        <v>297</v>
+        <v>350</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>298</v>
+        <v>351</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>299</v>
+        <v>352</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="12" t="s">
-        <v>287</v>
+        <v>340</v>
       </c>
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
@@ -11443,17 +12267,17 @@
     </row>
     <row r="43">
       <c r="A43" s="12" t="s">
-        <v>300</v>
+        <v>353</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>301</v>
+        <v>354</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>302</v>
+        <v>355</v>
       </c>
       <c r="D43" s="11"/>
       <c r="E43" s="12" t="s">
-        <v>287</v>
+        <v>340</v>
       </c>
       <c r="F43" s="11"/>
       <c r="G43" s="11"/>
@@ -11489,17 +12313,17 @@
     </row>
     <row r="44">
       <c r="A44" s="12" t="s">
-        <v>303</v>
+        <v>356</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>304</v>
+        <v>357</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>305</v>
+        <v>358</v>
       </c>
       <c r="D44" s="11"/>
       <c r="E44" s="12" t="s">
-        <v>287</v>
+        <v>340</v>
       </c>
       <c r="F44" s="11"/>
       <c r="G44" s="11"/>
@@ -11535,17 +12359,17 @@
     </row>
     <row r="45">
       <c r="A45" s="12" t="s">
-        <v>306</v>
+        <v>359</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>307</v>
+        <v>360</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>308</v>
+        <v>361</v>
       </c>
       <c r="D45" s="11"/>
       <c r="E45" s="12" t="s">
-        <v>287</v>
+        <v>340</v>
       </c>
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
@@ -11581,17 +12405,17 @@
     </row>
     <row r="46">
       <c r="A46" s="12" t="s">
-        <v>309</v>
+        <v>362</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>310</v>
+        <v>363</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>311</v>
+        <v>364</v>
       </c>
       <c r="D46" s="11"/>
       <c r="E46" s="12" t="s">
-        <v>287</v>
+        <v>340</v>
       </c>
       <c r="F46" s="11"/>
       <c r="G46" s="11"/>
@@ -11627,17 +12451,17 @@
     </row>
     <row r="47">
       <c r="A47" s="19" t="s">
-        <v>312</v>
+        <v>365</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>313</v>
+        <v>366</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>314</v>
+        <v>367</v>
       </c>
       <c r="D47" s="11"/>
       <c r="E47" s="12" t="s">
-        <v>287</v>
+        <v>340</v>
       </c>
       <c r="F47" s="11"/>
       <c r="G47" s="11"/>
@@ -14221,13 +15045,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>130</v>
+        <v>183</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>131</v>
+        <v>184</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>132</v>
+        <v>185</v>
       </c>
       <c r="G1" s="21" t="s">
         <v>6</v>
@@ -14242,7 +15066,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>133</v>
+        <v>186</v>
       </c>
       <c r="L1" s="26" t="s">
         <v>11</v>
@@ -14259,22 +15083,22 @@
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>315</v>
+        <v>368</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>316</v>
+        <v>369</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>317</v>
+        <v>370</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>192</v>
+        <v>245</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>137</v>
+        <v>190</v>
       </c>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
@@ -14291,7 +15115,7 @@
         <v>50</v>
       </c>
       <c r="O2" s="16" t="s">
-        <v>171</v>
+        <v>224</v>
       </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
@@ -14309,22 +15133,22 @@
     </row>
     <row r="3">
       <c r="A3" s="12" t="s">
-        <v>318</v>
+        <v>371</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>319</v>
+        <v>372</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>320</v>
+        <v>373</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>215</v>
+        <v>268</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>321</v>
+        <v>374</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -14341,7 +15165,7 @@
         <v>50</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>171</v>
+        <v>224</v>
       </c>
       <c r="P3" s="11"/>
       <c r="Q3" s="11"/>
@@ -14359,22 +15183,22 @@
     </row>
     <row r="4">
       <c r="A4" s="12" t="s">
-        <v>322</v>
+        <v>375</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>323</v>
+        <v>376</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>324</v>
+        <v>377</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>196</v>
+        <v>249</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>321</v>
+        <v>374</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
@@ -14391,7 +15215,7 @@
         <v>50</v>
       </c>
       <c r="O4" s="16" t="s">
-        <v>171</v>
+        <v>224</v>
       </c>
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
@@ -14409,22 +15233,22 @@
     </row>
     <row r="5">
       <c r="A5" s="12" t="s">
-        <v>325</v>
+        <v>378</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>326</v>
+        <v>379</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>327</v>
+        <v>380</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>254</v>
+        <v>307</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>321</v>
+        <v>374</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -14441,7 +15265,7 @@
         <v>50</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>328</v>
+        <v>381</v>
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
@@ -14459,22 +15283,22 @@
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>329</v>
+        <v>382</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>330</v>
+        <v>383</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>331</v>
+        <v>384</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>242</v>
+        <v>295</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>332</v>
+        <v>385</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>

</xml_diff>

<commit_message>
adds involvement, automation level; closes #108
- adds to processing context
- adds AutomationLevel
- adds EntityPermissiveInvolvement and EntityNonPermissiveInvolvement
- removes involvement concepts from Context/Status
</commit_message>
<xml_diff>
--- a/code/vocab_csv/context_status.xlsx
+++ b/code/vocab_csv/context_status.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="429">
   <si>
     <t>Term</t>
   </si>
@@ -607,6 +607,9 @@
   </si>
   <si>
     <t>dpv:hasEntity</t>
+  </si>
+  <si>
+    <t>removed</t>
   </si>
   <si>
     <t>The status or state of something</t>
@@ -6987,36 +6990,15 @@
       <c r="F16" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
       <c r="K16" s="14">
         <v>45422.0</v>
       </c>
-      <c r="L16" s="11"/>
       <c r="M16" s="12" t="s">
-        <v>20</v>
+        <v>193</v>
       </c>
       <c r="N16" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="11"/>
-      <c r="S16" s="11"/>
-      <c r="T16" s="11"/>
-      <c r="U16" s="11"/>
-      <c r="V16" s="11"/>
-      <c r="W16" s="11"/>
-      <c r="X16" s="11"/>
-      <c r="Y16" s="11"/>
-      <c r="Z16" s="11"/>
-      <c r="AA16" s="11"/>
-      <c r="AB16" s="11"/>
-      <c r="AC16" s="11"/>
-      <c r="AD16" s="11"/>
     </row>
     <row r="17">
       <c r="B17" s="19"/>
@@ -9981,7 +9963,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>25</v>
@@ -10037,16 +10019,16 @@
     </row>
     <row r="4">
       <c r="A4" s="15" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>26</v>
@@ -10087,17 +10069,17 @@
     </row>
     <row r="5">
       <c r="A5" s="12" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
@@ -10135,17 +10117,17 @@
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
@@ -10183,17 +10165,17 @@
     </row>
     <row r="7">
       <c r="A7" s="12" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
@@ -10231,17 +10213,17 @@
     </row>
     <row r="8">
       <c r="A8" s="50" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C8" s="50" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F8" s="52"/>
       <c r="G8" s="52"/>
@@ -10279,23 +10261,23 @@
     </row>
     <row r="9">
       <c r="A9" s="12" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="18" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="12" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="14">
@@ -10339,16 +10321,16 @@
     </row>
     <row r="11">
       <c r="A11" s="15" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D11" s="44" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>26</v>
@@ -10389,17 +10371,17 @@
     </row>
     <row r="12">
       <c r="A12" s="12" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="12" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
@@ -10437,23 +10419,23 @@
     </row>
     <row r="13">
       <c r="A13" s="12" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="12" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="12" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="J13" s="11"/>
       <c r="K13" s="17">
@@ -10461,7 +10443,7 @@
       </c>
       <c r="L13" s="11"/>
       <c r="M13" s="12" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="N13" s="12" t="s">
         <v>50</v>
@@ -10487,17 +10469,17 @@
     </row>
     <row r="14">
       <c r="A14" s="12" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="12" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
@@ -10535,23 +10517,23 @@
     </row>
     <row r="15">
       <c r="A15" s="12" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="12" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
       <c r="I15" s="12" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="J15" s="11"/>
       <c r="K15" s="17">
@@ -10587,23 +10569,23 @@
     </row>
     <row r="16">
       <c r="A16" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="12" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
       <c r="I16" s="12" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="J16" s="11"/>
       <c r="K16" s="17">
@@ -10639,17 +10621,17 @@
     </row>
     <row r="17">
       <c r="A17" s="12" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="12" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
@@ -10685,17 +10667,17 @@
     </row>
     <row r="18">
       <c r="A18" s="12" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="12" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
@@ -10738,16 +10720,16 @@
     </row>
     <row r="20">
       <c r="A20" s="15" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>26</v>
@@ -10768,7 +10750,7 @@
         <v>50</v>
       </c>
       <c r="O20" s="16" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="P20" s="11"/>
       <c r="Q20" s="11"/>
@@ -10788,17 +10770,17 @@
     </row>
     <row r="21">
       <c r="A21" s="12" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="12" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
@@ -10816,7 +10798,7 @@
         <v>50</v>
       </c>
       <c r="O21" s="16" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="P21" s="11"/>
       <c r="Q21" s="11"/>
@@ -10836,17 +10818,17 @@
     </row>
     <row r="22">
       <c r="A22" s="12" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="12" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
@@ -10864,7 +10846,7 @@
         <v>50</v>
       </c>
       <c r="O22" s="16" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="P22" s="11"/>
       <c r="Q22" s="11"/>
@@ -10884,17 +10866,17 @@
     </row>
     <row r="23">
       <c r="A23" s="13" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="12" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
@@ -10912,7 +10894,7 @@
         <v>50</v>
       </c>
       <c r="O23" s="16" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="P23" s="11"/>
       <c r="Q23" s="11"/>
@@ -10935,16 +10917,16 @@
     </row>
     <row r="25">
       <c r="A25" s="15" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D25" s="44" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>26</v>
@@ -10985,17 +10967,17 @@
     </row>
     <row r="26">
       <c r="A26" s="12" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="12" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
@@ -11033,23 +11015,23 @@
     </row>
     <row r="27">
       <c r="A27" s="12" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="12" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
       <c r="I27" s="12" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="J27" s="11"/>
       <c r="K27" s="17">
@@ -11060,10 +11042,10 @@
         <v>20</v>
       </c>
       <c r="N27" s="12" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="O27" s="45" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="P27" s="11"/>
       <c r="Q27" s="11"/>
@@ -11083,17 +11065,17 @@
     </row>
     <row r="28">
       <c r="A28" s="12" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="12" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
@@ -11131,17 +11113,17 @@
     </row>
     <row r="29">
       <c r="A29" s="12" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="12" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
@@ -11179,17 +11161,17 @@
     </row>
     <row r="30">
       <c r="A30" s="12" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D30" s="11"/>
       <c r="E30" s="12" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
@@ -11227,17 +11209,17 @@
     </row>
     <row r="31">
       <c r="A31" s="12" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D31" s="11"/>
       <c r="E31" s="12" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
@@ -11278,16 +11260,16 @@
     </row>
     <row r="33">
       <c r="A33" s="15" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E33" s="12" t="s">
         <v>26</v>
@@ -11326,17 +11308,17 @@
     </row>
     <row r="34">
       <c r="A34" s="12" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D34" s="11"/>
       <c r="E34" s="12" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
@@ -11372,17 +11354,17 @@
     </row>
     <row r="35">
       <c r="A35" s="12" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D35" s="11"/>
       <c r="E35" s="12" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
@@ -11421,16 +11403,16 @@
     </row>
     <row r="37">
       <c r="A37" s="15" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E37" s="12" t="s">
         <v>26</v>
@@ -11469,17 +11451,17 @@
     </row>
     <row r="38">
       <c r="A38" s="12" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D38" s="11"/>
       <c r="E38" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
@@ -11515,17 +11497,17 @@
     </row>
     <row r="39">
       <c r="A39" s="12" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D39" s="11"/>
       <c r="E39" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="F39" s="11"/>
       <c r="G39" s="11"/>
@@ -11561,17 +11543,17 @@
     </row>
     <row r="40">
       <c r="A40" s="12" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
@@ -11607,17 +11589,17 @@
     </row>
     <row r="41">
       <c r="A41" s="12" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D41" s="11"/>
       <c r="E41" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="F41" s="11"/>
       <c r="G41" s="11"/>
@@ -11653,17 +11635,17 @@
     </row>
     <row r="42">
       <c r="A42" s="12" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
@@ -11699,17 +11681,17 @@
     </row>
     <row r="43">
       <c r="A43" s="12" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D43" s="11"/>
       <c r="E43" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="F43" s="11"/>
       <c r="G43" s="11"/>
@@ -11745,17 +11727,17 @@
     </row>
     <row r="44">
       <c r="A44" s="12" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D44" s="11"/>
       <c r="E44" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="F44" s="11"/>
       <c r="G44" s="11"/>
@@ -11791,17 +11773,17 @@
     </row>
     <row r="45">
       <c r="A45" s="12" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D45" s="11"/>
       <c r="E45" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
@@ -11837,17 +11819,17 @@
     </row>
     <row r="46">
       <c r="A46" s="12" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D46" s="11"/>
       <c r="E46" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="F46" s="11"/>
       <c r="G46" s="11"/>
@@ -11883,17 +11865,17 @@
     </row>
     <row r="47">
       <c r="A47" s="18" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D47" s="11"/>
       <c r="E47" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="F47" s="11"/>
       <c r="G47" s="11"/>
@@ -11933,16 +11915,16 @@
     </row>
     <row r="49">
       <c r="A49" s="15" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E49" s="12" t="s">
         <v>26</v>
@@ -11960,7 +11942,7 @@
         <v>20</v>
       </c>
       <c r="N49" s="12" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="O49" s="11"/>
       <c r="P49" s="11"/>
@@ -11981,16 +11963,16 @@
     </row>
     <row r="50">
       <c r="A50" s="15" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E50" s="12" t="s">
         <v>18</v>
@@ -12008,7 +11990,7 @@
         <v>20</v>
       </c>
       <c r="N50" s="12" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="O50" s="11"/>
       <c r="P50" s="11"/>
@@ -12029,19 +12011,19 @@
     </row>
     <row r="51">
       <c r="A51" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="E51" s="12" t="s">
         <v>328</v>
-      </c>
-      <c r="B51" s="12" t="s">
-        <v>329</v>
-      </c>
-      <c r="C51" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="D51" s="12" t="s">
-        <v>331</v>
-      </c>
-      <c r="E51" s="12" t="s">
-        <v>327</v>
       </c>
       <c r="F51" s="11"/>
       <c r="G51" s="11"/>
@@ -12056,7 +12038,7 @@
         <v>20</v>
       </c>
       <c r="N51" s="12" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="O51" s="11"/>
       <c r="P51" s="11"/>
@@ -12077,19 +12059,19 @@
     </row>
     <row r="52">
       <c r="A52" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="D52" s="12" t="s">
         <v>332</v>
       </c>
-      <c r="B52" s="12" t="s">
-        <v>333</v>
-      </c>
-      <c r="C52" s="12" t="s">
-        <v>334</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>331</v>
-      </c>
       <c r="E52" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="F52" s="11"/>
       <c r="G52" s="11"/>
@@ -12104,7 +12086,7 @@
         <v>20</v>
       </c>
       <c r="N52" s="12" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="O52" s="11"/>
       <c r="P52" s="11"/>
@@ -12125,19 +12107,19 @@
     </row>
     <row r="53">
       <c r="A53" s="12" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="F53" s="11"/>
       <c r="G53" s="11"/>
@@ -12152,7 +12134,7 @@
         <v>20</v>
       </c>
       <c r="N53" s="12" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="O53" s="11"/>
       <c r="P53" s="11"/>
@@ -12173,19 +12155,19 @@
     </row>
     <row r="54">
       <c r="A54" s="12" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="F54" s="11"/>
       <c r="G54" s="11"/>
@@ -12200,7 +12182,7 @@
         <v>20</v>
       </c>
       <c r="N54" s="12" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="O54" s="11"/>
       <c r="P54" s="11"/>
@@ -12221,16 +12203,16 @@
     </row>
     <row r="55">
       <c r="A55" s="15" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E55" s="12" t="s">
         <v>26</v>
@@ -12248,7 +12230,7 @@
         <v>20</v>
       </c>
       <c r="N55" s="12" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="O55" s="11"/>
       <c r="P55" s="11"/>
@@ -12269,19 +12251,19 @@
     </row>
     <row r="56">
       <c r="A56" s="12" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="F56" s="11"/>
       <c r="G56" s="11"/>
@@ -12296,7 +12278,7 @@
         <v>20</v>
       </c>
       <c r="N56" s="12" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="O56" s="11"/>
       <c r="P56" s="11"/>
@@ -12317,19 +12299,19 @@
     </row>
     <row r="57">
       <c r="A57" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>350</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>351</v>
+      </c>
+      <c r="D57" s="12" t="s">
         <v>348</v>
       </c>
-      <c r="B57" s="12" t="s">
-        <v>349</v>
-      </c>
-      <c r="C57" s="12" t="s">
-        <v>350</v>
-      </c>
-      <c r="D57" s="12" t="s">
-        <v>347</v>
-      </c>
       <c r="E57" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="F57" s="11"/>
       <c r="G57" s="11"/>
@@ -12344,7 +12326,7 @@
         <v>20</v>
       </c>
       <c r="N57" s="12" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="O57" s="11"/>
       <c r="P57" s="11"/>
@@ -12365,19 +12347,19 @@
     </row>
     <row r="58">
       <c r="A58" s="12" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="F58" s="11"/>
       <c r="G58" s="11"/>
@@ -12392,7 +12374,7 @@
         <v>20</v>
       </c>
       <c r="N58" s="12" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="O58" s="11"/>
       <c r="P58" s="11"/>
@@ -12413,19 +12395,19 @@
     </row>
     <row r="59">
       <c r="A59" s="12" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="F59" s="11"/>
       <c r="G59" s="11"/>
@@ -12440,7 +12422,7 @@
         <v>20</v>
       </c>
       <c r="N59" s="12" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="O59" s="11"/>
       <c r="P59" s="11"/>
@@ -12465,16 +12447,16 @@
     </row>
     <row r="61">
       <c r="A61" s="15" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E61" s="12" t="s">
         <v>26</v>
@@ -12483,7 +12465,7 @@
       <c r="G61" s="11"/>
       <c r="H61" s="11"/>
       <c r="I61" s="12" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="J61" s="11"/>
       <c r="K61" s="17">
@@ -12494,7 +12476,7 @@
         <v>20</v>
       </c>
       <c r="N61" s="12" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="O61" s="11"/>
       <c r="P61" s="11"/>
@@ -12515,16 +12497,16 @@
     </row>
     <row r="62">
       <c r="A62" s="12" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="E62" s="12" t="s">
         <v>18</v>
@@ -12542,7 +12524,7 @@
         <v>20</v>
       </c>
       <c r="N62" s="12" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="O62" s="11"/>
       <c r="P62" s="11"/>
@@ -12563,16 +12545,16 @@
     </row>
     <row r="63">
       <c r="A63" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="B63" s="13" t="s">
+        <v>365</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>366</v>
+      </c>
+      <c r="D63" s="12" t="s">
         <v>364</v>
-      </c>
-      <c r="B63" s="13" t="s">
-        <v>364</v>
-      </c>
-      <c r="C63" s="12" t="s">
-        <v>365</v>
-      </c>
-      <c r="D63" s="12" t="s">
-        <v>363</v>
       </c>
       <c r="E63" s="12" t="s">
         <v>18</v>
@@ -12590,7 +12572,7 @@
         <v>20</v>
       </c>
       <c r="N63" s="12" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="O63" s="11"/>
       <c r="P63" s="11"/>
@@ -12615,23 +12597,23 @@
     </row>
     <row r="65">
       <c r="A65" s="15" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E65" s="11"/>
       <c r="F65" s="11"/>
       <c r="G65" s="11"/>
       <c r="H65" s="11"/>
       <c r="I65" s="12" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="J65" s="11"/>
       <c r="K65" s="17">
@@ -12642,7 +12624,7 @@
         <v>20</v>
       </c>
       <c r="N65" s="12" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="O65" s="11"/>
       <c r="P65" s="11"/>
@@ -12663,16 +12645,16 @@
     </row>
     <row r="66">
       <c r="A66" s="12" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="E66" s="12" t="s">
         <v>18</v>
@@ -12690,7 +12672,7 @@
         <v>20</v>
       </c>
       <c r="N66" s="12" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="O66" s="11"/>
       <c r="P66" s="11"/>
@@ -12711,16 +12693,16 @@
     </row>
     <row r="67">
       <c r="A67" s="12" t="s">
+        <v>373</v>
+      </c>
+      <c r="B67" s="13" t="s">
+        <v>373</v>
+      </c>
+      <c r="C67" s="12" t="s">
+        <v>374</v>
+      </c>
+      <c r="D67" s="12" t="s">
         <v>372</v>
-      </c>
-      <c r="B67" s="13" t="s">
-        <v>372</v>
-      </c>
-      <c r="C67" s="12" t="s">
-        <v>373</v>
-      </c>
-      <c r="D67" s="12" t="s">
-        <v>371</v>
       </c>
       <c r="E67" s="12" t="s">
         <v>18</v>
@@ -12738,7 +12720,7 @@
         <v>20</v>
       </c>
       <c r="N67" s="12" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="O67" s="11"/>
       <c r="P67" s="11"/>
@@ -12763,16 +12745,16 @@
     </row>
     <row r="69">
       <c r="A69" s="15" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D69" s="12" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E69" s="12" t="s">
         <v>26</v>
@@ -12790,7 +12772,7 @@
         <v>20</v>
       </c>
       <c r="N69" s="12" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="O69" s="11"/>
       <c r="P69" s="11"/>
@@ -12811,16 +12793,16 @@
     </row>
     <row r="70">
       <c r="A70" s="12" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E70" s="12" t="s">
         <v>18</v>
@@ -12829,7 +12811,7 @@
       <c r="G70" s="11"/>
       <c r="H70" s="11"/>
       <c r="I70" s="12" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="J70" s="11"/>
       <c r="K70" s="17">
@@ -12840,7 +12822,7 @@
         <v>20</v>
       </c>
       <c r="N70" s="12" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="O70" s="11"/>
       <c r="P70" s="11"/>
@@ -12861,16 +12843,16 @@
     </row>
     <row r="71">
       <c r="A71" s="12" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E71" s="12" t="s">
         <v>18</v>
@@ -12879,7 +12861,7 @@
       <c r="G71" s="11"/>
       <c r="H71" s="11"/>
       <c r="I71" s="12" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="J71" s="11"/>
       <c r="K71" s="17">
@@ -12890,7 +12872,7 @@
         <v>20</v>
       </c>
       <c r="N71" s="12" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="O71" s="11"/>
       <c r="P71" s="11"/>
@@ -12911,16 +12893,16 @@
     </row>
     <row r="72">
       <c r="A72" s="12" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D72" s="12" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E72" s="12" t="s">
         <v>18</v>
@@ -12938,7 +12920,7 @@
         <v>20</v>
       </c>
       <c r="N72" s="12" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="O72" s="11"/>
       <c r="P72" s="11"/>
@@ -15489,19 +15471,19 @@
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>137</v>
@@ -15541,22 +15523,22 @@
     </row>
     <row r="3">
       <c r="A3" s="12" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -15593,22 +15575,22 @@
     </row>
     <row r="4">
       <c r="A4" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
@@ -15645,22 +15627,22 @@
     </row>
     <row r="5">
       <c r="A5" s="12" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -15677,7 +15659,7 @@
         <v>50</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
@@ -15697,22 +15679,22 @@
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
@@ -15747,22 +15729,22 @@
     </row>
     <row r="7">
       <c r="A7" s="12" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -15797,22 +15779,22 @@
     </row>
     <row r="8">
       <c r="A8" s="12" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
@@ -15847,22 +15829,22 @@
     </row>
     <row r="9">
       <c r="A9" s="12" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
@@ -15897,22 +15879,22 @@
     </row>
     <row r="10">
       <c r="A10" s="12" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
@@ -15947,13 +15929,13 @@
     </row>
     <row r="11">
       <c r="A11" s="12" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>17</v>
@@ -15964,46 +15946,25 @@
       <c r="F11" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
       <c r="K11" s="14">
         <v>45422.0</v>
       </c>
-      <c r="L11" s="11"/>
       <c r="M11" s="12" t="s">
-        <v>20</v>
+        <v>193</v>
       </c>
       <c r="N11" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11"/>
-      <c r="U11" s="11"/>
-      <c r="V11" s="11"/>
-      <c r="W11" s="11"/>
-      <c r="X11" s="11"/>
-      <c r="Y11" s="11"/>
-      <c r="Z11" s="11"/>
-      <c r="AA11" s="11"/>
-      <c r="AB11" s="11"/>
-      <c r="AC11" s="11"/>
-      <c r="AD11" s="11"/>
     </row>
     <row r="12">
       <c r="A12" s="12" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>17</v>
@@ -16014,46 +15975,25 @@
       <c r="F12" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
       <c r="K12" s="14">
         <v>45422.0</v>
       </c>
-      <c r="L12" s="11"/>
       <c r="M12" s="12" t="s">
-        <v>20</v>
+        <v>193</v>
       </c>
       <c r="N12" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
-      <c r="S12" s="11"/>
-      <c r="T12" s="11"/>
-      <c r="U12" s="11"/>
-      <c r="V12" s="11"/>
-      <c r="W12" s="11"/>
-      <c r="X12" s="11"/>
-      <c r="Y12" s="11"/>
-      <c r="Z12" s="11"/>
-      <c r="AA12" s="11"/>
-      <c r="AB12" s="11"/>
-      <c r="AC12" s="11"/>
-      <c r="AD12" s="11"/>
     </row>
     <row r="13">
       <c r="A13" s="12" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>17</v>
@@ -16064,36 +16004,15 @@
       <c r="F13" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
       <c r="K13" s="14">
         <v>45422.0</v>
       </c>
-      <c r="L13" s="11"/>
       <c r="M13" s="12" t="s">
-        <v>20</v>
+        <v>193</v>
       </c>
       <c r="N13" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="11"/>
-      <c r="U13" s="11"/>
-      <c r="V13" s="11"/>
-      <c r="W13" s="11"/>
-      <c r="X13" s="11"/>
-      <c r="Y13" s="11"/>
-      <c r="Z13" s="11"/>
-      <c r="AA13" s="11"/>
-      <c r="AB13" s="11"/>
-      <c r="AC13" s="11"/>
-      <c r="AD13" s="11"/>
     </row>
     <row r="14">
       <c r="B14" s="19"/>

</xml_diff>

<commit_message>
adds risk, incident, data breach in eu-gdpr
- adds incident concepts to risk; closes #100
- adds data breach concepts to eu-gdpr; closes #64
- adds data breach guide for gdpr; see #103 (requires further edits)
- fixes profile metadata #141 bug where it was being documented as
  external concept in HTML; adds missing rdf:type for resources
- for Risk Extension: removes Assessment, Methodology, and Management
  concepts. The Management concepts have been moved to 'core' section.
- context-status in DPV: adds NotificationStatus concepts
</commit_message>
<xml_diff>
--- a/code/vocab_csv/context_status.xlsx
+++ b/code/vocab_csv/context_status.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="451">
   <si>
     <t>Term</t>
   </si>
@@ -633,12 +633,21 @@
     <t>Activity Proposed</t>
   </si>
   <si>
-    <t>State of an activity being proposed or planned i.e. yet to occur</t>
+    <t>State of an activity being proposed without any concrete plans for implementation</t>
   </si>
   <si>
     <t>dpv:ActivityStatus</t>
   </si>
   <si>
+    <t>ActivityPlanned</t>
+  </si>
+  <si>
+    <t>Activity Planned</t>
+  </si>
+  <si>
+    <t>State of an activity being planned with concrete plans for implementation</t>
+  </si>
+  <si>
     <t>ActivityOngoing</t>
   </si>
   <si>
@@ -1198,6 +1207,63 @@
   </si>
   <si>
     <t>Status indicating the specified context is 'not' involved</t>
+  </si>
+  <si>
+    <t>NotificationStatus</t>
+  </si>
+  <si>
+    <t>Notification Status</t>
+  </si>
+  <si>
+    <t>Status indicating whether notification(s) are planned, completed, or failed</t>
+  </si>
+  <si>
+    <t>NotificationPlanned</t>
+  </si>
+  <si>
+    <t>Notification Planned</t>
+  </si>
+  <si>
+    <t>Status indicating notification(s) are planned</t>
+  </si>
+  <si>
+    <t>dpv:NotificationStatus</t>
+  </si>
+  <si>
+    <t>NotificationOngoing</t>
+  </si>
+  <si>
+    <t>Notification Ongoing</t>
+  </si>
+  <si>
+    <t>Status indicating notification(s) are ongoing</t>
+  </si>
+  <si>
+    <t>NotificationCompleted</t>
+  </si>
+  <si>
+    <t>Notification Completed</t>
+  </si>
+  <si>
+    <t>Status indicating notification(s) are completed</t>
+  </si>
+  <si>
+    <t>NotificationNotNeeded</t>
+  </si>
+  <si>
+    <t>Notification Not Needed</t>
+  </si>
+  <si>
+    <t>Status indicating notification(s) are not needed</t>
+  </si>
+  <si>
+    <t>NotificationFailed</t>
+  </si>
+  <si>
+    <t>Notification Failed</t>
+  </si>
+  <si>
+    <t>Status indicating notification(s) could not be completed due to a failure</t>
   </si>
   <si>
     <t>hasStatus</t>
@@ -10089,7 +10155,9 @@
       <c r="K5" s="17">
         <v>44699.0</v>
       </c>
-      <c r="L5" s="17"/>
+      <c r="L5" s="17">
+        <v>45431.0</v>
+      </c>
       <c r="M5" s="12" t="s">
         <v>20</v>
       </c>
@@ -10135,7 +10203,7 @@
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
       <c r="K6" s="17">
-        <v>44699.0</v>
+        <v>45431.0</v>
       </c>
       <c r="L6" s="17"/>
       <c r="M6" s="12" t="s">
@@ -10144,9 +10212,7 @@
       <c r="N6" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O6" s="45" t="s">
-        <v>171</v>
-      </c>
+      <c r="O6" s="48"/>
       <c r="P6" s="11"/>
       <c r="Q6" s="11"/>
       <c r="R6" s="11"/>
@@ -10181,7 +10247,7 @@
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
-      <c r="J7" s="49"/>
+      <c r="J7" s="11"/>
       <c r="K7" s="17">
         <v>44699.0</v>
       </c>
@@ -10212,24 +10278,24 @@
       <c r="AD7" s="11"/>
     </row>
     <row r="8">
-      <c r="A8" s="50" t="s">
+      <c r="A8" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="13" t="s">
         <v>210</v>
       </c>
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="12" t="s">
         <v>211</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="52"/>
-      <c r="J8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="49"/>
       <c r="K8" s="17">
         <v>44699.0</v>
       </c>
@@ -10243,45 +10309,43 @@
       <c r="O8" s="45" t="s">
         <v>171</v>
       </c>
-      <c r="P8" s="52"/>
-      <c r="Q8" s="52"/>
-      <c r="R8" s="52"/>
-      <c r="S8" s="52"/>
-      <c r="T8" s="52"/>
-      <c r="U8" s="52"/>
-      <c r="V8" s="52"/>
-      <c r="W8" s="52"/>
-      <c r="X8" s="52"/>
-      <c r="Y8" s="52"/>
-      <c r="Z8" s="52"/>
-      <c r="AA8" s="52"/>
-      <c r="AB8" s="52"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="11"/>
       <c r="AC8" s="11"/>
       <c r="AD8" s="11"/>
     </row>
     <row r="9">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="50" t="s">
         <v>212</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="51" t="s">
         <v>213</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="50" t="s">
         <v>214</v>
       </c>
       <c r="D9" s="11"/>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="12" t="s">
-        <v>215</v>
-      </c>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
       <c r="J9" s="11"/>
-      <c r="K9" s="14">
-        <v>44895.0</v>
+      <c r="K9" s="17">
+        <v>44699.0</v>
       </c>
       <c r="L9" s="17"/>
       <c r="M9" s="12" t="s">
@@ -10290,98 +10354,100 @@
       <c r="N9" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O9" s="48"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="11"/>
-      <c r="W9" s="11"/>
-      <c r="X9" s="11"/>
-      <c r="Y9" s="11"/>
-      <c r="Z9" s="11"/>
-      <c r="AA9" s="11"/>
-      <c r="AB9" s="11"/>
+      <c r="O9" s="45" t="s">
+        <v>171</v>
+      </c>
+      <c r="P9" s="52"/>
+      <c r="Q9" s="52"/>
+      <c r="R9" s="52"/>
+      <c r="S9" s="52"/>
+      <c r="T9" s="52"/>
+      <c r="U9" s="52"/>
+      <c r="V9" s="52"/>
+      <c r="W9" s="52"/>
+      <c r="X9" s="52"/>
+      <c r="Y9" s="52"/>
+      <c r="Z9" s="52"/>
+      <c r="AA9" s="52"/>
+      <c r="AB9" s="52"/>
       <c r="AC9" s="11"/>
       <c r="AD9" s="11"/>
     </row>
     <row r="10">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="12"/>
-      <c r="K10" s="17"/>
+      <c r="A10" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="J10" s="11"/>
+      <c r="K10" s="14">
+        <v>44895.0</v>
+      </c>
       <c r="L10" s="17"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
+      <c r="M10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N10" s="12" t="s">
+        <v>50</v>
+      </c>
       <c r="O10" s="48"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="11"/>
+      <c r="AD10" s="11"/>
     </row>
     <row r="11">
-      <c r="A11" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="D11" s="44" t="s">
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="12"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="48"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D12" s="44" t="s">
         <v>198</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E12" s="12" t="s">
         <v>26</v>
-      </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="17">
-        <v>44699.0</v>
-      </c>
-      <c r="L11" s="17"/>
-      <c r="M11" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="N11" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="O11" s="45" t="s">
-        <v>171</v>
-      </c>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11"/>
-      <c r="U11" s="11"/>
-      <c r="V11" s="11"/>
-      <c r="W11" s="11"/>
-      <c r="X11" s="11"/>
-      <c r="Y11" s="11"/>
-      <c r="Z11" s="11"/>
-      <c r="AA11" s="11"/>
-      <c r="AB11" s="11"/>
-      <c r="AC11" s="11"/>
-      <c r="AD11" s="11"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12" t="s">
-        <v>221</v>
       </c>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
@@ -10391,7 +10457,7 @@
       <c r="K12" s="17">
         <v>44699.0</v>
       </c>
-      <c r="L12" s="11"/>
+      <c r="L12" s="17"/>
       <c r="M12" s="12" t="s">
         <v>20</v>
       </c>
@@ -10429,21 +10495,19 @@
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="12" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
-      <c r="I13" s="12" t="s">
-        <v>224</v>
-      </c>
+      <c r="I13" s="11"/>
       <c r="J13" s="11"/>
       <c r="K13" s="17">
         <v>44699.0</v>
       </c>
       <c r="L13" s="11"/>
       <c r="M13" s="12" t="s">
-        <v>225</v>
+        <v>20</v>
       </c>
       <c r="N13" s="12" t="s">
         <v>50</v>
@@ -10469,29 +10533,25 @@
     </row>
     <row r="14">
       <c r="A14" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="E14" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="I14" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>228</v>
-      </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
       <c r="K14" s="17">
         <v>44699.0</v>
       </c>
-      <c r="L14" s="11"/>
       <c r="M14" s="12" t="s">
-        <v>20</v>
+        <v>228</v>
       </c>
       <c r="N14" s="12" t="s">
         <v>50</v>
@@ -10499,21 +10559,6 @@
       <c r="O14" s="45" t="s">
         <v>171</v>
       </c>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="11"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="11"/>
-      <c r="U14" s="11"/>
-      <c r="V14" s="11"/>
-      <c r="W14" s="11"/>
-      <c r="X14" s="11"/>
-      <c r="Y14" s="11"/>
-      <c r="Z14" s="11"/>
-      <c r="AA14" s="11"/>
-      <c r="AB14" s="11"/>
-      <c r="AC14" s="11"/>
-      <c r="AD14" s="11"/>
     </row>
     <row r="15">
       <c r="A15" s="12" t="s">
@@ -10527,21 +10572,17 @@
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="12" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
-      <c r="I15" s="12" t="s">
-        <v>232</v>
-      </c>
+      <c r="I15" s="11"/>
       <c r="J15" s="11"/>
       <c r="K15" s="17">
         <v>44699.0</v>
       </c>
-      <c r="L15" s="17">
-        <v>44811.0</v>
-      </c>
+      <c r="L15" s="11"/>
       <c r="M15" s="12" t="s">
         <v>20</v>
       </c>
@@ -10569,23 +10610,23 @@
     </row>
     <row r="16">
       <c r="A16" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="C16" s="12" t="s">
         <v>234</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>235</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="12" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
       <c r="I16" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J16" s="11"/>
       <c r="K16" s="17">
@@ -10621,34 +10662,40 @@
     </row>
     <row r="17">
       <c r="A17" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="B17" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="C17" s="12" t="s">
         <v>238</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>239</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="12" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
+      <c r="I17" s="12" t="s">
+        <v>239</v>
+      </c>
       <c r="J17" s="11"/>
       <c r="K17" s="17">
+        <v>44699.0</v>
+      </c>
+      <c r="L17" s="17">
         <v>44811.0</v>
       </c>
-      <c r="L17" s="11"/>
       <c r="M17" s="12" t="s">
         <v>20</v>
       </c>
       <c r="N17" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O17" s="48"/>
+      <c r="O17" s="45" t="s">
+        <v>171</v>
+      </c>
       <c r="P17" s="11"/>
       <c r="Q17" s="11"/>
       <c r="R17" s="11"/>
@@ -10677,7 +10724,7 @@
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="12" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
@@ -10712,64 +10759,60 @@
       <c r="AD18" s="11"/>
     </row>
     <row r="19">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
+      <c r="A19" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="E19" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="17">
+        <v>44811.0</v>
+      </c>
+      <c r="L19" s="11"/>
+      <c r="M19" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N19" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="O19" s="48"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="11"/>
+      <c r="X19" s="11"/>
+      <c r="Y19" s="11"/>
+      <c r="Z19" s="11"/>
+      <c r="AA19" s="11"/>
+      <c r="AB19" s="11"/>
+      <c r="AC19" s="11"/>
+      <c r="AD19" s="11"/>
     </row>
     <row r="20">
-      <c r="A20" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>244</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="17">
-        <v>44853.0</v>
-      </c>
-      <c r="L20" s="11"/>
-      <c r="M20" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="N20" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="O20" s="16" t="s">
-        <v>245</v>
-      </c>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="11"/>
-      <c r="S20" s="11"/>
-      <c r="T20" s="11"/>
-      <c r="U20" s="11"/>
-      <c r="V20" s="11"/>
-      <c r="W20" s="11"/>
-      <c r="X20" s="11"/>
-      <c r="Y20" s="11"/>
-      <c r="Z20" s="11"/>
-      <c r="AA20" s="11"/>
-      <c r="AB20" s="11"/>
-      <c r="AC20" s="11"/>
-      <c r="AD20" s="11"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
     </row>
     <row r="21">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="15" t="s">
         <v>246</v>
       </c>
       <c r="B21" s="13" t="s">
@@ -10778,16 +10821,18 @@
       <c r="C21" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="D21" s="11"/>
+      <c r="D21" s="12" t="s">
+        <v>224</v>
+      </c>
       <c r="E21" s="12" t="s">
-        <v>248</v>
+        <v>26</v>
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
-      <c r="K21" s="14">
+      <c r="K21" s="17">
         <v>44853.0</v>
       </c>
       <c r="L21" s="11"/>
@@ -10798,7 +10843,7 @@
         <v>50</v>
       </c>
       <c r="O21" s="16" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="P21" s="11"/>
       <c r="Q21" s="11"/>
@@ -10828,7 +10873,7 @@
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="12" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
@@ -10846,7 +10891,7 @@
         <v>50</v>
       </c>
       <c r="O22" s="16" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="P22" s="11"/>
       <c r="Q22" s="11"/>
@@ -10865,10 +10910,10 @@
       <c r="AD22" s="11"/>
     </row>
     <row r="23">
-      <c r="A23" s="13" t="s">
-        <v>251</v>
-      </c>
-      <c r="B23" s="12" t="s">
+      <c r="A23" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="B23" s="13" t="s">
         <v>252</v>
       </c>
       <c r="C23" s="12" t="s">
@@ -10876,7 +10921,7 @@
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="12" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
@@ -10894,7 +10939,7 @@
         <v>50</v>
       </c>
       <c r="O23" s="16" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="P23" s="11"/>
       <c r="Q23" s="11"/>
@@ -10913,60 +10958,58 @@
       <c r="AD23" s="11"/>
     </row>
     <row r="24">
-      <c r="B24" s="19"/>
+      <c r="A24" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="D24" s="11"/>
+      <c r="E24" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="14">
+        <v>44853.0</v>
+      </c>
+      <c r="L24" s="11"/>
+      <c r="M24" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N24" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="O24" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="11"/>
+      <c r="V24" s="11"/>
+      <c r="W24" s="11"/>
+      <c r="X24" s="11"/>
+      <c r="Y24" s="11"/>
+      <c r="Z24" s="11"/>
+      <c r="AA24" s="11"/>
+      <c r="AB24" s="11"/>
+      <c r="AC24" s="11"/>
+      <c r="AD24" s="11"/>
     </row>
     <row r="25">
-      <c r="A25" s="15" t="s">
-        <v>254</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>255</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="D25" s="44" t="s">
-        <v>198</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="17">
-        <v>44699.0</v>
-      </c>
-      <c r="L25" s="11"/>
-      <c r="M25" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="N25" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="O25" s="45" t="s">
-        <v>171</v>
-      </c>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="11"/>
-      <c r="S25" s="11"/>
-      <c r="T25" s="11"/>
-      <c r="U25" s="11"/>
-      <c r="V25" s="11"/>
-      <c r="W25" s="11"/>
-      <c r="X25" s="11"/>
-      <c r="Y25" s="11"/>
-      <c r="Z25" s="11"/>
-      <c r="AA25" s="11"/>
-      <c r="AB25" s="11"/>
-      <c r="AC25" s="11"/>
-      <c r="AD25" s="11"/>
+      <c r="B25" s="19"/>
     </row>
     <row r="26">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="15" t="s">
         <v>257</v>
       </c>
       <c r="B26" s="13" t="s">
@@ -10975,9 +11018,11 @@
       <c r="C26" s="12" t="s">
         <v>259</v>
       </c>
-      <c r="D26" s="11"/>
+      <c r="D26" s="44" t="s">
+        <v>198</v>
+      </c>
       <c r="E26" s="12" t="s">
-        <v>260</v>
+        <v>26</v>
       </c>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
@@ -11015,37 +11060,35 @@
     </row>
     <row r="27">
       <c r="A27" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="B27" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="C27" s="12" t="s">
         <v>262</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>263</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="12" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
-      <c r="I27" s="12" t="s">
-        <v>264</v>
-      </c>
+      <c r="I27" s="11"/>
       <c r="J27" s="11"/>
       <c r="K27" s="17">
-        <v>44741.0</v>
+        <v>44699.0</v>
       </c>
       <c r="L27" s="11"/>
       <c r="M27" s="12" t="s">
         <v>20</v>
       </c>
       <c r="N27" s="12" t="s">
-        <v>265</v>
+        <v>50</v>
       </c>
       <c r="O27" s="45" t="s">
-        <v>266</v>
+        <v>171</v>
       </c>
       <c r="P27" s="11"/>
       <c r="Q27" s="11"/>
@@ -11065,35 +11108,37 @@
     </row>
     <row r="28">
       <c r="A28" s="12" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="12" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
+      <c r="I28" s="12" t="s">
+        <v>267</v>
+      </c>
       <c r="J28" s="11"/>
       <c r="K28" s="17">
-        <v>44699.0</v>
+        <v>44741.0</v>
       </c>
       <c r="L28" s="11"/>
       <c r="M28" s="12" t="s">
         <v>20</v>
       </c>
       <c r="N28" s="12" t="s">
-        <v>50</v>
+        <v>268</v>
       </c>
       <c r="O28" s="45" t="s">
-        <v>171</v>
+        <v>269</v>
       </c>
       <c r="P28" s="11"/>
       <c r="Q28" s="11"/>
@@ -11123,7 +11168,7 @@
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="12" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
@@ -11171,7 +11216,7 @@
       </c>
       <c r="D30" s="11"/>
       <c r="E30" s="12" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
@@ -11219,7 +11264,7 @@
       </c>
       <c r="D31" s="11"/>
       <c r="E31" s="12" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
@@ -11256,69 +11301,71 @@
       <c r="AD31" s="11"/>
     </row>
     <row r="32">
-      <c r="B32" s="19"/>
+      <c r="A32" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="D32" s="11"/>
+      <c r="E32" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="17">
+        <v>44699.0</v>
+      </c>
+      <c r="L32" s="11"/>
+      <c r="M32" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N32" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="O32" s="45" t="s">
+        <v>171</v>
+      </c>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="11"/>
+      <c r="T32" s="11"/>
+      <c r="U32" s="11"/>
+      <c r="V32" s="11"/>
+      <c r="W32" s="11"/>
+      <c r="X32" s="11"/>
+      <c r="Y32" s="11"/>
+      <c r="Z32" s="11"/>
+      <c r="AA32" s="11"/>
+      <c r="AB32" s="11"/>
+      <c r="AC32" s="11"/>
+      <c r="AD32" s="11"/>
     </row>
     <row r="33">
-      <c r="A33" s="15" t="s">
-        <v>279</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="D33" s="12" t="s">
+      <c r="B33" s="19"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="D34" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="E34" s="12" t="s">
         <v>26</v>
-      </c>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="17">
-        <v>44856.0</v>
-      </c>
-      <c r="L33" s="11"/>
-      <c r="M33" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="N33" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="O33" s="11"/>
-      <c r="P33" s="11"/>
-      <c r="Q33" s="11"/>
-      <c r="R33" s="11"/>
-      <c r="S33" s="11"/>
-      <c r="T33" s="11"/>
-      <c r="U33" s="11"/>
-      <c r="V33" s="11"/>
-      <c r="W33" s="11"/>
-      <c r="X33" s="11"/>
-      <c r="Y33" s="11"/>
-      <c r="Z33" s="11"/>
-      <c r="AA33" s="11"/>
-      <c r="AB33" s="11"/>
-      <c r="AC33" s="11"/>
-      <c r="AD33" s="11"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="12" t="s">
-        <v>282</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>282</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>283</v>
-      </c>
-      <c r="D34" s="11"/>
-      <c r="E34" s="12" t="s">
-        <v>284</v>
       </c>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
@@ -11364,7 +11411,7 @@
       </c>
       <c r="D35" s="11"/>
       <c r="E35" s="12" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
@@ -11399,58 +11446,56 @@
       <c r="AD35" s="11"/>
     </row>
     <row r="36">
-      <c r="B36" s="19"/>
+      <c r="A36" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="D36" s="11"/>
+      <c r="E36" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="17">
+        <v>44856.0</v>
+      </c>
+      <c r="L36" s="11"/>
+      <c r="M36" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N36" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="11"/>
+      <c r="T36" s="11"/>
+      <c r="U36" s="11"/>
+      <c r="V36" s="11"/>
+      <c r="W36" s="11"/>
+      <c r="X36" s="11"/>
+      <c r="Y36" s="11"/>
+      <c r="Z36" s="11"/>
+      <c r="AA36" s="11"/>
+      <c r="AB36" s="11"/>
+      <c r="AC36" s="11"/>
+      <c r="AD36" s="11"/>
     </row>
     <row r="37">
-      <c r="A37" s="15" t="s">
-        <v>287</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>289</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="14">
-        <v>44895.0</v>
-      </c>
-      <c r="L37" s="11"/>
-      <c r="M37" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="N37" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="O37" s="11"/>
-      <c r="P37" s="11"/>
-      <c r="Q37" s="11"/>
-      <c r="R37" s="11"/>
-      <c r="S37" s="11"/>
-      <c r="T37" s="11"/>
-      <c r="U37" s="11"/>
-      <c r="V37" s="11"/>
-      <c r="W37" s="11"/>
-      <c r="X37" s="11"/>
-      <c r="Y37" s="11"/>
-      <c r="Z37" s="11"/>
-      <c r="AA37" s="11"/>
-      <c r="AB37" s="11"/>
-      <c r="AC37" s="11"/>
-      <c r="AD37" s="11"/>
+      <c r="B37" s="19"/>
     </row>
     <row r="38">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="15" t="s">
         <v>290</v>
       </c>
       <c r="B38" s="13" t="s">
@@ -11459,9 +11504,11 @@
       <c r="C38" s="12" t="s">
         <v>292</v>
       </c>
-      <c r="D38" s="11"/>
+      <c r="D38" s="12" t="s">
+        <v>198</v>
+      </c>
       <c r="E38" s="12" t="s">
-        <v>293</v>
+        <v>26</v>
       </c>
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
@@ -11497,17 +11544,17 @@
     </row>
     <row r="39">
       <c r="A39" s="12" t="s">
+        <v>293</v>
+      </c>
+      <c r="B39" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="C39" s="12" t="s">
         <v>295</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>296</v>
       </c>
       <c r="D39" s="11"/>
       <c r="E39" s="12" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="F39" s="11"/>
       <c r="G39" s="11"/>
@@ -11553,7 +11600,7 @@
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="12" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
@@ -11599,7 +11646,7 @@
       </c>
       <c r="D41" s="11"/>
       <c r="E41" s="12" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="F41" s="11"/>
       <c r="G41" s="11"/>
@@ -11645,7 +11692,7 @@
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="12" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
@@ -11691,7 +11738,7 @@
       </c>
       <c r="D43" s="11"/>
       <c r="E43" s="12" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="F43" s="11"/>
       <c r="G43" s="11"/>
@@ -11737,7 +11784,7 @@
       </c>
       <c r="D44" s="11"/>
       <c r="E44" s="12" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="F44" s="11"/>
       <c r="G44" s="11"/>
@@ -11783,7 +11830,7 @@
       </c>
       <c r="D45" s="11"/>
       <c r="E45" s="12" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
@@ -11829,7 +11876,7 @@
       </c>
       <c r="D46" s="11"/>
       <c r="E46" s="12" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="F46" s="11"/>
       <c r="G46" s="11"/>
@@ -11864,7 +11911,7 @@
       <c r="AD46" s="11"/>
     </row>
     <row r="47">
-      <c r="A47" s="18" t="s">
+      <c r="A47" s="12" t="s">
         <v>318</v>
       </c>
       <c r="B47" s="13" t="s">
@@ -11875,7 +11922,7 @@
       </c>
       <c r="D47" s="11"/>
       <c r="E47" s="12" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="F47" s="11"/>
       <c r="G47" s="11"/>
@@ -11910,72 +11957,70 @@
       <c r="AD47" s="11"/>
     </row>
     <row r="48">
-      <c r="A48" s="12"/>
-      <c r="B48" s="19"/>
+      <c r="A48" s="18" t="s">
+        <v>321</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>322</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="D48" s="11"/>
+      <c r="E48" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="14">
+        <v>44895.0</v>
+      </c>
+      <c r="L48" s="11"/>
+      <c r="M48" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N48" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="O48" s="11"/>
+      <c r="P48" s="11"/>
+      <c r="Q48" s="11"/>
+      <c r="R48" s="11"/>
+      <c r="S48" s="11"/>
+      <c r="T48" s="11"/>
+      <c r="U48" s="11"/>
+      <c r="V48" s="11"/>
+      <c r="W48" s="11"/>
+      <c r="X48" s="11"/>
+      <c r="Y48" s="11"/>
+      <c r="Z48" s="11"/>
+      <c r="AA48" s="11"/>
+      <c r="AB48" s="11"/>
+      <c r="AC48" s="11"/>
+      <c r="AD48" s="11"/>
     </row>
     <row r="49">
-      <c r="A49" s="15" t="s">
-        <v>321</v>
-      </c>
-      <c r="B49" s="13" t="s">
-        <v>322</v>
-      </c>
-      <c r="C49" s="12" t="s">
-        <v>323</v>
-      </c>
-      <c r="D49" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="E49" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
-      <c r="J49" s="11"/>
-      <c r="K49" s="17">
-        <v>45422.0</v>
-      </c>
-      <c r="L49" s="11"/>
-      <c r="M49" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="N49" s="12" t="s">
-        <v>324</v>
-      </c>
-      <c r="O49" s="11"/>
-      <c r="P49" s="11"/>
-      <c r="Q49" s="11"/>
-      <c r="R49" s="11"/>
-      <c r="S49" s="11"/>
-      <c r="T49" s="11"/>
-      <c r="U49" s="11"/>
-      <c r="V49" s="11"/>
-      <c r="W49" s="11"/>
-      <c r="X49" s="11"/>
-      <c r="Y49" s="11"/>
-      <c r="Z49" s="11"/>
-      <c r="AA49" s="11"/>
-      <c r="AB49" s="11"/>
-      <c r="AC49" s="11"/>
-      <c r="AD49" s="11"/>
+      <c r="A49" s="12"/>
+      <c r="B49" s="19"/>
     </row>
     <row r="50">
       <c r="A50" s="15" t="s">
+        <v>324</v>
+      </c>
+      <c r="B50" s="13" t="s">
         <v>325</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="C50" s="12" t="s">
         <v>326</v>
       </c>
-      <c r="C50" s="12" t="s">
-        <v>327</v>
-      </c>
       <c r="D50" s="12" t="s">
-        <v>328</v>
+        <v>198</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F50" s="11"/>
       <c r="G50" s="11"/>
@@ -11990,7 +12035,7 @@
         <v>20</v>
       </c>
       <c r="N50" s="12" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="O50" s="11"/>
       <c r="P50" s="11"/>
@@ -12010,20 +12055,20 @@
       <c r="AD50" s="11"/>
     </row>
     <row r="51">
-      <c r="A51" s="12" t="s">
+      <c r="A51" s="15" t="s">
+        <v>328</v>
+      </c>
+      <c r="B51" s="13" t="s">
         <v>329</v>
       </c>
-      <c r="B51" s="12" t="s">
+      <c r="C51" s="12" t="s">
         <v>330</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="D51" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="D51" s="12" t="s">
-        <v>332</v>
-      </c>
       <c r="E51" s="12" t="s">
-        <v>328</v>
+        <v>18</v>
       </c>
       <c r="F51" s="11"/>
       <c r="G51" s="11"/>
@@ -12038,7 +12083,7 @@
         <v>20</v>
       </c>
       <c r="N51" s="12" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="O51" s="11"/>
       <c r="P51" s="11"/>
@@ -12059,19 +12104,19 @@
     </row>
     <row r="52">
       <c r="A52" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="B52" s="12" t="s">
         <v>333</v>
       </c>
-      <c r="B52" s="12" t="s">
+      <c r="C52" s="12" t="s">
         <v>334</v>
       </c>
-      <c r="C52" s="12" t="s">
+      <c r="D52" s="12" t="s">
         <v>335</v>
       </c>
-      <c r="D52" s="12" t="s">
-        <v>332</v>
-      </c>
       <c r="E52" s="12" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="F52" s="11"/>
       <c r="G52" s="11"/>
@@ -12086,7 +12131,7 @@
         <v>20</v>
       </c>
       <c r="N52" s="12" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="O52" s="11"/>
       <c r="P52" s="11"/>
@@ -12116,10 +12161,10 @@
         <v>338</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="F53" s="11"/>
       <c r="G53" s="11"/>
@@ -12134,7 +12179,7 @@
         <v>20</v>
       </c>
       <c r="N53" s="12" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="O53" s="11"/>
       <c r="P53" s="11"/>
@@ -12164,10 +12209,10 @@
         <v>341</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="F54" s="11"/>
       <c r="G54" s="11"/>
@@ -12182,7 +12227,7 @@
         <v>20</v>
       </c>
       <c r="N54" s="12" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="O54" s="11"/>
       <c r="P54" s="11"/>
@@ -12202,20 +12247,20 @@
       <c r="AD54" s="11"/>
     </row>
     <row r="55">
-      <c r="A55" s="15" t="s">
+      <c r="A55" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="B55" s="13" t="s">
+      <c r="B55" s="12" t="s">
         <v>343</v>
       </c>
       <c r="C55" s="12" t="s">
         <v>344</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>26</v>
+        <v>331</v>
       </c>
       <c r="F55" s="11"/>
       <c r="G55" s="11"/>
@@ -12230,7 +12275,7 @@
         <v>20</v>
       </c>
       <c r="N55" s="12" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="O55" s="11"/>
       <c r="P55" s="11"/>
@@ -12250,20 +12295,20 @@
       <c r="AD55" s="11"/>
     </row>
     <row r="56">
-      <c r="A56" s="12" t="s">
+      <c r="A56" s="15" t="s">
         <v>345</v>
       </c>
-      <c r="B56" s="12" t="s">
+      <c r="B56" s="13" t="s">
         <v>346</v>
       </c>
       <c r="C56" s="12" t="s">
         <v>347</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>348</v>
+        <v>331</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>328</v>
+        <v>26</v>
       </c>
       <c r="F56" s="11"/>
       <c r="G56" s="11"/>
@@ -12278,7 +12323,7 @@
         <v>20</v>
       </c>
       <c r="N56" s="12" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="O56" s="11"/>
       <c r="P56" s="11"/>
@@ -12299,19 +12344,19 @@
     </row>
     <row r="57">
       <c r="A57" s="12" t="s">
+        <v>348</v>
+      </c>
+      <c r="B57" s="12" t="s">
         <v>349</v>
       </c>
-      <c r="B57" s="12" t="s">
+      <c r="C57" s="12" t="s">
         <v>350</v>
       </c>
-      <c r="C57" s="12" t="s">
+      <c r="D57" s="12" t="s">
         <v>351</v>
       </c>
-      <c r="D57" s="12" t="s">
-        <v>348</v>
-      </c>
       <c r="E57" s="12" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="F57" s="11"/>
       <c r="G57" s="11"/>
@@ -12326,7 +12371,7 @@
         <v>20</v>
       </c>
       <c r="N57" s="12" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="O57" s="11"/>
       <c r="P57" s="11"/>
@@ -12356,10 +12401,10 @@
         <v>354</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="F58" s="11"/>
       <c r="G58" s="11"/>
@@ -12374,7 +12419,7 @@
         <v>20</v>
       </c>
       <c r="N58" s="12" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="O58" s="11"/>
       <c r="P58" s="11"/>
@@ -12404,10 +12449,10 @@
         <v>357</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="F59" s="11"/>
       <c r="G59" s="11"/>
@@ -12422,7 +12467,7 @@
         <v>20</v>
       </c>
       <c r="N59" s="12" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="O59" s="11"/>
       <c r="P59" s="11"/>
@@ -12442,62 +12487,60 @@
       <c r="AD59" s="11"/>
     </row>
     <row r="60">
-      <c r="B60" s="19"/>
-      <c r="K60" s="17"/>
+      <c r="A60" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>359</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>360</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>351</v>
+      </c>
+      <c r="E60" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11"/>
+      <c r="I60" s="11"/>
+      <c r="J60" s="11"/>
+      <c r="K60" s="17">
+        <v>45422.0</v>
+      </c>
+      <c r="L60" s="11"/>
+      <c r="M60" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N60" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="O60" s="11"/>
+      <c r="P60" s="11"/>
+      <c r="Q60" s="11"/>
+      <c r="R60" s="11"/>
+      <c r="S60" s="11"/>
+      <c r="T60" s="11"/>
+      <c r="U60" s="11"/>
+      <c r="V60" s="11"/>
+      <c r="W60" s="11"/>
+      <c r="X60" s="11"/>
+      <c r="Y60" s="11"/>
+      <c r="Z60" s="11"/>
+      <c r="AA60" s="11"/>
+      <c r="AB60" s="11"/>
+      <c r="AC60" s="11"/>
+      <c r="AD60" s="11"/>
     </row>
     <row r="61">
-      <c r="A61" s="15" t="s">
-        <v>358</v>
-      </c>
-      <c r="B61" s="13" t="s">
-        <v>359</v>
-      </c>
-      <c r="C61" s="12" t="s">
-        <v>360</v>
-      </c>
-      <c r="D61" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="E61" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F61" s="11"/>
-      <c r="G61" s="11"/>
-      <c r="H61" s="11"/>
-      <c r="I61" s="12" t="s">
+      <c r="B61" s="19"/>
+      <c r="K61" s="17"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="15" t="s">
         <v>361</v>
-      </c>
-      <c r="J61" s="11"/>
-      <c r="K61" s="17">
-        <v>45422.0</v>
-      </c>
-      <c r="L61" s="11"/>
-      <c r="M61" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="N61" s="12" t="s">
-        <v>324</v>
-      </c>
-      <c r="O61" s="11"/>
-      <c r="P61" s="11"/>
-      <c r="Q61" s="11"/>
-      <c r="R61" s="11"/>
-      <c r="S61" s="11"/>
-      <c r="T61" s="11"/>
-      <c r="U61" s="11"/>
-      <c r="V61" s="11"/>
-      <c r="W61" s="11"/>
-      <c r="X61" s="11"/>
-      <c r="Y61" s="11"/>
-      <c r="Z61" s="11"/>
-      <c r="AA61" s="11"/>
-      <c r="AB61" s="11"/>
-      <c r="AC61" s="11"/>
-      <c r="AD61" s="11"/>
-    </row>
-    <row r="62">
-      <c r="A62" s="12" t="s">
-        <v>362</v>
       </c>
       <c r="B62" s="13" t="s">
         <v>362</v>
@@ -12506,15 +12549,17 @@
         <v>363</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>364</v>
+        <v>198</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F62" s="11"/>
       <c r="G62" s="11"/>
       <c r="H62" s="11"/>
-      <c r="I62" s="11"/>
+      <c r="I62" s="12" t="s">
+        <v>364</v>
+      </c>
       <c r="J62" s="11"/>
       <c r="K62" s="17">
         <v>45422.0</v>
@@ -12524,7 +12569,7 @@
         <v>20</v>
       </c>
       <c r="N62" s="12" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="O62" s="11"/>
       <c r="P62" s="11"/>
@@ -12554,7 +12599,7 @@
         <v>366</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="E63" s="12" t="s">
         <v>18</v>
@@ -12572,7 +12617,7 @@
         <v>20</v>
       </c>
       <c r="N63" s="12" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="O63" s="11"/>
       <c r="P63" s="11"/>
@@ -12592,77 +12637,77 @@
       <c r="AD63" s="11"/>
     </row>
     <row r="64">
-      <c r="B64" s="19"/>
-      <c r="K64" s="17"/>
+      <c r="A64" s="12" t="s">
+        <v>368</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>369</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>367</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="11"/>
+      <c r="J64" s="11"/>
+      <c r="K64" s="17">
+        <v>45422.0</v>
+      </c>
+      <c r="L64" s="11"/>
+      <c r="M64" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N64" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="O64" s="11"/>
+      <c r="P64" s="11"/>
+      <c r="Q64" s="11"/>
+      <c r="R64" s="11"/>
+      <c r="S64" s="11"/>
+      <c r="T64" s="11"/>
+      <c r="U64" s="11"/>
+      <c r="V64" s="11"/>
+      <c r="W64" s="11"/>
+      <c r="X64" s="11"/>
+      <c r="Y64" s="11"/>
+      <c r="Z64" s="11"/>
+      <c r="AA64" s="11"/>
+      <c r="AB64" s="11"/>
+      <c r="AC64" s="11"/>
+      <c r="AD64" s="11"/>
     </row>
     <row r="65">
-      <c r="A65" s="15" t="s">
-        <v>367</v>
-      </c>
-      <c r="B65" s="13" t="s">
-        <v>368</v>
-      </c>
-      <c r="C65" s="12" t="s">
-        <v>360</v>
-      </c>
-      <c r="D65" s="12" t="s">
+      <c r="B65" s="19"/>
+      <c r="K65" s="17"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="15" t="s">
+        <v>370</v>
+      </c>
+      <c r="B66" s="13" t="s">
+        <v>371</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="D66" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="E65" s="11"/>
-      <c r="F65" s="11"/>
-      <c r="G65" s="11"/>
-      <c r="H65" s="11"/>
-      <c r="I65" s="12" t="s">
-        <v>369</v>
-      </c>
-      <c r="J65" s="11"/>
-      <c r="K65" s="17">
-        <v>45422.0</v>
-      </c>
-      <c r="L65" s="11"/>
-      <c r="M65" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="N65" s="12" t="s">
-        <v>324</v>
-      </c>
-      <c r="O65" s="11"/>
-      <c r="P65" s="11"/>
-      <c r="Q65" s="11"/>
-      <c r="R65" s="11"/>
-      <c r="S65" s="11"/>
-      <c r="T65" s="11"/>
-      <c r="U65" s="11"/>
-      <c r="V65" s="11"/>
-      <c r="W65" s="11"/>
-      <c r="X65" s="11"/>
-      <c r="Y65" s="11"/>
-      <c r="Z65" s="11"/>
-      <c r="AA65" s="11"/>
-      <c r="AB65" s="11"/>
-      <c r="AC65" s="11"/>
-      <c r="AD65" s="11"/>
-    </row>
-    <row r="66">
-      <c r="A66" s="12" t="s">
-        <v>370</v>
-      </c>
-      <c r="B66" s="13" t="s">
-        <v>370</v>
-      </c>
-      <c r="C66" s="12" t="s">
-        <v>371</v>
-      </c>
-      <c r="D66" s="12" t="s">
-        <v>372</v>
-      </c>
-      <c r="E66" s="12" t="s">
-        <v>18</v>
-      </c>
+      <c r="E66" s="11"/>
       <c r="F66" s="11"/>
       <c r="G66" s="11"/>
       <c r="H66" s="11"/>
-      <c r="I66" s="11"/>
+      <c r="I66" s="12" t="s">
+        <v>372</v>
+      </c>
       <c r="J66" s="11"/>
       <c r="K66" s="17">
         <v>45422.0</v>
@@ -12672,7 +12717,7 @@
         <v>20</v>
       </c>
       <c r="N66" s="12" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="O66" s="11"/>
       <c r="P66" s="11"/>
@@ -12702,7 +12747,7 @@
         <v>374</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="E67" s="12" t="s">
         <v>18</v>
@@ -12720,7 +12765,7 @@
         <v>20</v>
       </c>
       <c r="N67" s="12" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="O67" s="11"/>
       <c r="P67" s="11"/>
@@ -12740,79 +12785,77 @@
       <c r="AD67" s="11"/>
     </row>
     <row r="68">
-      <c r="B68" s="19"/>
-      <c r="K68" s="17"/>
+      <c r="A68" s="12" t="s">
+        <v>376</v>
+      </c>
+      <c r="B68" s="13" t="s">
+        <v>376</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>375</v>
+      </c>
+      <c r="E68" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F68" s="11"/>
+      <c r="G68" s="11"/>
+      <c r="H68" s="11"/>
+      <c r="I68" s="11"/>
+      <c r="J68" s="11"/>
+      <c r="K68" s="17">
+        <v>45422.0</v>
+      </c>
+      <c r="L68" s="11"/>
+      <c r="M68" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N68" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="O68" s="11"/>
+      <c r="P68" s="11"/>
+      <c r="Q68" s="11"/>
+      <c r="R68" s="11"/>
+      <c r="S68" s="11"/>
+      <c r="T68" s="11"/>
+      <c r="U68" s="11"/>
+      <c r="V68" s="11"/>
+      <c r="W68" s="11"/>
+      <c r="X68" s="11"/>
+      <c r="Y68" s="11"/>
+      <c r="Z68" s="11"/>
+      <c r="AA68" s="11"/>
+      <c r="AB68" s="11"/>
+      <c r="AC68" s="11"/>
+      <c r="AD68" s="11"/>
     </row>
     <row r="69">
-      <c r="A69" s="15" t="s">
-        <v>375</v>
-      </c>
-      <c r="B69" s="12" t="s">
-        <v>376</v>
-      </c>
-      <c r="C69" s="12" t="s">
-        <v>377</v>
-      </c>
-      <c r="D69" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="E69" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F69" s="11"/>
-      <c r="G69" s="11"/>
-      <c r="H69" s="11"/>
-      <c r="I69" s="11"/>
-      <c r="J69" s="11"/>
-      <c r="K69" s="17">
-        <v>45422.0</v>
-      </c>
-      <c r="L69" s="11"/>
-      <c r="M69" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="N69" s="12" t="s">
-        <v>324</v>
-      </c>
-      <c r="O69" s="11"/>
-      <c r="P69" s="11"/>
-      <c r="Q69" s="11"/>
-      <c r="R69" s="11"/>
-      <c r="S69" s="11"/>
-      <c r="T69" s="11"/>
-      <c r="U69" s="11"/>
-      <c r="V69" s="11"/>
-      <c r="W69" s="11"/>
-      <c r="X69" s="11"/>
-      <c r="Y69" s="11"/>
-      <c r="Z69" s="11"/>
-      <c r="AA69" s="11"/>
-      <c r="AB69" s="11"/>
-      <c r="AC69" s="11"/>
-      <c r="AD69" s="11"/>
+      <c r="B69" s="19"/>
+      <c r="K69" s="17"/>
     </row>
     <row r="70">
-      <c r="A70" s="12" t="s">
+      <c r="A70" s="15" t="s">
         <v>378</v>
       </c>
-      <c r="B70" s="13" t="s">
+      <c r="B70" s="12" t="s">
         <v>379</v>
       </c>
       <c r="C70" s="12" t="s">
         <v>380</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>381</v>
+        <v>198</v>
       </c>
       <c r="E70" s="12" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F70" s="11"/>
       <c r="G70" s="11"/>
       <c r="H70" s="11"/>
-      <c r="I70" s="12" t="s">
-        <v>382</v>
-      </c>
+      <c r="I70" s="11"/>
       <c r="J70" s="11"/>
       <c r="K70" s="17">
         <v>45422.0</v>
@@ -12822,7 +12865,7 @@
         <v>20</v>
       </c>
       <c r="N70" s="12" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="O70" s="11"/>
       <c r="P70" s="11"/>
@@ -12843,16 +12886,16 @@
     </row>
     <row r="71">
       <c r="A71" s="12" t="s">
+        <v>381</v>
+      </c>
+      <c r="B71" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="C71" s="12" t="s">
         <v>383</v>
       </c>
-      <c r="B71" s="13" t="s">
+      <c r="D71" s="12" t="s">
         <v>384</v>
-      </c>
-      <c r="C71" s="12" t="s">
-        <v>385</v>
-      </c>
-      <c r="D71" s="12" t="s">
-        <v>381</v>
       </c>
       <c r="E71" s="12" t="s">
         <v>18</v>
@@ -12861,7 +12904,7 @@
       <c r="G71" s="11"/>
       <c r="H71" s="11"/>
       <c r="I71" s="12" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="J71" s="11"/>
       <c r="K71" s="17">
@@ -12872,7 +12915,7 @@
         <v>20</v>
       </c>
       <c r="N71" s="12" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="O71" s="11"/>
       <c r="P71" s="11"/>
@@ -12893,16 +12936,16 @@
     </row>
     <row r="72">
       <c r="A72" s="12" t="s">
+        <v>386</v>
+      </c>
+      <c r="B72" s="13" t="s">
         <v>387</v>
       </c>
-      <c r="B72" s="13" t="s">
+      <c r="C72" s="12" t="s">
         <v>388</v>
       </c>
-      <c r="C72" s="12" t="s">
-        <v>389</v>
-      </c>
       <c r="D72" s="12" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="E72" s="12" t="s">
         <v>18</v>
@@ -12910,7 +12953,9 @@
       <c r="F72" s="11"/>
       <c r="G72" s="11"/>
       <c r="H72" s="11"/>
-      <c r="I72" s="11"/>
+      <c r="I72" s="12" t="s">
+        <v>389</v>
+      </c>
       <c r="J72" s="11"/>
       <c r="K72" s="17">
         <v>45422.0</v>
@@ -12920,7 +12965,7 @@
         <v>20</v>
       </c>
       <c r="N72" s="12" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="O72" s="11"/>
       <c r="P72" s="11"/>
@@ -12940,28 +12985,333 @@
       <c r="AD72" s="11"/>
     </row>
     <row r="73">
-      <c r="B73" s="19"/>
+      <c r="A73" s="12" t="s">
+        <v>390</v>
+      </c>
+      <c r="B73" s="13" t="s">
+        <v>391</v>
+      </c>
+      <c r="C73" s="12" t="s">
+        <v>392</v>
+      </c>
+      <c r="D73" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="E73" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F73" s="11"/>
+      <c r="G73" s="11"/>
+      <c r="H73" s="11"/>
+      <c r="I73" s="11"/>
+      <c r="J73" s="11"/>
+      <c r="K73" s="17">
+        <v>45422.0</v>
+      </c>
+      <c r="L73" s="11"/>
+      <c r="M73" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N73" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="O73" s="11"/>
+      <c r="P73" s="11"/>
+      <c r="Q73" s="11"/>
+      <c r="R73" s="11"/>
+      <c r="S73" s="11"/>
+      <c r="T73" s="11"/>
+      <c r="U73" s="11"/>
+      <c r="V73" s="11"/>
+      <c r="W73" s="11"/>
+      <c r="X73" s="11"/>
+      <c r="Y73" s="11"/>
+      <c r="Z73" s="11"/>
+      <c r="AA73" s="11"/>
+      <c r="AB73" s="11"/>
+      <c r="AC73" s="11"/>
+      <c r="AD73" s="11"/>
     </row>
     <row r="74">
       <c r="B74" s="19"/>
     </row>
     <row r="75">
-      <c r="B75" s="19"/>
+      <c r="A75" s="15" t="s">
+        <v>393</v>
+      </c>
+      <c r="B75" s="13" t="s">
+        <v>394</v>
+      </c>
+      <c r="C75" s="12" t="s">
+        <v>395</v>
+      </c>
+      <c r="D75" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="E75" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F75" s="11"/>
+      <c r="G75" s="11"/>
+      <c r="H75" s="11"/>
+      <c r="I75" s="11"/>
+      <c r="J75" s="11"/>
+      <c r="K75" s="17">
+        <v>45431.0</v>
+      </c>
+      <c r="L75" s="11"/>
+      <c r="M75" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N75" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="O75" s="11"/>
+      <c r="P75" s="11"/>
+      <c r="Q75" s="11"/>
+      <c r="R75" s="11"/>
+      <c r="S75" s="11"/>
+      <c r="T75" s="11"/>
+      <c r="U75" s="11"/>
+      <c r="V75" s="11"/>
+      <c r="W75" s="11"/>
+      <c r="X75" s="11"/>
+      <c r="Y75" s="11"/>
+      <c r="Z75" s="11"/>
+      <c r="AA75" s="11"/>
+      <c r="AB75" s="11"/>
+      <c r="AC75" s="11"/>
+      <c r="AD75" s="11"/>
     </row>
     <row r="76">
-      <c r="B76" s="19"/>
+      <c r="A76" s="12" t="s">
+        <v>396</v>
+      </c>
+      <c r="B76" s="12" t="s">
+        <v>397</v>
+      </c>
+      <c r="C76" s="12" t="s">
+        <v>398</v>
+      </c>
+      <c r="D76" s="11"/>
+      <c r="E76" s="12" t="s">
+        <v>399</v>
+      </c>
+      <c r="F76" s="11"/>
+      <c r="G76" s="11"/>
+      <c r="H76" s="11"/>
+      <c r="I76" s="11"/>
+      <c r="J76" s="11"/>
+      <c r="K76" s="17">
+        <v>45431.0</v>
+      </c>
+      <c r="L76" s="11"/>
+      <c r="M76" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N76" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="O76" s="11"/>
+      <c r="P76" s="11"/>
+      <c r="Q76" s="11"/>
+      <c r="R76" s="11"/>
+      <c r="S76" s="11"/>
+      <c r="T76" s="11"/>
+      <c r="U76" s="11"/>
+      <c r="V76" s="11"/>
+      <c r="W76" s="11"/>
+      <c r="X76" s="11"/>
+      <c r="Y76" s="11"/>
+      <c r="Z76" s="11"/>
+      <c r="AA76" s="11"/>
+      <c r="AB76" s="11"/>
+      <c r="AC76" s="11"/>
+      <c r="AD76" s="11"/>
     </row>
     <row r="77">
-      <c r="B77" s="19"/>
+      <c r="A77" s="12" t="s">
+        <v>400</v>
+      </c>
+      <c r="B77" s="12" t="s">
+        <v>401</v>
+      </c>
+      <c r="C77" s="12" t="s">
+        <v>402</v>
+      </c>
+      <c r="D77" s="11"/>
+      <c r="E77" s="12" t="s">
+        <v>399</v>
+      </c>
+      <c r="F77" s="11"/>
+      <c r="G77" s="11"/>
+      <c r="H77" s="11"/>
+      <c r="I77" s="11"/>
+      <c r="J77" s="11"/>
+      <c r="K77" s="17">
+        <v>45431.0</v>
+      </c>
+      <c r="L77" s="11"/>
+      <c r="M77" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N77" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="O77" s="11"/>
+      <c r="P77" s="11"/>
+      <c r="Q77" s="11"/>
+      <c r="R77" s="11"/>
+      <c r="S77" s="11"/>
+      <c r="T77" s="11"/>
+      <c r="U77" s="11"/>
+      <c r="V77" s="11"/>
+      <c r="W77" s="11"/>
+      <c r="X77" s="11"/>
+      <c r="Y77" s="11"/>
+      <c r="Z77" s="11"/>
+      <c r="AA77" s="11"/>
+      <c r="AB77" s="11"/>
+      <c r="AC77" s="11"/>
+      <c r="AD77" s="11"/>
     </row>
     <row r="78">
-      <c r="B78" s="19"/>
+      <c r="A78" s="12" t="s">
+        <v>403</v>
+      </c>
+      <c r="B78" s="12" t="s">
+        <v>404</v>
+      </c>
+      <c r="C78" s="12" t="s">
+        <v>405</v>
+      </c>
+      <c r="D78" s="11"/>
+      <c r="E78" s="12" t="s">
+        <v>399</v>
+      </c>
+      <c r="F78" s="11"/>
+      <c r="G78" s="11"/>
+      <c r="H78" s="11"/>
+      <c r="I78" s="11"/>
+      <c r="J78" s="11"/>
+      <c r="K78" s="17">
+        <v>45431.0</v>
+      </c>
+      <c r="L78" s="11"/>
+      <c r="M78" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N78" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="O78" s="11"/>
+      <c r="P78" s="11"/>
+      <c r="Q78" s="11"/>
+      <c r="R78" s="11"/>
+      <c r="S78" s="11"/>
+      <c r="T78" s="11"/>
+      <c r="U78" s="11"/>
+      <c r="V78" s="11"/>
+      <c r="W78" s="11"/>
+      <c r="X78" s="11"/>
+      <c r="Y78" s="11"/>
+      <c r="Z78" s="11"/>
+      <c r="AA78" s="11"/>
+      <c r="AB78" s="11"/>
+      <c r="AC78" s="11"/>
+      <c r="AD78" s="11"/>
     </row>
     <row r="79">
-      <c r="B79" s="19"/>
+      <c r="A79" s="12" t="s">
+        <v>406</v>
+      </c>
+      <c r="B79" s="12" t="s">
+        <v>407</v>
+      </c>
+      <c r="C79" s="12" t="s">
+        <v>408</v>
+      </c>
+      <c r="D79" s="11"/>
+      <c r="E79" s="12" t="s">
+        <v>399</v>
+      </c>
+      <c r="F79" s="11"/>
+      <c r="G79" s="11"/>
+      <c r="H79" s="11"/>
+      <c r="I79" s="11"/>
+      <c r="J79" s="11"/>
+      <c r="K79" s="17">
+        <v>45431.0</v>
+      </c>
+      <c r="L79" s="11"/>
+      <c r="M79" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N79" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="O79" s="11"/>
+      <c r="P79" s="11"/>
+      <c r="Q79" s="11"/>
+      <c r="R79" s="11"/>
+      <c r="S79" s="11"/>
+      <c r="T79" s="11"/>
+      <c r="U79" s="11"/>
+      <c r="V79" s="11"/>
+      <c r="W79" s="11"/>
+      <c r="X79" s="11"/>
+      <c r="Y79" s="11"/>
+      <c r="Z79" s="11"/>
+      <c r="AA79" s="11"/>
+      <c r="AB79" s="11"/>
+      <c r="AC79" s="11"/>
+      <c r="AD79" s="11"/>
     </row>
     <row r="80">
-      <c r="B80" s="19"/>
+      <c r="A80" s="12" t="s">
+        <v>409</v>
+      </c>
+      <c r="B80" s="12" t="s">
+        <v>410</v>
+      </c>
+      <c r="C80" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="D80" s="11"/>
+      <c r="E80" s="12" t="s">
+        <v>399</v>
+      </c>
+      <c r="F80" s="11"/>
+      <c r="G80" s="11"/>
+      <c r="H80" s="11"/>
+      <c r="I80" s="11"/>
+      <c r="J80" s="11"/>
+      <c r="K80" s="17">
+        <v>45431.0</v>
+      </c>
+      <c r="L80" s="11"/>
+      <c r="M80" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N80" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="O80" s="11"/>
+      <c r="P80" s="11"/>
+      <c r="Q80" s="11"/>
+      <c r="R80" s="11"/>
+      <c r="S80" s="11"/>
+      <c r="T80" s="11"/>
+      <c r="U80" s="11"/>
+      <c r="V80" s="11"/>
+      <c r="W80" s="11"/>
+      <c r="X80" s="11"/>
+      <c r="Y80" s="11"/>
+      <c r="Z80" s="11"/>
+      <c r="AA80" s="11"/>
+      <c r="AB80" s="11"/>
+      <c r="AC80" s="11"/>
+      <c r="AD80" s="11"/>
     </row>
     <row r="81">
       <c r="B81" s="19"/>
@@ -15333,71 +15683,54 @@
     <row r="870">
       <c r="B870" s="19"/>
     </row>
+    <row r="871">
+      <c r="B871" s="19"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A49:AD72">
+  <conditionalFormatting sqref="A50:AD73">
     <cfRule type="expression" dxfId="2" priority="1">
-      <formula>$M49="modified"</formula>
+      <formula>$M50="modified"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A49:AD72">
+  <conditionalFormatting sqref="A50:AD73">
     <cfRule type="expression" dxfId="3" priority="2">
-      <formula>$M49="deprecated"</formula>
+      <formula>$M50="deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A49:AB72">
+  <conditionalFormatting sqref="A50:AB73">
     <cfRule type="expression" dxfId="0" priority="3">
-      <formula>$M49="proposed"</formula>
+      <formula>$M50="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A49:AD72">
+  <conditionalFormatting sqref="A1:AD200">
     <cfRule type="expression" dxfId="1" priority="4">
-      <formula>$M49="accepted"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:C48 D2:D49 E2:AD48 D61 D65 D69 A73:AD193">
-    <cfRule type="expression" dxfId="0" priority="5">
-      <formula>$M2="proposed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:C48 D2:D49 E2:AD48 D61 D65 D69">
-    <cfRule type="expression" dxfId="1" priority="6">
-      <formula>$M2="accepted"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M2:N48 AC2:AD48 A12:C48 D12:D49 E12:L48 O12:AB48 D61 D65 D69 A73:AD192">
-    <cfRule type="expression" dxfId="2" priority="7">
-      <formula>$M2="changed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M2:N48 AC2:AD48 A12:C48 D12:D49 E12:L48 O12:AB48 D61 D65 D69 A73:AD192">
-    <cfRule type="expression" dxfId="3" priority="8">
-      <formula>$M2="deprecated"</formula>
+      <formula>$M1="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="O2"/>
     <hyperlink r:id="rId2" ref="O4"/>
     <hyperlink r:id="rId3" ref="O5"/>
-    <hyperlink r:id="rId4" ref="O6"/>
-    <hyperlink r:id="rId5" ref="O7"/>
-    <hyperlink r:id="rId6" ref="O8"/>
-    <hyperlink r:id="rId7" ref="O11"/>
-    <hyperlink r:id="rId8" ref="O12"/>
-    <hyperlink r:id="rId9" ref="O13"/>
-    <hyperlink r:id="rId10" ref="O14"/>
-    <hyperlink r:id="rId11" ref="O15"/>
-    <hyperlink r:id="rId12" ref="O16"/>
-    <hyperlink r:id="rId13" ref="O20"/>
-    <hyperlink r:id="rId14" ref="O21"/>
-    <hyperlink r:id="rId15" ref="O22"/>
-    <hyperlink r:id="rId16" ref="O23"/>
-    <hyperlink r:id="rId17" ref="O25"/>
-    <hyperlink r:id="rId18" ref="O26"/>
-    <hyperlink r:id="rId19" ref="O27"/>
-    <hyperlink r:id="rId20" ref="O28"/>
-    <hyperlink r:id="rId21" ref="O29"/>
-    <hyperlink r:id="rId22" ref="O30"/>
-    <hyperlink r:id="rId23" ref="O31"/>
+    <hyperlink r:id="rId4" ref="O7"/>
+    <hyperlink r:id="rId5" ref="O8"/>
+    <hyperlink r:id="rId6" ref="O9"/>
+    <hyperlink r:id="rId7" ref="O12"/>
+    <hyperlink r:id="rId8" ref="O13"/>
+    <hyperlink r:id="rId9" ref="O14"/>
+    <hyperlink r:id="rId10" ref="O15"/>
+    <hyperlink r:id="rId11" ref="O16"/>
+    <hyperlink r:id="rId12" ref="O17"/>
+    <hyperlink r:id="rId13" ref="O21"/>
+    <hyperlink r:id="rId14" ref="O22"/>
+    <hyperlink r:id="rId15" ref="O23"/>
+    <hyperlink r:id="rId16" ref="O24"/>
+    <hyperlink r:id="rId17" ref="O26"/>
+    <hyperlink r:id="rId18" ref="O27"/>
+    <hyperlink r:id="rId19" ref="O28"/>
+    <hyperlink r:id="rId20" ref="O29"/>
+    <hyperlink r:id="rId21" ref="O30"/>
+    <hyperlink r:id="rId22" ref="O31"/>
+    <hyperlink r:id="rId23" ref="O32"/>
   </hyperlinks>
   <drawing r:id="rId24"/>
 </worksheet>
@@ -15471,13 +15804,13 @@
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>390</v>
+        <v>412</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>391</v>
+        <v>413</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>392</v>
+        <v>414</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>17</v>
@@ -15523,22 +15856,22 @@
     </row>
     <row r="3">
       <c r="A3" s="12" t="s">
-        <v>393</v>
+        <v>415</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>394</v>
+        <v>416</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>395</v>
+        <v>417</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>396</v>
+        <v>418</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -15575,13 +15908,13 @@
     </row>
     <row r="4">
       <c r="A4" s="12" t="s">
-        <v>397</v>
+        <v>419</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>398</v>
+        <v>420</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>399</v>
+        <v>421</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>17</v>
@@ -15590,7 +15923,7 @@
         <v>202</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>396</v>
+        <v>418</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
@@ -15627,22 +15960,22 @@
     </row>
     <row r="5">
       <c r="A5" s="12" t="s">
-        <v>400</v>
+        <v>422</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>401</v>
+        <v>423</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>402</v>
+        <v>424</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>396</v>
+        <v>418</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -15659,7 +15992,7 @@
         <v>50</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>403</v>
+        <v>425</v>
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
@@ -15679,22 +16012,22 @@
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>404</v>
+        <v>426</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>405</v>
+        <v>427</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>406</v>
+        <v>428</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>407</v>
+        <v>429</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
@@ -15729,22 +16062,22 @@
     </row>
     <row r="7">
       <c r="A7" s="12" t="s">
-        <v>408</v>
+        <v>430</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>409</v>
+        <v>431</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>410</v>
+        <v>432</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>396</v>
+        <v>418</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -15779,22 +16112,22 @@
     </row>
     <row r="8">
       <c r="A8" s="12" t="s">
-        <v>411</v>
+        <v>433</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>412</v>
+        <v>434</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>413</v>
+        <v>435</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>396</v>
+        <v>418</v>
       </c>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
@@ -15829,22 +16162,22 @@
     </row>
     <row r="9">
       <c r="A9" s="12" t="s">
-        <v>414</v>
+        <v>436</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>415</v>
+        <v>437</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>416</v>
+        <v>438</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>396</v>
+        <v>418</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
@@ -15879,22 +16212,22 @@
     </row>
     <row r="10">
       <c r="A10" s="12" t="s">
-        <v>417</v>
+        <v>439</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>418</v>
+        <v>440</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>419</v>
+        <v>441</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>396</v>
+        <v>418</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
@@ -15929,13 +16262,13 @@
     </row>
     <row r="11">
       <c r="A11" s="12" t="s">
-        <v>420</v>
+        <v>442</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>421</v>
+        <v>443</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>422</v>
+        <v>444</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>17</v>
@@ -15958,13 +16291,13 @@
     </row>
     <row r="12">
       <c r="A12" s="12" t="s">
-        <v>423</v>
+        <v>445</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>424</v>
+        <v>446</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>425</v>
+        <v>447</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>17</v>
@@ -15987,13 +16320,13 @@
     </row>
     <row r="13">
       <c r="A13" s="12" t="s">
-        <v>426</v>
+        <v>448</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>427</v>
+        <v>449</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>428</v>
+        <v>450</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
updates DPV spec for v2 (module pages not updated)
- updates the main DPV spec page with content:
- scope change for v2
- updated diagram
- new sections for v2 e.g. Process, Automation, Entity Involvement
- examples for Process
- fixes broken links to module pages
- Primer: updates example for consistency with DPV spec, removes old
  diagram for serialisations
</commit_message>
<xml_diff>
--- a/code/vocab_csv/context_status.xlsx
+++ b/code/vocab_csv/context_status.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="456">
   <si>
     <t>Term</t>
   </si>
@@ -1320,7 +1320,7 @@
     <t>Indicates whether the specified context was intended or unintended</t>
   </si>
   <si>
-    <t>hasExpecation</t>
+    <t>hasExpectation</t>
   </si>
   <si>
     <t>has expectation</t>
@@ -1329,10 +1329,10 @@
     <t>Indicates whether the specified context was expected or unexpected</t>
   </si>
   <si>
-    <t>hasInvolvementStatus</t>
-  </si>
-  <si>
-    <t>has involvement status</t>
+    <t>hasInvolvement</t>
+  </si>
+  <si>
+    <t>has involvement</t>
   </si>
   <si>
     <t>Indicates the involvement status for the specified context</t>
@@ -1369,6 +1369,33 @@
   </si>
   <si>
     <t>Indicates the indicated entity is not involved in the specified context</t>
+  </si>
+  <si>
+    <t>hasConformanceStatus</t>
+  </si>
+  <si>
+    <t>has conformance status</t>
+  </si>
+  <si>
+    <t>Indicates the status of being conformant or non-conformant</t>
+  </si>
+  <si>
+    <t>hasRequestStatus</t>
+  </si>
+  <si>
+    <t>has request status</t>
+  </si>
+  <si>
+    <t>Indicates the status associated with a request</t>
+  </si>
+  <si>
+    <t>hasNotificationStatus</t>
+  </si>
+  <si>
+    <t>has notification status</t>
+  </si>
+  <si>
+    <t>Indicates the status associated with a notice</t>
   </si>
 </sst>
 </file>
@@ -16149,7 +16176,9 @@
       <c r="K9" s="14">
         <v>45422.0</v>
       </c>
-      <c r="L9" s="11"/>
+      <c r="L9" s="17">
+        <v>45453.0</v>
+      </c>
       <c r="M9" s="12" t="s">
         <v>20</v>
       </c>
@@ -16311,13 +16340,91 @@
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="19"/>
+      <c r="A14" s="12" t="s">
+        <v>447</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>448</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>449</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="K14" s="17">
+        <v>45453.0</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" s="12" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="15">
-      <c r="B15" s="19"/>
+      <c r="A15" s="12" t="s">
+        <v>450</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>451</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="K15" s="17">
+        <v>45453.0</v>
+      </c>
+      <c r="M15" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N15" s="12" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="16">
-      <c r="B16" s="19"/>
+      <c r="A16" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>454</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>455</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>393</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="K16" s="17">
+        <v>45453.0</v>
+      </c>
+      <c r="M16" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N16" s="12" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="17">
       <c r="B17" s="19"/>

</xml_diff>

<commit_message>
adds Notice concepts to DPV
- adds Notice types e.g. LayeredNotice
- adds NoticeLayer and hasNoticeLayer
- adds NoticeIcon and hasNoticeIcon
- adds new section DPV HTML called "Notice"
- moves notice concepts into a separate module called 'notice' - was in
  organisational concepts before
- minot costmetic change to search.html
</commit_message>
<xml_diff>
--- a/code/vocab_csv/context_status.xlsx
+++ b/code/vocab_csv/context_status.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="460">
   <si>
     <t>Term</t>
   </si>
@@ -502,6 +502,18 @@
   </si>
   <si>
     <t>https://www.w3.org/2022/03/02-dpvcg-minutes.html</t>
+  </si>
+  <si>
+    <t>isDuring</t>
+  </si>
+  <si>
+    <t>is during</t>
+  </si>
+  <si>
+    <t>Indicates the specified concepts occur 'during' this concept in some context</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/meetings/meeting-2024-08-13</t>
   </si>
   <si>
     <t>isAfter</t>
@@ -6618,17 +6630,17 @@
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
       <c r="K7" s="17">
-        <v>44622.0</v>
+        <v>45517.0</v>
       </c>
       <c r="L7" s="11"/>
       <c r="M7" s="12" t="s">
         <v>20</v>
       </c>
       <c r="N7" s="18" t="s">
-        <v>156</v>
+        <v>50</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
@@ -6648,21 +6660,21 @@
     </row>
     <row r="8">
       <c r="A8" s="12" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="D8" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="D8" s="44" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="F8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="44" t="s">
         <v>138</v>
       </c>
       <c r="G8" s="11"/>
@@ -6670,17 +6682,17 @@
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
       <c r="K8" s="17">
-        <v>44727.0</v>
+        <v>44622.0</v>
       </c>
       <c r="L8" s="11"/>
       <c r="M8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="12" t="s">
-        <v>50</v>
+      <c r="N8" s="18" t="s">
+        <v>156</v>
       </c>
       <c r="O8" s="16" t="s">
-        <v>51</v>
+        <v>157</v>
       </c>
       <c r="P8" s="11"/>
       <c r="Q8" s="11"/>
@@ -6764,7 +6776,7 @@
         <v>17</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>17</v>
+        <v>172</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>138</v>
@@ -6774,7 +6786,7 @@
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
       <c r="K10" s="17">
-        <v>44699.0</v>
+        <v>44727.0</v>
       </c>
       <c r="L10" s="11"/>
       <c r="M10" s="12" t="s">
@@ -6783,8 +6795,8 @@
       <c r="N10" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O10" s="45" t="s">
-        <v>172</v>
+      <c r="O10" s="16" t="s">
+        <v>51</v>
       </c>
       <c r="P10" s="11"/>
       <c r="Q10" s="11"/>
@@ -6806,17 +6818,17 @@
       <c r="A11" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="12" t="s">
         <v>175</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>164</v>
+        <v>17</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>138</v>
@@ -6826,16 +6838,18 @@
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
       <c r="K11" s="17">
-        <v>45395.0</v>
+        <v>44699.0</v>
       </c>
       <c r="L11" s="11"/>
       <c r="M11" s="12" t="s">
         <v>20</v>
       </c>
       <c r="N11" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="O11" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="O11" s="11"/>
       <c r="P11" s="11"/>
       <c r="Q11" s="11"/>
       <c r="R11" s="11"/>
@@ -6866,7 +6880,7 @@
         <v>17</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>138</v>
@@ -6883,7 +6897,7 @@
         <v>20</v>
       </c>
       <c r="N12" s="12" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="O12" s="11"/>
       <c r="P12" s="11"/>
@@ -6904,19 +6918,19 @@
     </row>
     <row r="13">
       <c r="A13" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="B13" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="B13" s="12" t="s">
         <v>182</v>
+      </c>
+      <c r="C13" s="46" t="s">
+        <v>183</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>33</v>
+        <v>168</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>138</v>
@@ -6933,7 +6947,7 @@
         <v>20</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>50</v>
+        <v>180</v>
       </c>
       <c r="O13" s="11"/>
       <c r="P13" s="11"/>
@@ -6953,20 +6967,20 @@
       <c r="AD13" s="11"/>
     </row>
     <row r="14">
-      <c r="A14" s="47" t="s">
-        <v>183</v>
+      <c r="A14" s="12" t="s">
+        <v>184</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>138</v>
@@ -7004,19 +7018,19 @@
     </row>
     <row r="15">
       <c r="A15" s="47" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>121</v>
+        <v>42</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>138</v>
@@ -7026,7 +7040,7 @@
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
       <c r="K15" s="17">
-        <v>45162.0</v>
+        <v>45395.0</v>
       </c>
       <c r="L15" s="11"/>
       <c r="M15" s="12" t="s">
@@ -7053,11 +7067,58 @@
       <c r="AD15" s="11"/>
     </row>
     <row r="16">
-      <c r="B16" s="13"/>
-      <c r="K16" s="14"/>
+      <c r="A16" s="47" t="s">
+        <v>190</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="17">
+        <v>45162.0</v>
+      </c>
+      <c r="L16" s="11"/>
+      <c r="M16" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N16" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+      <c r="V16" s="11"/>
+      <c r="W16" s="11"/>
+      <c r="X16" s="11"/>
+      <c r="Y16" s="11"/>
+      <c r="Z16" s="11"/>
+      <c r="AA16" s="11"/>
+      <c r="AB16" s="11"/>
+      <c r="AC16" s="11"/>
+      <c r="AD16" s="11"/>
     </row>
     <row r="17">
-      <c r="B17" s="19"/>
+      <c r="B17" s="13"/>
+      <c r="K17" s="14"/>
     </row>
     <row r="18">
       <c r="B18" s="19"/>
@@ -9891,38 +9952,41 @@
     <row r="961">
       <c r="B961" s="19"/>
     </row>
+    <row r="962">
+      <c r="B962" s="19"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:AD191">
+  <conditionalFormatting sqref="A2:AD192">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>$M2="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AD191">
+  <conditionalFormatting sqref="A2:AD192">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>$M2="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AD191">
+  <conditionalFormatting sqref="A2:AD192">
     <cfRule type="expression" dxfId="4" priority="3">
       <formula>$M2="deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC11:AD12">
+  <conditionalFormatting sqref="AC12:AD13">
     <cfRule type="expression" dxfId="2" priority="4">
-      <formula>$M11="changed"</formula>
+      <formula>$M12="changed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC11:AD12">
+  <conditionalFormatting sqref="AC12:AD13">
     <cfRule type="expression" dxfId="3" priority="5">
-      <formula>$M11="deprecated"</formula>
+      <formula>$M12="deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC11:AD12">
+  <conditionalFormatting sqref="AC12:AD13">
     <cfRule type="expression" dxfId="1" priority="6">
-      <formula>$M11="accepted"</formula>
+      <formula>$M12="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AD191">
+  <conditionalFormatting sqref="A2:AD192">
     <cfRule type="expression" dxfId="5" priority="7">
       <formula>$M2="changed"</formula>
     </cfRule>
@@ -9938,8 +10002,9 @@
     <hyperlink r:id="rId8" ref="O8"/>
     <hyperlink r:id="rId9" ref="O9"/>
     <hyperlink r:id="rId10" ref="O10"/>
+    <hyperlink r:id="rId11" ref="O11"/>
   </hyperlinks>
-  <drawing r:id="rId11"/>
+  <drawing r:id="rId12"/>
 </worksheet>
 </file>
 
@@ -10019,7 +10084,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>25</v>
@@ -10043,7 +10108,7 @@
         <v>50</v>
       </c>
       <c r="O2" s="45" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
@@ -10075,16 +10140,16 @@
     </row>
     <row r="4">
       <c r="A4" s="15" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>26</v>
@@ -10105,7 +10170,7 @@
         <v>50</v>
       </c>
       <c r="O4" s="45" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
@@ -10125,17 +10190,17 @@
     </row>
     <row r="5">
       <c r="A5" s="12" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="12" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
@@ -10155,7 +10220,7 @@
         <v>50</v>
       </c>
       <c r="O5" s="45" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
@@ -10175,17 +10240,17 @@
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="12" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
@@ -10221,17 +10286,17 @@
     </row>
     <row r="7">
       <c r="A7" s="12" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="12" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
@@ -10249,7 +10314,7 @@
         <v>50</v>
       </c>
       <c r="O7" s="45" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
@@ -10269,17 +10334,17 @@
     </row>
     <row r="8">
       <c r="A8" s="12" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="12" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
@@ -10297,7 +10362,7 @@
         <v>50</v>
       </c>
       <c r="O8" s="45" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="P8" s="11"/>
       <c r="Q8" s="11"/>
@@ -10317,17 +10382,17 @@
     </row>
     <row r="9">
       <c r="A9" s="50" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="B9" s="51" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="12" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="F9" s="52"/>
       <c r="G9" s="52"/>
@@ -10345,7 +10410,7 @@
         <v>50</v>
       </c>
       <c r="O9" s="45" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="P9" s="52"/>
       <c r="Q9" s="52"/>
@@ -10365,17 +10430,17 @@
     </row>
     <row r="10">
       <c r="A10" s="12" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="18" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
@@ -10425,16 +10490,16 @@
     </row>
     <row r="12">
       <c r="A12" s="15" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="D12" s="44" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>26</v>
@@ -10455,7 +10520,7 @@
         <v>50</v>
       </c>
       <c r="O12" s="45" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="P12" s="11"/>
       <c r="Q12" s="11"/>
@@ -10475,17 +10540,17 @@
     </row>
     <row r="13">
       <c r="A13" s="12" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="12" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
@@ -10503,7 +10568,7 @@
         <v>50</v>
       </c>
       <c r="O13" s="45" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="P13" s="11"/>
       <c r="Q13" s="11"/>
@@ -10523,46 +10588,46 @@
     </row>
     <row r="14">
       <c r="A14" s="12" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="K14" s="17">
         <v>44699.0</v>
       </c>
       <c r="M14" s="12" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="N14" s="12" t="s">
         <v>50</v>
       </c>
       <c r="O14" s="45" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="12" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="12" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
@@ -10580,7 +10645,7 @@
         <v>50</v>
       </c>
       <c r="O15" s="45" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="P15" s="11"/>
       <c r="Q15" s="11"/>
@@ -10600,23 +10665,23 @@
     </row>
     <row r="16">
       <c r="A16" s="12" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="12" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
       <c r="I16" s="12" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="J16" s="11"/>
       <c r="K16" s="17">
@@ -10632,7 +10697,7 @@
         <v>50</v>
       </c>
       <c r="O16" s="45" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="P16" s="11"/>
       <c r="Q16" s="11"/>
@@ -10652,23 +10717,23 @@
     </row>
     <row r="17">
       <c r="A17" s="12" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="12" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
       <c r="I17" s="12" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="J17" s="11"/>
       <c r="K17" s="17">
@@ -10684,7 +10749,7 @@
         <v>50</v>
       </c>
       <c r="O17" s="45" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="P17" s="11"/>
       <c r="Q17" s="11"/>
@@ -10704,17 +10769,17 @@
     </row>
     <row r="18">
       <c r="A18" s="12" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="12" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
@@ -10750,17 +10815,17 @@
     </row>
     <row r="19">
       <c r="A19" s="12" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="12" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
@@ -10803,16 +10868,16 @@
     </row>
     <row r="21">
       <c r="A21" s="15" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>26</v>
@@ -10833,7 +10898,7 @@
         <v>50</v>
       </c>
       <c r="O21" s="16" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="P21" s="11"/>
       <c r="Q21" s="11"/>
@@ -10853,17 +10918,17 @@
     </row>
     <row r="22">
       <c r="A22" s="12" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="12" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
@@ -10881,7 +10946,7 @@
         <v>50</v>
       </c>
       <c r="O22" s="16" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="P22" s="11"/>
       <c r="Q22" s="11"/>
@@ -10901,17 +10966,17 @@
     </row>
     <row r="23">
       <c r="A23" s="12" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="12" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
@@ -10929,7 +10994,7 @@
         <v>50</v>
       </c>
       <c r="O23" s="16" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="P23" s="11"/>
       <c r="Q23" s="11"/>
@@ -10949,17 +11014,17 @@
     </row>
     <row r="24">
       <c r="A24" s="13" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="12" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
@@ -10977,7 +11042,7 @@
         <v>50</v>
       </c>
       <c r="O24" s="16" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="P24" s="11"/>
       <c r="Q24" s="11"/>
@@ -11000,16 +11065,16 @@
     </row>
     <row r="26">
       <c r="A26" s="15" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="D26" s="44" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>26</v>
@@ -11030,7 +11095,7 @@
         <v>50</v>
       </c>
       <c r="O26" s="45" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="P26" s="11"/>
       <c r="Q26" s="11"/>
@@ -11050,17 +11115,17 @@
     </row>
     <row r="27">
       <c r="A27" s="12" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="12" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
@@ -11078,7 +11143,7 @@
         <v>50</v>
       </c>
       <c r="O27" s="45" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="P27" s="11"/>
       <c r="Q27" s="11"/>
@@ -11098,23 +11163,23 @@
     </row>
     <row r="28">
       <c r="A28" s="12" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="12" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
       <c r="I28" s="12" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="J28" s="11"/>
       <c r="K28" s="17">
@@ -11125,10 +11190,10 @@
         <v>20</v>
       </c>
       <c r="N28" s="12" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="O28" s="45" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="P28" s="11"/>
       <c r="Q28" s="11"/>
@@ -11148,17 +11213,17 @@
     </row>
     <row r="29">
       <c r="A29" s="12" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="12" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
@@ -11176,7 +11241,7 @@
         <v>50</v>
       </c>
       <c r="O29" s="45" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="P29" s="11"/>
       <c r="Q29" s="11"/>
@@ -11196,17 +11261,17 @@
     </row>
     <row r="30">
       <c r="A30" s="12" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="D30" s="11"/>
       <c r="E30" s="12" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
@@ -11224,7 +11289,7 @@
         <v>50</v>
       </c>
       <c r="O30" s="45" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="P30" s="11"/>
       <c r="Q30" s="11"/>
@@ -11244,17 +11309,17 @@
     </row>
     <row r="31">
       <c r="A31" s="12" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="D31" s="11"/>
       <c r="E31" s="12" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
@@ -11272,7 +11337,7 @@
         <v>50</v>
       </c>
       <c r="O31" s="45" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="P31" s="11"/>
       <c r="Q31" s="11"/>
@@ -11292,17 +11357,17 @@
     </row>
     <row r="32">
       <c r="A32" s="12" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="D32" s="11"/>
       <c r="E32" s="12" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="F32" s="11"/>
       <c r="G32" s="11"/>
@@ -11320,7 +11385,7 @@
         <v>50</v>
       </c>
       <c r="O32" s="45" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="P32" s="11"/>
       <c r="Q32" s="11"/>
@@ -11343,16 +11408,16 @@
     </row>
     <row r="34">
       <c r="A34" s="15" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="E34" s="12" t="s">
         <v>26</v>
@@ -11391,17 +11456,17 @@
     </row>
     <row r="35">
       <c r="A35" s="12" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="D35" s="11"/>
       <c r="E35" s="12" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
@@ -11437,17 +11502,17 @@
     </row>
     <row r="36">
       <c r="A36" s="12" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="D36" s="11"/>
       <c r="E36" s="12" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
@@ -11486,16 +11551,16 @@
     </row>
     <row r="38">
       <c r="A38" s="15" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="E38" s="12" t="s">
         <v>26</v>
@@ -11534,17 +11599,17 @@
     </row>
     <row r="39">
       <c r="A39" s="12" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="D39" s="11"/>
       <c r="E39" s="12" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="F39" s="11"/>
       <c r="G39" s="11"/>
@@ -11580,17 +11645,17 @@
     </row>
     <row r="40">
       <c r="A40" s="12" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="12" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
@@ -11626,17 +11691,17 @@
     </row>
     <row r="41">
       <c r="A41" s="12" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="D41" s="11"/>
       <c r="E41" s="12" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="F41" s="11"/>
       <c r="G41" s="11"/>
@@ -11672,17 +11737,17 @@
     </row>
     <row r="42">
       <c r="A42" s="12" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="12" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
@@ -11718,17 +11783,17 @@
     </row>
     <row r="43">
       <c r="A43" s="12" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="D43" s="11"/>
       <c r="E43" s="12" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="F43" s="11"/>
       <c r="G43" s="11"/>
@@ -11764,17 +11829,17 @@
     </row>
     <row r="44">
       <c r="A44" s="12" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="D44" s="11"/>
       <c r="E44" s="12" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="F44" s="11"/>
       <c r="G44" s="11"/>
@@ -11810,17 +11875,17 @@
     </row>
     <row r="45">
       <c r="A45" s="12" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="D45" s="11"/>
       <c r="E45" s="12" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
@@ -11856,17 +11921,17 @@
     </row>
     <row r="46">
       <c r="A46" s="12" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="D46" s="11"/>
       <c r="E46" s="12" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="F46" s="11"/>
       <c r="G46" s="11"/>
@@ -11902,17 +11967,17 @@
     </row>
     <row r="47">
       <c r="A47" s="12" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="D47" s="11"/>
       <c r="E47" s="12" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="F47" s="11"/>
       <c r="G47" s="11"/>
@@ -11948,17 +12013,17 @@
     </row>
     <row r="48">
       <c r="A48" s="18" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="D48" s="11"/>
       <c r="E48" s="12" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="F48" s="11"/>
       <c r="G48" s="11"/>
@@ -11998,16 +12063,16 @@
     </row>
     <row r="50">
       <c r="A50" s="15" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="E50" s="12" t="s">
         <v>26</v>
@@ -12025,7 +12090,7 @@
         <v>20</v>
       </c>
       <c r="N50" s="12" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="O50" s="11"/>
       <c r="P50" s="11"/>
@@ -12046,16 +12111,16 @@
     </row>
     <row r="51">
       <c r="A51" s="15" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="E51" s="12" t="s">
         <v>18</v>
@@ -12073,7 +12138,7 @@
         <v>20</v>
       </c>
       <c r="N51" s="12" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="O51" s="11"/>
       <c r="P51" s="11"/>
@@ -12094,19 +12159,19 @@
     </row>
     <row r="52">
       <c r="A52" s="12" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="D52" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="E52" s="12" t="s">
         <v>329</v>
-      </c>
-      <c r="E52" s="12" t="s">
-        <v>325</v>
       </c>
       <c r="F52" s="11"/>
       <c r="G52" s="11"/>
@@ -12121,7 +12186,7 @@
         <v>20</v>
       </c>
       <c r="N52" s="12" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="O52" s="11"/>
       <c r="P52" s="11"/>
@@ -12142,19 +12207,19 @@
     </row>
     <row r="53">
       <c r="A53" s="12" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="D53" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="E53" s="12" t="s">
         <v>329</v>
-      </c>
-      <c r="E53" s="12" t="s">
-        <v>325</v>
       </c>
       <c r="F53" s="11"/>
       <c r="G53" s="11"/>
@@ -12169,7 +12234,7 @@
         <v>20</v>
       </c>
       <c r="N53" s="12" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="O53" s="11"/>
       <c r="P53" s="11"/>
@@ -12190,19 +12255,19 @@
     </row>
     <row r="54">
       <c r="A54" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="D54" s="12" t="s">
         <v>333</v>
       </c>
-      <c r="B54" s="12" t="s">
-        <v>334</v>
-      </c>
-      <c r="C54" s="12" t="s">
-        <v>335</v>
-      </c>
-      <c r="D54" s="12" t="s">
+      <c r="E54" s="12" t="s">
         <v>329</v>
-      </c>
-      <c r="E54" s="12" t="s">
-        <v>325</v>
       </c>
       <c r="F54" s="11"/>
       <c r="G54" s="11"/>
@@ -12217,7 +12282,7 @@
         <v>20</v>
       </c>
       <c r="N54" s="12" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="O54" s="11"/>
       <c r="P54" s="11"/>
@@ -12238,19 +12303,19 @@
     </row>
     <row r="55">
       <c r="A55" s="12" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="D55" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="E55" s="12" t="s">
         <v>329</v>
-      </c>
-      <c r="E55" s="12" t="s">
-        <v>325</v>
       </c>
       <c r="F55" s="11"/>
       <c r="G55" s="11"/>
@@ -12265,7 +12330,7 @@
         <v>20</v>
       </c>
       <c r="N55" s="12" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="O55" s="11"/>
       <c r="P55" s="11"/>
@@ -12286,16 +12351,16 @@
     </row>
     <row r="56">
       <c r="A56" s="15" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="E56" s="12" t="s">
         <v>26</v>
@@ -12313,7 +12378,7 @@
         <v>20</v>
       </c>
       <c r="N56" s="12" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="O56" s="11"/>
       <c r="P56" s="11"/>
@@ -12334,19 +12399,19 @@
     </row>
     <row r="57">
       <c r="A57" s="12" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="F57" s="11"/>
       <c r="G57" s="11"/>
@@ -12361,7 +12426,7 @@
         <v>20</v>
       </c>
       <c r="N57" s="12" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="O57" s="11"/>
       <c r="P57" s="11"/>
@@ -12382,19 +12447,19 @@
     </row>
     <row r="58">
       <c r="A58" s="12" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="F58" s="11"/>
       <c r="G58" s="11"/>
@@ -12409,7 +12474,7 @@
         <v>20</v>
       </c>
       <c r="N58" s="12" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="O58" s="11"/>
       <c r="P58" s="11"/>
@@ -12430,19 +12495,19 @@
     </row>
     <row r="59">
       <c r="A59" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>354</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="D59" s="12" t="s">
         <v>349</v>
       </c>
-      <c r="B59" s="12" t="s">
-        <v>350</v>
-      </c>
-      <c r="C59" s="12" t="s">
-        <v>351</v>
-      </c>
-      <c r="D59" s="12" t="s">
-        <v>345</v>
-      </c>
       <c r="E59" s="12" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="F59" s="11"/>
       <c r="G59" s="11"/>
@@ -12457,7 +12522,7 @@
         <v>20</v>
       </c>
       <c r="N59" s="12" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="O59" s="11"/>
       <c r="P59" s="11"/>
@@ -12478,19 +12543,19 @@
     </row>
     <row r="60">
       <c r="A60" s="12" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="F60" s="11"/>
       <c r="G60" s="11"/>
@@ -12505,7 +12570,7 @@
         <v>20</v>
       </c>
       <c r="N60" s="12" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="O60" s="11"/>
       <c r="P60" s="11"/>
@@ -12530,16 +12595,16 @@
     </row>
     <row r="62">
       <c r="A62" s="15" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="E62" s="12" t="s">
         <v>26</v>
@@ -12548,7 +12613,7 @@
       <c r="G62" s="11"/>
       <c r="H62" s="11"/>
       <c r="I62" s="12" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="J62" s="11"/>
       <c r="K62" s="17">
@@ -12559,7 +12624,7 @@
         <v>20</v>
       </c>
       <c r="N62" s="12" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="O62" s="11"/>
       <c r="P62" s="11"/>
@@ -12580,16 +12645,16 @@
     </row>
     <row r="63">
       <c r="A63" s="12" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="E63" s="12" t="s">
         <v>18</v>
@@ -12607,7 +12672,7 @@
         <v>20</v>
       </c>
       <c r="N63" s="12" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="O63" s="11"/>
       <c r="P63" s="11"/>
@@ -12628,16 +12693,16 @@
     </row>
     <row r="64">
       <c r="A64" s="12" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="E64" s="12" t="s">
         <v>18</v>
@@ -12655,7 +12720,7 @@
         <v>20</v>
       </c>
       <c r="N64" s="12" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="O64" s="11"/>
       <c r="P64" s="11"/>
@@ -12680,23 +12745,23 @@
     </row>
     <row r="66">
       <c r="A66" s="15" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="E66" s="11"/>
       <c r="F66" s="11"/>
       <c r="G66" s="11"/>
       <c r="H66" s="11"/>
       <c r="I66" s="12" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="J66" s="11"/>
       <c r="K66" s="17">
@@ -12707,7 +12772,7 @@
         <v>20</v>
       </c>
       <c r="N66" s="12" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="O66" s="11"/>
       <c r="P66" s="11"/>
@@ -12728,16 +12793,16 @@
     </row>
     <row r="67">
       <c r="A67" s="12" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="E67" s="12" t="s">
         <v>18</v>
@@ -12755,7 +12820,7 @@
         <v>20</v>
       </c>
       <c r="N67" s="12" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="O67" s="11"/>
       <c r="P67" s="11"/>
@@ -12776,16 +12841,16 @@
     </row>
     <row r="68">
       <c r="A68" s="12" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="E68" s="12" t="s">
         <v>18</v>
@@ -12803,7 +12868,7 @@
         <v>20</v>
       </c>
       <c r="N68" s="12" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="O68" s="11"/>
       <c r="P68" s="11"/>
@@ -12828,16 +12893,16 @@
     </row>
     <row r="70">
       <c r="A70" s="15" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="E70" s="12" t="s">
         <v>26</v>
@@ -12855,7 +12920,7 @@
         <v>20</v>
       </c>
       <c r="N70" s="12" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="O70" s="11"/>
       <c r="P70" s="11"/>
@@ -12876,16 +12941,16 @@
     </row>
     <row r="71">
       <c r="A71" s="12" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="E71" s="12" t="s">
         <v>18</v>
@@ -12894,7 +12959,7 @@
       <c r="G71" s="11"/>
       <c r="H71" s="11"/>
       <c r="I71" s="12" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="J71" s="11"/>
       <c r="K71" s="17">
@@ -12905,7 +12970,7 @@
         <v>20</v>
       </c>
       <c r="N71" s="12" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="O71" s="11"/>
       <c r="P71" s="11"/>
@@ -12926,16 +12991,16 @@
     </row>
     <row r="72">
       <c r="A72" s="12" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="C72" s="12" t="s">
+        <v>386</v>
+      </c>
+      <c r="D72" s="12" t="s">
         <v>382</v>
-      </c>
-      <c r="D72" s="12" t="s">
-        <v>378</v>
       </c>
       <c r="E72" s="12" t="s">
         <v>18</v>
@@ -12944,7 +13009,7 @@
       <c r="G72" s="11"/>
       <c r="H72" s="11"/>
       <c r="I72" s="12" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="J72" s="11"/>
       <c r="K72" s="17">
@@ -12955,7 +13020,7 @@
         <v>20</v>
       </c>
       <c r="N72" s="12" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="O72" s="11"/>
       <c r="P72" s="11"/>
@@ -12976,16 +13041,16 @@
     </row>
     <row r="73">
       <c r="A73" s="12" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="D73" s="12" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="E73" s="12" t="s">
         <v>18</v>
@@ -13003,7 +13068,7 @@
         <v>20</v>
       </c>
       <c r="N73" s="12" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="O73" s="11"/>
       <c r="P73" s="11"/>
@@ -13027,16 +13092,16 @@
     </row>
     <row r="75">
       <c r="A75" s="15" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="C75" s="12" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="D75" s="12" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="E75" s="12" t="s">
         <v>26</v>
@@ -13075,17 +13140,17 @@
     </row>
     <row r="76">
       <c r="A76" s="12" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="D76" s="11"/>
       <c r="E76" s="12" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="F76" s="11"/>
       <c r="G76" s="11"/>
@@ -13121,17 +13186,17 @@
     </row>
     <row r="77">
       <c r="A77" s="12" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="D77" s="11"/>
       <c r="E77" s="12" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="F77" s="11"/>
       <c r="G77" s="11"/>
@@ -13167,17 +13232,17 @@
     </row>
     <row r="78">
       <c r="A78" s="12" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="D78" s="11"/>
       <c r="E78" s="12" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="F78" s="11"/>
       <c r="G78" s="11"/>
@@ -13213,17 +13278,17 @@
     </row>
     <row r="79">
       <c r="A79" s="12" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="C79" s="12" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="D79" s="11"/>
       <c r="E79" s="12" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="F79" s="11"/>
       <c r="G79" s="11"/>
@@ -13259,17 +13324,17 @@
     </row>
     <row r="80">
       <c r="A80" s="12" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="D80" s="11"/>
       <c r="E80" s="12" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="F80" s="11"/>
       <c r="G80" s="11"/>
@@ -15794,19 +15859,19 @@
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>138</v>
@@ -15826,7 +15891,7 @@
         <v>50</v>
       </c>
       <c r="O2" s="16" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
@@ -15846,22 +15911,22 @@
     </row>
     <row r="3">
       <c r="A3" s="12" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -15878,7 +15943,7 @@
         <v>50</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="P3" s="11"/>
       <c r="Q3" s="11"/>
@@ -15898,22 +15963,22 @@
     </row>
     <row r="4">
       <c r="A4" s="12" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
@@ -15930,7 +15995,7 @@
         <v>50</v>
       </c>
       <c r="O4" s="16" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
@@ -15950,22 +16015,22 @@
     </row>
     <row r="5">
       <c r="A5" s="12" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -15982,7 +16047,7 @@
         <v>50</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
@@ -16002,22 +16067,22 @@
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
@@ -16052,22 +16117,22 @@
     </row>
     <row r="7">
       <c r="A7" s="12" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -16102,22 +16167,22 @@
     </row>
     <row r="8">
       <c r="A8" s="12" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
@@ -16152,22 +16217,22 @@
     </row>
     <row r="9">
       <c r="A9" s="12" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
@@ -16204,22 +16269,22 @@
     </row>
     <row r="10">
       <c r="A10" s="12" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
@@ -16254,19 +16319,19 @@
     </row>
     <row r="11">
       <c r="A11" s="12" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>138</v>
@@ -16275,7 +16340,7 @@
         <v>45422.0</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="N11" s="12" t="s">
         <v>50</v>
@@ -16283,19 +16348,19 @@
     </row>
     <row r="12">
       <c r="A12" s="12" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>138</v>
@@ -16304,7 +16369,7 @@
         <v>45422.0</v>
       </c>
       <c r="M12" s="12" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="N12" s="12" t="s">
         <v>50</v>
@@ -16312,19 +16377,19 @@
     </row>
     <row r="13">
       <c r="A13" s="12" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>138</v>
@@ -16333,7 +16398,7 @@
         <v>45422.0</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="N13" s="12" t="s">
         <v>50</v>
@@ -16341,19 +16406,19 @@
     </row>
     <row r="14">
       <c r="A14" s="12" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>138</v>
@@ -16370,19 +16435,19 @@
     </row>
     <row r="15">
       <c r="A15" s="12" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>138</v>
@@ -16399,19 +16464,19 @@
     </row>
     <row r="16">
       <c r="A16" s="12" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>138</v>

</xml_diff>

<commit_message>
DPV: adds contract types and legal basis statuses
- #111 adds contract types, statuses, clause types, fulfilment status,
  and controls to DPV legal basis (but as separate modules)
- #111 adds status types for other legal bases - legitimate interest,
  legal obligation, official authority, public and vital interests
- The documentation for these concepts is NOT included in this concept
  and should be implemented after agreement on the concept structuring
- #185 adds Fee concept as `FeeRequired` in DPV. The concept is to be
  removed from the RISK extension (not implemented in this commit)
</commit_message>
<xml_diff>
--- a/code/vocab_csv/context_status.xlsx
+++ b/code/vocab_csv/context_status.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="473">
   <si>
     <t>Term</t>
   </si>
@@ -407,6 +407,36 @@
   </si>
   <si>
     <t>This concept is useful when describing situations where information is required but is not available (yet). For example, if in a form a field asks about whether a process X was completed, and it is correct to interpret that process X is applicable and must be completed, but the information is not yet available as to whether this was done - then NotAvailable is useful to represent this.</t>
+  </si>
+  <si>
+    <t>FeeRequirement</t>
+  </si>
+  <si>
+    <t>Fee Requirement</t>
+  </si>
+  <si>
+    <t>Concept indicating whether a fee is required</t>
+  </si>
+  <si>
+    <t>FeeRequired</t>
+  </si>
+  <si>
+    <t>Fee Required</t>
+  </si>
+  <si>
+    <t>Concept indicating a fee is required. The value of the fee should be specified using rdf:value or an another relevant means</t>
+  </si>
+  <si>
+    <t>dpv:FeeRequirement</t>
+  </si>
+  <si>
+    <t>FeeNotRequired</t>
+  </si>
+  <si>
+    <t>Fee Not Required</t>
+  </si>
+  <si>
+    <t>Concept indicating a fee is not required. This is distinct from a Fee of zero as it indicates a fee is not applicable in the context</t>
   </si>
   <si>
     <t>domain</t>
@@ -607,6 +637,15 @@
   </si>
   <si>
     <t>Indicates situations where the context is not applicable, information is not available, or this is unknown. An appropriate instance of dpv:Applicability should be used with this relation to express the situation</t>
+  </si>
+  <si>
+    <t>hasFee</t>
+  </si>
+  <si>
+    <t>has fee</t>
+  </si>
+  <si>
+    <t>Indicates whether a fee is required for the specified context</t>
   </si>
   <si>
     <t>The status or state of something</t>
@@ -1531,14 +1570,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEFEFEF"/>
-        <bgColor rgb="FFEFEFEF"/>
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor rgb="FFD9EAD3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9EAD3"/>
-        <bgColor rgb="FFD9EAD3"/>
+        <fgColor rgb="FFEFEFEF"/>
+        <bgColor rgb="FFEFEFEF"/>
       </patternFill>
     </fill>
   </fills>
@@ -1595,7 +1634,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1652,25 +1691,34 @@
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="3" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1697,31 +1745,31 @@
     <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="14" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="2" fontId="14" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -3778,8 +3826,77 @@
       <c r="AC41" s="11"/>
       <c r="AD41" s="11"/>
     </row>
-    <row r="66">
-      <c r="B66" s="19"/>
+    <row r="43">
+      <c r="A43" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K43" s="20">
+        <v>45531.0</v>
+      </c>
+      <c r="L43" s="21"/>
+      <c r="M43" s="22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K44" s="20">
+        <v>45531.0</v>
+      </c>
+      <c r="L44" s="21"/>
+      <c r="M44" s="22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K45" s="20">
+        <v>45531.0</v>
+      </c>
+      <c r="L45" s="21"/>
+      <c r="M45" s="22" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="67">
       <c r="B67" s="19"/>
@@ -6232,23 +6349,26 @@
     <row r="883">
       <c r="B883" s="19"/>
     </row>
+    <row r="884">
+      <c r="B884" s="19"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:AB41 A66:AB254">
+  <conditionalFormatting sqref="A2:AB41 A67:AB255">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$M2="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AD41 A66:AD274">
+  <conditionalFormatting sqref="A2:AD41 A67:AD275">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>$M2="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AD41 A66:AD204">
+  <conditionalFormatting sqref="A2:AD41 A67:AD205">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>$M2="modified"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AD41 A66:AD204">
+  <conditionalFormatting sqref="A2:AD41 A67:AD205">
     <cfRule type="expression" dxfId="3" priority="4">
       <formula>$M2="deprecated"</formula>
     </cfRule>
@@ -6300,46 +6420,46 @@
   </cols>
   <sheetData>
     <row r="1" ht="28.5" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="G1" s="20" t="s">
+      <c r="D1" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="L1" s="25" t="s">
+      <c r="K1" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="L1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="M1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="26" t="s">
+      <c r="N1" s="29" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="15" t="s">
@@ -6348,13 +6468,13 @@
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>17</v>
@@ -6363,7 +6483,7 @@
         <v>25</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
@@ -6397,120 +6517,120 @@
       <c r="AD2" s="11"/>
     </row>
     <row r="3">
-      <c r="A3" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="D3" s="27" t="s">
+      <c r="A3" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="D3" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="30" t="s">
         <v>75</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="K3" s="31">
+        <v>148</v>
+      </c>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="K3" s="34">
         <v>43560.0</v>
       </c>
-      <c r="L3" s="32"/>
+      <c r="L3" s="35"/>
       <c r="M3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="33" t="s">
-        <v>143</v>
-      </c>
-      <c r="O3" s="34" t="s">
+      <c r="N3" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="O3" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="29"/>
-      <c r="V3" s="29"/>
-      <c r="W3" s="29"/>
-      <c r="X3" s="29"/>
-      <c r="Y3" s="29"/>
-      <c r="Z3" s="29"/>
-      <c r="AA3" s="29"/>
-      <c r="AB3" s="29"/>
-      <c r="AC3" s="29"/>
-      <c r="AD3" s="29"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="32"/>
+      <c r="U3" s="32"/>
+      <c r="V3" s="32"/>
+      <c r="W3" s="32"/>
+      <c r="X3" s="32"/>
+      <c r="Y3" s="32"/>
+      <c r="Z3" s="32"/>
+      <c r="AA3" s="32"/>
+      <c r="AB3" s="32"/>
+      <c r="AC3" s="32"/>
+      <c r="AD3" s="32"/>
     </row>
     <row r="4">
-      <c r="A4" s="35" t="s">
-        <v>144</v>
-      </c>
-      <c r="B4" s="35" t="s">
-        <v>145</v>
-      </c>
-      <c r="C4" s="36" t="s">
-        <v>146</v>
-      </c>
-      <c r="D4" s="37" t="s">
+      <c r="A4" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>155</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="D4" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="40" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="40">
+        <v>148</v>
+      </c>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="43">
         <v>44160.0</v>
       </c>
-      <c r="L4" s="35"/>
+      <c r="L4" s="38"/>
       <c r="M4" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="N4" s="41" t="s">
-        <v>147</v>
-      </c>
-      <c r="O4" s="42" t="s">
-        <v>148</v>
-      </c>
-      <c r="P4" s="43"/>
-      <c r="Q4" s="43"/>
-      <c r="R4" s="38"/>
-      <c r="S4" s="38"/>
-      <c r="T4" s="38"/>
-      <c r="U4" s="38"/>
-      <c r="V4" s="38"/>
-      <c r="W4" s="38"/>
-      <c r="X4" s="38"/>
-      <c r="Y4" s="38"/>
-      <c r="Z4" s="38"/>
-      <c r="AA4" s="38"/>
-      <c r="AB4" s="38"/>
-      <c r="AC4" s="38"/>
-      <c r="AD4" s="38"/>
+      <c r="N4" s="44" t="s">
+        <v>157</v>
+      </c>
+      <c r="O4" s="45" t="s">
+        <v>158</v>
+      </c>
+      <c r="P4" s="46"/>
+      <c r="Q4" s="46"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="41"/>
+      <c r="T4" s="41"/>
+      <c r="U4" s="41"/>
+      <c r="V4" s="41"/>
+      <c r="W4" s="41"/>
+      <c r="X4" s="41"/>
+      <c r="Y4" s="41"/>
+      <c r="Z4" s="41"/>
+      <c r="AA4" s="41"/>
+      <c r="AB4" s="41"/>
+      <c r="AC4" s="41"/>
+      <c r="AD4" s="41"/>
     </row>
     <row r="5">
       <c r="A5" s="12" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>17</v>
@@ -6519,7 +6639,7 @@
         <v>60</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -6536,7 +6656,7 @@
         <v>50</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
@@ -6556,22 +6676,22 @@
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="D6" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="D6" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="44" t="s">
+      <c r="E6" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="44" t="s">
-        <v>138</v>
+      <c r="F6" s="47" t="s">
+        <v>148</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
@@ -6585,10 +6705,10 @@
         <v>20</v>
       </c>
       <c r="N6" s="12" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="P6" s="11"/>
       <c r="Q6" s="11"/>
@@ -6608,22 +6728,22 @@
     </row>
     <row r="7">
       <c r="A7" s="12" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="D7" s="44" t="s">
+        <v>170</v>
+      </c>
+      <c r="D7" s="47" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="44" t="s">
-        <v>138</v>
+      <c r="F7" s="47" t="s">
+        <v>148</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -6640,7 +6760,7 @@
         <v>50</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
@@ -6660,22 +6780,22 @@
     </row>
     <row r="8">
       <c r="A8" s="12" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="D8" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="D8" s="47" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="44" t="s">
-        <v>138</v>
+      <c r="F8" s="47" t="s">
+        <v>148</v>
       </c>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
@@ -6689,10 +6809,10 @@
         <v>20</v>
       </c>
       <c r="N8" s="18" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="O8" s="16" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="P8" s="11"/>
       <c r="Q8" s="11"/>
@@ -6712,22 +6832,22 @@
     </row>
     <row r="9">
       <c r="A9" s="12" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
@@ -6764,22 +6884,22 @@
     </row>
     <row r="10">
       <c r="A10" s="12" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
@@ -6816,13 +6936,13 @@
     </row>
     <row r="11">
       <c r="A11" s="12" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>17</v>
@@ -6831,7 +6951,7 @@
         <v>17</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -6847,8 +6967,8 @@
       <c r="N11" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O11" s="45" t="s">
-        <v>176</v>
+      <c r="O11" s="48" t="s">
+        <v>186</v>
       </c>
       <c r="P11" s="11"/>
       <c r="Q11" s="11"/>
@@ -6868,22 +6988,22 @@
     </row>
     <row r="12">
       <c r="A12" s="12" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="C12" s="46" t="s">
-        <v>179</v>
+        <v>188</v>
+      </c>
+      <c r="C12" s="49" t="s">
+        <v>189</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
@@ -6897,7 +7017,7 @@
         <v>20</v>
       </c>
       <c r="N12" s="12" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="O12" s="11"/>
       <c r="P12" s="11"/>
@@ -6918,22 +7038,22 @@
     </row>
     <row r="13">
       <c r="A13" s="12" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="C13" s="46" t="s">
-        <v>183</v>
+        <v>192</v>
+      </c>
+      <c r="C13" s="49" t="s">
+        <v>193</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
@@ -6947,7 +7067,7 @@
         <v>20</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="O13" s="11"/>
       <c r="P13" s="11"/>
@@ -6968,13 +7088,13 @@
     </row>
     <row r="14">
       <c r="A14" s="12" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>17</v>
@@ -6983,7 +7103,7 @@
         <v>33</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
@@ -7017,14 +7137,14 @@
       <c r="AD14" s="11"/>
     </row>
     <row r="15">
-      <c r="A15" s="47" t="s">
-        <v>187</v>
+      <c r="A15" s="50" t="s">
+        <v>197</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>17</v>
@@ -7033,7 +7153,7 @@
         <v>42</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
@@ -7067,14 +7187,14 @@
       <c r="AD15" s="11"/>
     </row>
     <row r="16">
-      <c r="A16" s="47" t="s">
-        <v>190</v>
+      <c r="A16" s="50" t="s">
+        <v>200</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>17</v>
@@ -7083,7 +7203,7 @@
         <v>121</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
@@ -7117,8 +7237,52 @@
       <c r="AD16" s="11"/>
     </row>
     <row r="17">
-      <c r="B17" s="13"/>
-      <c r="K17" s="14"/>
+      <c r="A17" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="20">
+        <v>45531.0</v>
+      </c>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="11"/>
+      <c r="V17" s="11"/>
+      <c r="W17" s="11"/>
+      <c r="X17" s="11"/>
+      <c r="Y17" s="11"/>
+      <c r="Z17" s="11"/>
+      <c r="AA17" s="11"/>
+      <c r="AB17" s="11"/>
+      <c r="AC17" s="11"/>
+      <c r="AD17" s="11"/>
     </row>
     <row r="18">
       <c r="B18" s="19"/>
@@ -10084,7 +10248,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>25</v>
@@ -10107,8 +10271,8 @@
       <c r="N2" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O2" s="45" t="s">
-        <v>176</v>
+      <c r="O2" s="48" t="s">
+        <v>186</v>
       </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
@@ -10136,20 +10300,20 @@
       <c r="L3" s="17"/>
       <c r="M3" s="12"/>
       <c r="N3" s="12"/>
-      <c r="O3" s="48"/>
+      <c r="O3" s="51"/>
     </row>
     <row r="4">
       <c r="A4" s="15" t="s">
-        <v>194</v>
+        <v>207</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>26</v>
@@ -10169,8 +10333,8 @@
       <c r="N4" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O4" s="45" t="s">
-        <v>176</v>
+      <c r="O4" s="48" t="s">
+        <v>186</v>
       </c>
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
@@ -10190,17 +10354,17 @@
     </row>
     <row r="5">
       <c r="A5" s="12" t="s">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>199</v>
+        <v>212</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="12" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
@@ -10219,8 +10383,8 @@
       <c r="N5" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O5" s="45" t="s">
-        <v>176</v>
+      <c r="O5" s="48" t="s">
+        <v>186</v>
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
@@ -10240,17 +10404,17 @@
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>203</v>
+        <v>216</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="12" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
@@ -10267,7 +10431,7 @@
       <c r="N6" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O6" s="48"/>
+      <c r="O6" s="51"/>
       <c r="P6" s="11"/>
       <c r="Q6" s="11"/>
       <c r="R6" s="11"/>
@@ -10286,17 +10450,17 @@
     </row>
     <row r="7">
       <c r="A7" s="12" t="s">
-        <v>205</v>
+        <v>218</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>206</v>
+        <v>219</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>207</v>
+        <v>220</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="12" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
@@ -10313,8 +10477,8 @@
       <c r="N7" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O7" s="45" t="s">
-        <v>176</v>
+      <c r="O7" s="48" t="s">
+        <v>186</v>
       </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
@@ -10334,23 +10498,23 @@
     </row>
     <row r="8">
       <c r="A8" s="12" t="s">
-        <v>208</v>
+        <v>221</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>209</v>
+        <v>222</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="12" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
-      <c r="J8" s="49"/>
+      <c r="J8" s="52"/>
       <c r="K8" s="17">
         <v>44699.0</v>
       </c>
@@ -10361,8 +10525,8 @@
       <c r="N8" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O8" s="45" t="s">
-        <v>176</v>
+      <c r="O8" s="48" t="s">
+        <v>186</v>
       </c>
       <c r="P8" s="11"/>
       <c r="Q8" s="11"/>
@@ -10381,23 +10545,23 @@
       <c r="AD8" s="11"/>
     </row>
     <row r="9">
-      <c r="A9" s="50" t="s">
-        <v>211</v>
-      </c>
-      <c r="B9" s="51" t="s">
-        <v>212</v>
-      </c>
-      <c r="C9" s="50" t="s">
-        <v>213</v>
+      <c r="A9" s="53" t="s">
+        <v>224</v>
+      </c>
+      <c r="B9" s="54" t="s">
+        <v>225</v>
+      </c>
+      <c r="C9" s="53" t="s">
+        <v>226</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="F9" s="52"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="52"/>
-      <c r="I9" s="52"/>
+        <v>214</v>
+      </c>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
       <c r="J9" s="11"/>
       <c r="K9" s="17">
         <v>44699.0</v>
@@ -10409,38 +10573,38 @@
       <c r="N9" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O9" s="45" t="s">
-        <v>176</v>
-      </c>
-      <c r="P9" s="52"/>
-      <c r="Q9" s="52"/>
-      <c r="R9" s="52"/>
-      <c r="S9" s="52"/>
-      <c r="T9" s="52"/>
-      <c r="U9" s="52"/>
-      <c r="V9" s="52"/>
-      <c r="W9" s="52"/>
-      <c r="X9" s="52"/>
-      <c r="Y9" s="52"/>
-      <c r="Z9" s="52"/>
-      <c r="AA9" s="52"/>
-      <c r="AB9" s="52"/>
+      <c r="O9" s="48" t="s">
+        <v>186</v>
+      </c>
+      <c r="P9" s="55"/>
+      <c r="Q9" s="55"/>
+      <c r="R9" s="55"/>
+      <c r="S9" s="55"/>
+      <c r="T9" s="55"/>
+      <c r="U9" s="55"/>
+      <c r="V9" s="55"/>
+      <c r="W9" s="55"/>
+      <c r="X9" s="55"/>
+      <c r="Y9" s="55"/>
+      <c r="Z9" s="55"/>
+      <c r="AA9" s="55"/>
+      <c r="AB9" s="55"/>
       <c r="AC9" s="11"/>
       <c r="AD9" s="11"/>
     </row>
     <row r="10">
       <c r="A10" s="12" t="s">
-        <v>214</v>
+        <v>227</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>216</v>
+        <v>229</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="18" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
@@ -10459,7 +10623,7 @@
       <c r="N10" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O10" s="48"/>
+      <c r="O10" s="51"/>
       <c r="P10" s="11"/>
       <c r="Q10" s="11"/>
       <c r="R10" s="11"/>
@@ -10480,26 +10644,26 @@
       <c r="A11" s="12"/>
       <c r="B11" s="13"/>
       <c r="C11" s="12"/>
-      <c r="D11" s="44"/>
+      <c r="D11" s="47"/>
       <c r="E11" s="12"/>
       <c r="K11" s="17"/>
       <c r="L11" s="17"/>
       <c r="M11" s="12"/>
       <c r="N11" s="12"/>
-      <c r="O11" s="48"/>
+      <c r="O11" s="51"/>
     </row>
     <row r="12">
       <c r="A12" s="15" t="s">
-        <v>217</v>
+        <v>230</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>218</v>
+        <v>231</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="D12" s="44" t="s">
-        <v>197</v>
+        <v>232</v>
+      </c>
+      <c r="D12" s="47" t="s">
+        <v>210</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>26</v>
@@ -10519,8 +10683,8 @@
       <c r="N12" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O12" s="45" t="s">
-        <v>176</v>
+      <c r="O12" s="48" t="s">
+        <v>186</v>
       </c>
       <c r="P12" s="11"/>
       <c r="Q12" s="11"/>
@@ -10540,17 +10704,17 @@
     </row>
     <row r="13">
       <c r="A13" s="12" t="s">
-        <v>220</v>
+        <v>233</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>220</v>
+        <v>233</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>221</v>
+        <v>234</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="12" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
@@ -10567,8 +10731,8 @@
       <c r="N13" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O13" s="45" t="s">
-        <v>176</v>
+      <c r="O13" s="48" t="s">
+        <v>186</v>
       </c>
       <c r="P13" s="11"/>
       <c r="Q13" s="11"/>
@@ -10588,46 +10752,46 @@
     </row>
     <row r="14">
       <c r="A14" s="12" t="s">
-        <v>223</v>
+        <v>236</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>223</v>
+        <v>236</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>224</v>
+        <v>237</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>225</v>
+        <v>238</v>
       </c>
       <c r="K14" s="17">
         <v>44699.0</v>
       </c>
       <c r="M14" s="12" t="s">
-        <v>226</v>
+        <v>239</v>
       </c>
       <c r="N14" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O14" s="45" t="s">
-        <v>176</v>
+      <c r="O14" s="48" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="12" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>229</v>
+        <v>242</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="12" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
@@ -10644,8 +10808,8 @@
       <c r="N15" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O15" s="45" t="s">
-        <v>176</v>
+      <c r="O15" s="48" t="s">
+        <v>186</v>
       </c>
       <c r="P15" s="11"/>
       <c r="Q15" s="11"/>
@@ -10665,23 +10829,23 @@
     </row>
     <row r="16">
       <c r="A16" s="12" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>231</v>
+        <v>244</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="12" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
       <c r="I16" s="12" t="s">
-        <v>233</v>
+        <v>246</v>
       </c>
       <c r="J16" s="11"/>
       <c r="K16" s="17">
@@ -10696,8 +10860,8 @@
       <c r="N16" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O16" s="45" t="s">
-        <v>176</v>
+      <c r="O16" s="48" t="s">
+        <v>186</v>
       </c>
       <c r="P16" s="11"/>
       <c r="Q16" s="11"/>
@@ -10717,23 +10881,23 @@
     </row>
     <row r="17">
       <c r="A17" s="12" t="s">
-        <v>234</v>
+        <v>247</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>235</v>
+        <v>248</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>236</v>
+        <v>249</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="12" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
       <c r="I17" s="12" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="J17" s="11"/>
       <c r="K17" s="17">
@@ -10748,8 +10912,8 @@
       <c r="N17" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O17" s="45" t="s">
-        <v>176</v>
+      <c r="O17" s="48" t="s">
+        <v>186</v>
       </c>
       <c r="P17" s="11"/>
       <c r="Q17" s="11"/>
@@ -10769,17 +10933,17 @@
     </row>
     <row r="18">
       <c r="A18" s="12" t="s">
-        <v>238</v>
+        <v>251</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="12" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
@@ -10796,7 +10960,7 @@
       <c r="N18" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O18" s="48"/>
+      <c r="O18" s="51"/>
       <c r="P18" s="11"/>
       <c r="Q18" s="11"/>
       <c r="R18" s="11"/>
@@ -10815,17 +10979,17 @@
     </row>
     <row r="19">
       <c r="A19" s="12" t="s">
-        <v>241</v>
+        <v>254</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>242</v>
+        <v>255</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>243</v>
+        <v>256</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="12" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
@@ -10842,7 +11006,7 @@
       <c r="N19" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O19" s="48"/>
+      <c r="O19" s="51"/>
       <c r="P19" s="11"/>
       <c r="Q19" s="11"/>
       <c r="R19" s="11"/>
@@ -10868,16 +11032,16 @@
     </row>
     <row r="21">
       <c r="A21" s="15" t="s">
-        <v>244</v>
+        <v>257</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>244</v>
+        <v>257</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>245</v>
+        <v>258</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>26</v>
@@ -10898,7 +11062,7 @@
         <v>50</v>
       </c>
       <c r="O21" s="16" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
       <c r="P21" s="11"/>
       <c r="Q21" s="11"/>
@@ -10918,17 +11082,17 @@
     </row>
     <row r="22">
       <c r="A22" s="12" t="s">
-        <v>247</v>
+        <v>260</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>247</v>
+        <v>260</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>248</v>
+        <v>261</v>
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="12" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
@@ -10946,7 +11110,7 @@
         <v>50</v>
       </c>
       <c r="O22" s="16" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
       <c r="P22" s="11"/>
       <c r="Q22" s="11"/>
@@ -10966,17 +11130,17 @@
     </row>
     <row r="23">
       <c r="A23" s="12" t="s">
-        <v>250</v>
+        <v>263</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>250</v>
+        <v>263</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="12" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
@@ -10994,7 +11158,7 @@
         <v>50</v>
       </c>
       <c r="O23" s="16" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
       <c r="P23" s="11"/>
       <c r="Q23" s="11"/>
@@ -11014,17 +11178,17 @@
     </row>
     <row r="24">
       <c r="A24" s="13" t="s">
-        <v>252</v>
+        <v>265</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>253</v>
+        <v>266</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>254</v>
+        <v>267</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="12" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
@@ -11042,7 +11206,7 @@
         <v>50</v>
       </c>
       <c r="O24" s="16" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
       <c r="P24" s="11"/>
       <c r="Q24" s="11"/>
@@ -11065,16 +11229,16 @@
     </row>
     <row r="26">
       <c r="A26" s="15" t="s">
-        <v>255</v>
+        <v>268</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>256</v>
+        <v>269</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>257</v>
-      </c>
-      <c r="D26" s="44" t="s">
-        <v>197</v>
+        <v>270</v>
+      </c>
+      <c r="D26" s="47" t="s">
+        <v>210</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>26</v>
@@ -11094,8 +11258,8 @@
       <c r="N26" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O26" s="45" t="s">
-        <v>176</v>
+      <c r="O26" s="48" t="s">
+        <v>186</v>
       </c>
       <c r="P26" s="11"/>
       <c r="Q26" s="11"/>
@@ -11115,17 +11279,17 @@
     </row>
     <row r="27">
       <c r="A27" s="12" t="s">
-        <v>258</v>
+        <v>271</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>259</v>
+        <v>272</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>260</v>
+        <v>273</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="12" t="s">
-        <v>261</v>
+        <v>274</v>
       </c>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
@@ -11142,8 +11306,8 @@
       <c r="N27" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O27" s="45" t="s">
-        <v>176</v>
+      <c r="O27" s="48" t="s">
+        <v>186</v>
       </c>
       <c r="P27" s="11"/>
       <c r="Q27" s="11"/>
@@ -11163,23 +11327,23 @@
     </row>
     <row r="28">
       <c r="A28" s="12" t="s">
-        <v>262</v>
+        <v>275</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>263</v>
+        <v>276</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>264</v>
+        <v>277</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="12" t="s">
-        <v>261</v>
+        <v>274</v>
       </c>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
       <c r="I28" s="12" t="s">
-        <v>265</v>
+        <v>278</v>
       </c>
       <c r="J28" s="11"/>
       <c r="K28" s="17">
@@ -11190,10 +11354,10 @@
         <v>20</v>
       </c>
       <c r="N28" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="O28" s="45" t="s">
-        <v>267</v>
+        <v>279</v>
+      </c>
+      <c r="O28" s="48" t="s">
+        <v>280</v>
       </c>
       <c r="P28" s="11"/>
       <c r="Q28" s="11"/>
@@ -11213,17 +11377,17 @@
     </row>
     <row r="29">
       <c r="A29" s="12" t="s">
-        <v>268</v>
+        <v>281</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>269</v>
+        <v>282</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>270</v>
+        <v>283</v>
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="12" t="s">
-        <v>261</v>
+        <v>274</v>
       </c>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
@@ -11240,8 +11404,8 @@
       <c r="N29" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O29" s="45" t="s">
-        <v>176</v>
+      <c r="O29" s="48" t="s">
+        <v>186</v>
       </c>
       <c r="P29" s="11"/>
       <c r="Q29" s="11"/>
@@ -11261,17 +11425,17 @@
     </row>
     <row r="30">
       <c r="A30" s="12" t="s">
-        <v>271</v>
+        <v>284</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>272</v>
+        <v>285</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>273</v>
+        <v>286</v>
       </c>
       <c r="D30" s="11"/>
       <c r="E30" s="12" t="s">
-        <v>261</v>
+        <v>274</v>
       </c>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
@@ -11288,8 +11452,8 @@
       <c r="N30" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O30" s="45" t="s">
-        <v>176</v>
+      <c r="O30" s="48" t="s">
+        <v>186</v>
       </c>
       <c r="P30" s="11"/>
       <c r="Q30" s="11"/>
@@ -11309,17 +11473,17 @@
     </row>
     <row r="31">
       <c r="A31" s="12" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>275</v>
+        <v>288</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>276</v>
+        <v>289</v>
       </c>
       <c r="D31" s="11"/>
       <c r="E31" s="12" t="s">
-        <v>261</v>
+        <v>274</v>
       </c>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
@@ -11336,8 +11500,8 @@
       <c r="N31" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O31" s="45" t="s">
-        <v>176</v>
+      <c r="O31" s="48" t="s">
+        <v>186</v>
       </c>
       <c r="P31" s="11"/>
       <c r="Q31" s="11"/>
@@ -11357,17 +11521,17 @@
     </row>
     <row r="32">
       <c r="A32" s="12" t="s">
-        <v>277</v>
+        <v>290</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>279</v>
+        <v>292</v>
       </c>
       <c r="D32" s="11"/>
       <c r="E32" s="12" t="s">
-        <v>261</v>
+        <v>274</v>
       </c>
       <c r="F32" s="11"/>
       <c r="G32" s="11"/>
@@ -11384,8 +11548,8 @@
       <c r="N32" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O32" s="45" t="s">
-        <v>176</v>
+      <c r="O32" s="48" t="s">
+        <v>186</v>
       </c>
       <c r="P32" s="11"/>
       <c r="Q32" s="11"/>
@@ -11408,16 +11572,16 @@
     </row>
     <row r="34">
       <c r="A34" s="15" t="s">
-        <v>280</v>
+        <v>293</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>281</v>
+        <v>294</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>282</v>
+        <v>295</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="E34" s="12" t="s">
         <v>26</v>
@@ -11456,17 +11620,17 @@
     </row>
     <row r="35">
       <c r="A35" s="12" t="s">
-        <v>283</v>
+        <v>296</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>283</v>
+        <v>296</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>284</v>
+        <v>297</v>
       </c>
       <c r="D35" s="11"/>
       <c r="E35" s="12" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
@@ -11502,17 +11666,17 @@
     </row>
     <row r="36">
       <c r="A36" s="12" t="s">
-        <v>286</v>
+        <v>299</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>286</v>
+        <v>299</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>287</v>
+        <v>300</v>
       </c>
       <c r="D36" s="11"/>
       <c r="E36" s="12" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
@@ -11551,16 +11715,16 @@
     </row>
     <row r="38">
       <c r="A38" s="15" t="s">
-        <v>288</v>
+        <v>301</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>289</v>
+        <v>302</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>290</v>
+        <v>303</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="E38" s="12" t="s">
         <v>26</v>
@@ -11599,17 +11763,17 @@
     </row>
     <row r="39">
       <c r="A39" s="12" t="s">
-        <v>291</v>
+        <v>304</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>293</v>
+        <v>306</v>
       </c>
       <c r="D39" s="11"/>
       <c r="E39" s="12" t="s">
-        <v>294</v>
+        <v>307</v>
       </c>
       <c r="F39" s="11"/>
       <c r="G39" s="11"/>
@@ -11645,17 +11809,17 @@
     </row>
     <row r="40">
       <c r="A40" s="12" t="s">
-        <v>295</v>
+        <v>308</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>296</v>
+        <v>309</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>297</v>
+        <v>310</v>
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="12" t="s">
-        <v>294</v>
+        <v>307</v>
       </c>
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
@@ -11691,17 +11855,17 @@
     </row>
     <row r="41">
       <c r="A41" s="12" t="s">
-        <v>298</v>
+        <v>311</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>300</v>
+        <v>313</v>
       </c>
       <c r="D41" s="11"/>
       <c r="E41" s="12" t="s">
-        <v>294</v>
+        <v>307</v>
       </c>
       <c r="F41" s="11"/>
       <c r="G41" s="11"/>
@@ -11737,17 +11901,17 @@
     </row>
     <row r="42">
       <c r="A42" s="12" t="s">
-        <v>301</v>
+        <v>314</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>302</v>
+        <v>315</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>303</v>
+        <v>316</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="12" t="s">
-        <v>294</v>
+        <v>307</v>
       </c>
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
@@ -11783,17 +11947,17 @@
     </row>
     <row r="43">
       <c r="A43" s="12" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>306</v>
+        <v>319</v>
       </c>
       <c r="D43" s="11"/>
       <c r="E43" s="12" t="s">
-        <v>294</v>
+        <v>307</v>
       </c>
       <c r="F43" s="11"/>
       <c r="G43" s="11"/>
@@ -11829,17 +11993,17 @@
     </row>
     <row r="44">
       <c r="A44" s="12" t="s">
-        <v>307</v>
+        <v>320</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>308</v>
+        <v>321</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>309</v>
+        <v>322</v>
       </c>
       <c r="D44" s="11"/>
       <c r="E44" s="12" t="s">
-        <v>294</v>
+        <v>307</v>
       </c>
       <c r="F44" s="11"/>
       <c r="G44" s="11"/>
@@ -11875,17 +12039,17 @@
     </row>
     <row r="45">
       <c r="A45" s="12" t="s">
-        <v>310</v>
+        <v>323</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>311</v>
+        <v>324</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>312</v>
+        <v>325</v>
       </c>
       <c r="D45" s="11"/>
       <c r="E45" s="12" t="s">
-        <v>294</v>
+        <v>307</v>
       </c>
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
@@ -11921,17 +12085,17 @@
     </row>
     <row r="46">
       <c r="A46" s="12" t="s">
-        <v>313</v>
+        <v>326</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>314</v>
+        <v>327</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>315</v>
+        <v>328</v>
       </c>
       <c r="D46" s="11"/>
       <c r="E46" s="12" t="s">
-        <v>294</v>
+        <v>307</v>
       </c>
       <c r="F46" s="11"/>
       <c r="G46" s="11"/>
@@ -11967,17 +12131,17 @@
     </row>
     <row r="47">
       <c r="A47" s="12" t="s">
-        <v>316</v>
+        <v>329</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>317</v>
+        <v>330</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>318</v>
+        <v>331</v>
       </c>
       <c r="D47" s="11"/>
       <c r="E47" s="12" t="s">
-        <v>294</v>
+        <v>307</v>
       </c>
       <c r="F47" s="11"/>
       <c r="G47" s="11"/>
@@ -12013,17 +12177,17 @@
     </row>
     <row r="48">
       <c r="A48" s="18" t="s">
-        <v>319</v>
+        <v>332</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>320</v>
+        <v>333</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="D48" s="11"/>
       <c r="E48" s="12" t="s">
-        <v>294</v>
+        <v>307</v>
       </c>
       <c r="F48" s="11"/>
       <c r="G48" s="11"/>
@@ -12063,16 +12227,16 @@
     </row>
     <row r="50">
       <c r="A50" s="15" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>323</v>
+        <v>336</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>324</v>
+        <v>337</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="E50" s="12" t="s">
         <v>26</v>
@@ -12090,7 +12254,7 @@
         <v>20</v>
       </c>
       <c r="N50" s="12" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="O50" s="11"/>
       <c r="P50" s="11"/>
@@ -12111,16 +12275,16 @@
     </row>
     <row r="51">
       <c r="A51" s="15" t="s">
-        <v>326</v>
+        <v>339</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>327</v>
+        <v>340</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>328</v>
+        <v>341</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>329</v>
+        <v>342</v>
       </c>
       <c r="E51" s="12" t="s">
         <v>18</v>
@@ -12138,7 +12302,7 @@
         <v>20</v>
       </c>
       <c r="N51" s="12" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="O51" s="11"/>
       <c r="P51" s="11"/>
@@ -12159,19 +12323,19 @@
     </row>
     <row r="52">
       <c r="A52" s="12" t="s">
-        <v>330</v>
+        <v>343</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>331</v>
+        <v>344</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>332</v>
+        <v>345</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>333</v>
+        <v>346</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>329</v>
+        <v>342</v>
       </c>
       <c r="F52" s="11"/>
       <c r="G52" s="11"/>
@@ -12186,7 +12350,7 @@
         <v>20</v>
       </c>
       <c r="N52" s="12" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="O52" s="11"/>
       <c r="P52" s="11"/>
@@ -12207,19 +12371,19 @@
     </row>
     <row r="53">
       <c r="A53" s="12" t="s">
-        <v>334</v>
+        <v>347</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>335</v>
+        <v>348</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>336</v>
+        <v>349</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>333</v>
+        <v>346</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>329</v>
+        <v>342</v>
       </c>
       <c r="F53" s="11"/>
       <c r="G53" s="11"/>
@@ -12234,7 +12398,7 @@
         <v>20</v>
       </c>
       <c r="N53" s="12" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="O53" s="11"/>
       <c r="P53" s="11"/>
@@ -12255,19 +12419,19 @@
     </row>
     <row r="54">
       <c r="A54" s="12" t="s">
-        <v>337</v>
+        <v>350</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>338</v>
+        <v>351</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>339</v>
+        <v>352</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>333</v>
+        <v>346</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>329</v>
+        <v>342</v>
       </c>
       <c r="F54" s="11"/>
       <c r="G54" s="11"/>
@@ -12282,7 +12446,7 @@
         <v>20</v>
       </c>
       <c r="N54" s="12" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="O54" s="11"/>
       <c r="P54" s="11"/>
@@ -12303,19 +12467,19 @@
     </row>
     <row r="55">
       <c r="A55" s="12" t="s">
-        <v>340</v>
+        <v>353</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>341</v>
+        <v>354</v>
       </c>
       <c r="C55" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="E55" s="12" t="s">
         <v>342</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>333</v>
-      </c>
-      <c r="E55" s="12" t="s">
-        <v>329</v>
       </c>
       <c r="F55" s="11"/>
       <c r="G55" s="11"/>
@@ -12330,7 +12494,7 @@
         <v>20</v>
       </c>
       <c r="N55" s="12" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="O55" s="11"/>
       <c r="P55" s="11"/>
@@ -12351,16 +12515,16 @@
     </row>
     <row r="56">
       <c r="A56" s="15" t="s">
-        <v>343</v>
+        <v>356</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>344</v>
+        <v>357</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>345</v>
+        <v>358</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>329</v>
+        <v>342</v>
       </c>
       <c r="E56" s="12" t="s">
         <v>26</v>
@@ -12378,7 +12542,7 @@
         <v>20</v>
       </c>
       <c r="N56" s="12" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="O56" s="11"/>
       <c r="P56" s="11"/>
@@ -12399,19 +12563,19 @@
     </row>
     <row r="57">
       <c r="A57" s="12" t="s">
-        <v>346</v>
+        <v>359</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>347</v>
+        <v>360</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>348</v>
+        <v>361</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>349</v>
+        <v>362</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>329</v>
+        <v>342</v>
       </c>
       <c r="F57" s="11"/>
       <c r="G57" s="11"/>
@@ -12426,7 +12590,7 @@
         <v>20</v>
       </c>
       <c r="N57" s="12" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="O57" s="11"/>
       <c r="P57" s="11"/>
@@ -12447,19 +12611,19 @@
     </row>
     <row r="58">
       <c r="A58" s="12" t="s">
-        <v>350</v>
+        <v>363</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>351</v>
+        <v>364</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>352</v>
+        <v>365</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>349</v>
+        <v>362</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>329</v>
+        <v>342</v>
       </c>
       <c r="F58" s="11"/>
       <c r="G58" s="11"/>
@@ -12474,7 +12638,7 @@
         <v>20</v>
       </c>
       <c r="N58" s="12" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="O58" s="11"/>
       <c r="P58" s="11"/>
@@ -12495,19 +12659,19 @@
     </row>
     <row r="59">
       <c r="A59" s="12" t="s">
-        <v>353</v>
+        <v>366</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>354</v>
+        <v>367</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>355</v>
+        <v>368</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>349</v>
+        <v>362</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>329</v>
+        <v>342</v>
       </c>
       <c r="F59" s="11"/>
       <c r="G59" s="11"/>
@@ -12522,7 +12686,7 @@
         <v>20</v>
       </c>
       <c r="N59" s="12" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="O59" s="11"/>
       <c r="P59" s="11"/>
@@ -12543,19 +12707,19 @@
     </row>
     <row r="60">
       <c r="A60" s="12" t="s">
-        <v>356</v>
+        <v>369</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>357</v>
+        <v>370</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>358</v>
+        <v>371</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>349</v>
+        <v>362</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>329</v>
+        <v>342</v>
       </c>
       <c r="F60" s="11"/>
       <c r="G60" s="11"/>
@@ -12570,7 +12734,7 @@
         <v>20</v>
       </c>
       <c r="N60" s="12" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="O60" s="11"/>
       <c r="P60" s="11"/>
@@ -12595,16 +12759,16 @@
     </row>
     <row r="62">
       <c r="A62" s="15" t="s">
-        <v>359</v>
+        <v>372</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>360</v>
+        <v>373</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>361</v>
+        <v>374</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="E62" s="12" t="s">
         <v>26</v>
@@ -12613,7 +12777,7 @@
       <c r="G62" s="11"/>
       <c r="H62" s="11"/>
       <c r="I62" s="12" t="s">
-        <v>362</v>
+        <v>375</v>
       </c>
       <c r="J62" s="11"/>
       <c r="K62" s="17">
@@ -12624,7 +12788,7 @@
         <v>20</v>
       </c>
       <c r="N62" s="12" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="O62" s="11"/>
       <c r="P62" s="11"/>
@@ -12645,16 +12809,16 @@
     </row>
     <row r="63">
       <c r="A63" s="12" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>364</v>
+        <v>377</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>365</v>
+        <v>378</v>
       </c>
       <c r="E63" s="12" t="s">
         <v>18</v>
@@ -12672,7 +12836,7 @@
         <v>20</v>
       </c>
       <c r="N63" s="12" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="O63" s="11"/>
       <c r="P63" s="11"/>
@@ -12693,16 +12857,16 @@
     </row>
     <row r="64">
       <c r="A64" s="12" t="s">
-        <v>366</v>
+        <v>379</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>366</v>
+        <v>379</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>367</v>
+        <v>380</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>365</v>
+        <v>378</v>
       </c>
       <c r="E64" s="12" t="s">
         <v>18</v>
@@ -12720,7 +12884,7 @@
         <v>20</v>
       </c>
       <c r="N64" s="12" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="O64" s="11"/>
       <c r="P64" s="11"/>
@@ -12745,23 +12909,23 @@
     </row>
     <row r="66">
       <c r="A66" s="15" t="s">
-        <v>368</v>
+        <v>381</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>369</v>
+        <v>382</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>361</v>
+        <v>374</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="E66" s="11"/>
       <c r="F66" s="11"/>
       <c r="G66" s="11"/>
       <c r="H66" s="11"/>
       <c r="I66" s="12" t="s">
-        <v>370</v>
+        <v>383</v>
       </c>
       <c r="J66" s="11"/>
       <c r="K66" s="17">
@@ -12772,7 +12936,7 @@
         <v>20</v>
       </c>
       <c r="N66" s="12" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="O66" s="11"/>
       <c r="P66" s="11"/>
@@ -12793,16 +12957,16 @@
     </row>
     <row r="67">
       <c r="A67" s="12" t="s">
-        <v>371</v>
+        <v>384</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>371</v>
+        <v>384</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>372</v>
+        <v>385</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>373</v>
+        <v>386</v>
       </c>
       <c r="E67" s="12" t="s">
         <v>18</v>
@@ -12820,7 +12984,7 @@
         <v>20</v>
       </c>
       <c r="N67" s="12" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="O67" s="11"/>
       <c r="P67" s="11"/>
@@ -12841,16 +13005,16 @@
     </row>
     <row r="68">
       <c r="A68" s="12" t="s">
-        <v>374</v>
+        <v>387</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>374</v>
+        <v>387</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>375</v>
+        <v>388</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>373</v>
+        <v>386</v>
       </c>
       <c r="E68" s="12" t="s">
         <v>18</v>
@@ -12868,7 +13032,7 @@
         <v>20</v>
       </c>
       <c r="N68" s="12" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="O68" s="11"/>
       <c r="P68" s="11"/>
@@ -12893,16 +13057,16 @@
     </row>
     <row r="70">
       <c r="A70" s="15" t="s">
-        <v>376</v>
+        <v>389</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>377</v>
+        <v>390</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>378</v>
+        <v>391</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="E70" s="12" t="s">
         <v>26</v>
@@ -12920,7 +13084,7 @@
         <v>20</v>
       </c>
       <c r="N70" s="12" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="O70" s="11"/>
       <c r="P70" s="11"/>
@@ -12941,16 +13105,16 @@
     </row>
     <row r="71">
       <c r="A71" s="12" t="s">
-        <v>379</v>
+        <v>392</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>381</v>
+        <v>394</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>382</v>
+        <v>395</v>
       </c>
       <c r="E71" s="12" t="s">
         <v>18</v>
@@ -12959,7 +13123,7 @@
       <c r="G71" s="11"/>
       <c r="H71" s="11"/>
       <c r="I71" s="12" t="s">
-        <v>383</v>
+        <v>396</v>
       </c>
       <c r="J71" s="11"/>
       <c r="K71" s="17">
@@ -12970,7 +13134,7 @@
         <v>20</v>
       </c>
       <c r="N71" s="12" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="O71" s="11"/>
       <c r="P71" s="11"/>
@@ -12991,16 +13155,16 @@
     </row>
     <row r="72">
       <c r="A72" s="12" t="s">
-        <v>384</v>
+        <v>397</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>385</v>
+        <v>398</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>386</v>
+        <v>399</v>
       </c>
       <c r="D72" s="12" t="s">
-        <v>382</v>
+        <v>395</v>
       </c>
       <c r="E72" s="12" t="s">
         <v>18</v>
@@ -13009,7 +13173,7 @@
       <c r="G72" s="11"/>
       <c r="H72" s="11"/>
       <c r="I72" s="12" t="s">
-        <v>387</v>
+        <v>400</v>
       </c>
       <c r="J72" s="11"/>
       <c r="K72" s="17">
@@ -13020,7 +13184,7 @@
         <v>20</v>
       </c>
       <c r="N72" s="12" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="O72" s="11"/>
       <c r="P72" s="11"/>
@@ -13041,16 +13205,16 @@
     </row>
     <row r="73">
       <c r="A73" s="12" t="s">
-        <v>388</v>
+        <v>401</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>389</v>
+        <v>402</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>390</v>
+        <v>403</v>
       </c>
       <c r="D73" s="12" t="s">
-        <v>382</v>
+        <v>395</v>
       </c>
       <c r="E73" s="12" t="s">
         <v>18</v>
@@ -13068,7 +13232,7 @@
         <v>20</v>
       </c>
       <c r="N73" s="12" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="O73" s="11"/>
       <c r="P73" s="11"/>
@@ -13092,16 +13256,16 @@
     </row>
     <row r="75">
       <c r="A75" s="15" t="s">
-        <v>391</v>
+        <v>404</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>392</v>
+        <v>405</v>
       </c>
       <c r="C75" s="12" t="s">
-        <v>393</v>
+        <v>406</v>
       </c>
       <c r="D75" s="12" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="E75" s="12" t="s">
         <v>26</v>
@@ -13140,17 +13304,17 @@
     </row>
     <row r="76">
       <c r="A76" s="12" t="s">
-        <v>394</v>
+        <v>407</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>395</v>
+        <v>408</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>396</v>
+        <v>409</v>
       </c>
       <c r="D76" s="11"/>
       <c r="E76" s="12" t="s">
-        <v>397</v>
+        <v>410</v>
       </c>
       <c r="F76" s="11"/>
       <c r="G76" s="11"/>
@@ -13186,17 +13350,17 @@
     </row>
     <row r="77">
       <c r="A77" s="12" t="s">
-        <v>398</v>
+        <v>411</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>399</v>
+        <v>412</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>400</v>
+        <v>413</v>
       </c>
       <c r="D77" s="11"/>
       <c r="E77" s="12" t="s">
-        <v>397</v>
+        <v>410</v>
       </c>
       <c r="F77" s="11"/>
       <c r="G77" s="11"/>
@@ -13232,17 +13396,17 @@
     </row>
     <row r="78">
       <c r="A78" s="12" t="s">
-        <v>401</v>
+        <v>414</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>402</v>
+        <v>415</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>403</v>
+        <v>416</v>
       </c>
       <c r="D78" s="11"/>
       <c r="E78" s="12" t="s">
-        <v>397</v>
+        <v>410</v>
       </c>
       <c r="F78" s="11"/>
       <c r="G78" s="11"/>
@@ -13278,17 +13442,17 @@
     </row>
     <row r="79">
       <c r="A79" s="12" t="s">
-        <v>404</v>
+        <v>417</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>405</v>
+        <v>418</v>
       </c>
       <c r="C79" s="12" t="s">
-        <v>406</v>
+        <v>419</v>
       </c>
       <c r="D79" s="11"/>
       <c r="E79" s="12" t="s">
-        <v>397</v>
+        <v>410</v>
       </c>
       <c r="F79" s="11"/>
       <c r="G79" s="11"/>
@@ -13324,17 +13488,17 @@
     </row>
     <row r="80">
       <c r="A80" s="12" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>408</v>
+        <v>421</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>409</v>
+        <v>422</v>
       </c>
       <c r="D80" s="11"/>
       <c r="E80" s="12" t="s">
-        <v>397</v>
+        <v>410</v>
       </c>
       <c r="F80" s="11"/>
       <c r="G80" s="11"/>
@@ -15811,46 +15975,46 @@
   </cols>
   <sheetData>
     <row r="1" ht="28.5" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="G1" s="20" t="s">
+      <c r="D1" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="L1" s="25" t="s">
+      <c r="K1" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="L1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="M1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="26" t="s">
+      <c r="N1" s="29" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="15" t="s">
@@ -15859,22 +16023,22 @@
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>410</v>
+        <v>423</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>411</v>
+        <v>424</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>412</v>
+        <v>425</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
@@ -15891,7 +16055,7 @@
         <v>50</v>
       </c>
       <c r="O2" s="16" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
@@ -15911,22 +16075,22 @@
     </row>
     <row r="3">
       <c r="A3" s="12" t="s">
-        <v>413</v>
+        <v>426</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>414</v>
+        <v>427</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>415</v>
+        <v>428</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>416</v>
+        <v>429</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -15943,7 +16107,7 @@
         <v>50</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="P3" s="11"/>
       <c r="Q3" s="11"/>
@@ -15963,22 +16127,22 @@
     </row>
     <row r="4">
       <c r="A4" s="12" t="s">
-        <v>417</v>
+        <v>430</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>418</v>
+        <v>431</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>419</v>
+        <v>432</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>416</v>
+        <v>429</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
@@ -15995,7 +16159,7 @@
         <v>50</v>
       </c>
       <c r="O4" s="16" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
@@ -16015,22 +16179,22 @@
     </row>
     <row r="5">
       <c r="A5" s="12" t="s">
-        <v>420</v>
+        <v>433</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>421</v>
+        <v>434</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>422</v>
+        <v>435</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>261</v>
+        <v>274</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>416</v>
+        <v>429</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -16047,7 +16211,7 @@
         <v>50</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>423</v>
+        <v>436</v>
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
@@ -16067,22 +16231,22 @@
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>424</v>
+        <v>437</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>425</v>
+        <v>438</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>426</v>
+        <v>439</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>427</v>
+        <v>440</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
@@ -16117,22 +16281,22 @@
     </row>
     <row r="7">
       <c r="A7" s="12" t="s">
-        <v>428</v>
+        <v>441</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>429</v>
+        <v>442</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>430</v>
+        <v>443</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>329</v>
+        <v>342</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>416</v>
+        <v>429</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -16167,22 +16331,22 @@
     </row>
     <row r="8">
       <c r="A8" s="12" t="s">
-        <v>431</v>
+        <v>444</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>432</v>
+        <v>445</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>433</v>
+        <v>446</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>365</v>
+        <v>378</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>416</v>
+        <v>429</v>
       </c>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
@@ -16217,22 +16381,22 @@
     </row>
     <row r="9">
       <c r="A9" s="12" t="s">
-        <v>434</v>
+        <v>447</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>435</v>
+        <v>448</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>436</v>
+        <v>449</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>373</v>
+        <v>386</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>416</v>
+        <v>429</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
@@ -16269,22 +16433,22 @@
     </row>
     <row r="10">
       <c r="A10" s="12" t="s">
-        <v>437</v>
+        <v>450</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>438</v>
+        <v>451</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>439</v>
+        <v>452</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>382</v>
+        <v>395</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>416</v>
+        <v>429</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
@@ -16319,28 +16483,28 @@
     </row>
     <row r="11">
       <c r="A11" s="12" t="s">
-        <v>440</v>
+        <v>453</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>441</v>
+        <v>454</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>442</v>
+        <v>455</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>443</v>
+        <v>456</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="K11" s="14">
         <v>45422.0</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>444</v>
+        <v>457</v>
       </c>
       <c r="N11" s="12" t="s">
         <v>50</v>
@@ -16348,28 +16512,28 @@
     </row>
     <row r="12">
       <c r="A12" s="12" t="s">
-        <v>445</v>
+        <v>458</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>446</v>
+        <v>459</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>447</v>
+        <v>460</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>443</v>
+        <v>456</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="K12" s="14">
         <v>45422.0</v>
       </c>
       <c r="M12" s="12" t="s">
-        <v>444</v>
+        <v>457</v>
       </c>
       <c r="N12" s="12" t="s">
         <v>50</v>
@@ -16377,28 +16541,28 @@
     </row>
     <row r="13">
       <c r="A13" s="12" t="s">
-        <v>448</v>
+        <v>461</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>449</v>
+        <v>462</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>443</v>
+        <v>456</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="K13" s="14">
         <v>45422.0</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>444</v>
+        <v>457</v>
       </c>
       <c r="N13" s="12" t="s">
         <v>50</v>
@@ -16406,22 +16570,22 @@
     </row>
     <row r="14">
       <c r="A14" s="12" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>452</v>
+        <v>465</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>453</v>
+        <v>466</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="K14" s="17">
         <v>45453.0</v>
@@ -16435,22 +16599,22 @@
     </row>
     <row r="15">
       <c r="A15" s="12" t="s">
-        <v>454</v>
+        <v>467</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>455</v>
+        <v>468</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>456</v>
+        <v>469</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>294</v>
+        <v>307</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="K15" s="17">
         <v>45453.0</v>
@@ -16464,22 +16628,22 @@
     </row>
     <row r="16">
       <c r="A16" s="12" t="s">
-        <v>457</v>
+        <v>470</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>458</v>
+        <v>471</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>459</v>
+        <v>472</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>397</v>
+        <v>410</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="K16" s="17">
         <v>45453.0</v>

</xml_diff>

<commit_message>
Adds dpv:ReuseCompatibility taxonomy to DPV
- closes #283
- adds dpv:ReuseCompatibility and dpv:hasReuseCompatibility
- adds dpv:PrimaryUse and dpv:SecondaryUse
- includes RDF and HTML outputs including Context section

Co-authored-by: Beatriz Esteves <beatriz.gc.esteves@gmail.com>
Co-authored-by: Delaram Golpayegani <sgolpays@tcd.ie>
Co-authored-by: Georg P. Krog <georg@signatu.com>
Co-authored-by: Paul Ryan <71695536+Paul-Ryan76@users.noreply.github.com>
Co-authored-by: Julian Flake <flake@uni-koblenz.de>
Co-authored-by: Arthit Suriyawongkul <arthit@gmail.com>
</commit_message>
<xml_diff>
--- a/code/vocab_csv/context_status.xlsx
+++ b/code/vocab_csv/context_status.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="521">
   <si>
     <t>Term</t>
   </si>
@@ -391,9 +391,6 @@
     <t>Indication that the specified context has a subsequent occurrence or that it applies after the initial occurrence or not at the beginning</t>
   </si>
   <si>
-    <t>Indication that the specified context has an initial occurence or that it applies initially or at the beginning</t>
-  </si>
-  <si>
     <t>Applicability</t>
   </si>
   <si>
@@ -451,6 +448,9 @@
     <t>Concept indicating whether a fee is required</t>
   </si>
   <si>
+    <t>Harshvardhan J. Pandit, Georg P. Krog</t>
+  </si>
+  <si>
     <t>FeeRequired</t>
   </si>
   <si>
@@ -470,6 +470,108 @@
   </si>
   <si>
     <t>Concept indicating a fee is not required. This is distinct from a Fee of zero as it indicates a fee is not applicable in the context</t>
+  </si>
+  <si>
+    <t>ReuseCompatibility</t>
+  </si>
+  <si>
+    <t>Concept indicating whether the specified context is compatible with another earlier context</t>
+  </si>
+  <si>
+    <t>Compatibility refers to whether two contexts, such as dpv:Process instances, are compatible with each other based on a criteria which is not defined by the concept. This criteria can be based on requirements from law, such as GDPR's purpose compatibility or can be based on privacy norms such as contextual integrity. To express such interpretations, further concepts should be expanded from this base concept</t>
+  </si>
+  <si>
+    <t>Harshvardhan J. Pandit, Georg P. Krog, Beatriz Esteves, Delaram Golpayegani, Julian Flake, Arthit Suriyawongkul</t>
+  </si>
+  <si>
+    <t>PrimaryUse</t>
+  </si>
+  <si>
+    <t>Primary Use</t>
+  </si>
+  <si>
+    <t>Concept indicating compatibility based on the use being either the original context or something that is compatible with it</t>
+  </si>
+  <si>
+    <t>dpv:ReuseCompatibility</t>
+  </si>
+  <si>
+    <t>Primary Use refers to an assessment where two contexts are found to be compatible, e.g. if purpose is used to test compatibility, then for two activities the second activity is said be the primary use if its purpose is compatible with the first activity's purpose</t>
+  </si>
+  <si>
+    <t>SecondaryUse</t>
+  </si>
+  <si>
+    <t>Secondary Use</t>
+  </si>
+  <si>
+    <t>Concept indicating incompatibility based on the use not being compatible with an earlier context</t>
+  </si>
+  <si>
+    <t>Secondary Use refers to an assessment where two contexts are found to be incompatible, e.g. if purpose is used to test compatibility, then for two activities the second activity is said be the secondary use if its purpose is incompatible with the first activity's purpose</t>
+  </si>
+  <si>
+    <t>PrimaryInitialUse</t>
+  </si>
+  <si>
+    <t>Primary Initial Use</t>
+  </si>
+  <si>
+    <t>Concept indicating this is the first or initial context which will be used for comparing compatibility with</t>
+  </si>
+  <si>
+    <t>dpv:PrimaryUse</t>
+  </si>
+  <si>
+    <t>Primary Initial Use is useful to indicate this is the original or initial context which will be used as the measure to compare with for compatibility assessments</t>
+  </si>
+  <si>
+    <t>PrimarySubsequentReuse</t>
+  </si>
+  <si>
+    <t>Primary Subsequent Reuse</t>
+  </si>
+  <si>
+    <t>Concept indicating this is a compatible reuse with a prior initial context</t>
+  </si>
+  <si>
+    <t>Primary Subsequent Reuse indicates that this is not the original or initial context but another context which is compatible with it</t>
+  </si>
+  <si>
+    <t>SecondaryContextualReuse</t>
+  </si>
+  <si>
+    <t>Secondary Contextual Reuse</t>
+  </si>
+  <si>
+    <t>Concept indicating incompatibility based on the use not being compatible with an earlier context but still being within the same broader context i.e. the degree of incompability does not violate or go beyond some established parameters or norms</t>
+  </si>
+  <si>
+    <t>dpv:SecondaryUse</t>
+  </si>
+  <si>
+    <t>Secondary Contextual Reuse is useful to indicate that even if the context is incompatible, the degree of incompatibility does not go beyond an established norm. For example, in healthcare settings, reusing data from patients for medical research is considered secondary use, however, it still occurs within the aegis and duties of the hospital and therefore is different from cases where another external for-profit company is reusing the data (which is represented as Tertiary Use)</t>
+  </si>
+  <si>
+    <t>TertiaryUse</t>
+  </si>
+  <si>
+    <t>Tertiary Use</t>
+  </si>
+  <si>
+    <t>Concept indicating incompatibility that goes beyond some established parameters or norms to the extent that it is considered tertiary or completely removed or detached from the initial primary use</t>
+  </si>
+  <si>
+    <t>Tertiary Use is useful to indicate that the incompatibility is to such a degree that it should not be considered mere secondary use of the data and should be further distinguished from it. For example, in healthcare, reusing data from patients for medical research is considered secondary use, but if the same data is being used by external third parties who have no relation to the patients and are not using it for public good, then it can be considered as a Tertiary Use. This concept is intended to be analogous to "Third Party" in privacy contexts</t>
+  </si>
+  <si>
+    <t>CompatibilityUnknown</t>
+  </si>
+  <si>
+    <t>Compatibility Unknown</t>
+  </si>
+  <si>
+    <t>Concept indicating the compatibility of the context with an earlier context is currently unknown</t>
   </si>
   <si>
     <t>domain</t>
@@ -679,6 +781,15 @@
   </si>
   <si>
     <t>Indicates whether a fee is required for the specified context</t>
+  </si>
+  <si>
+    <t>hasReuseCompatibility</t>
+  </si>
+  <si>
+    <t>has reuse compatibility</t>
+  </si>
+  <si>
+    <t>Indicates the reuse compatibility for the specified context</t>
   </si>
   <si>
     <t>The status or state of something</t>
@@ -1837,6 +1948,30 @@
   <dxfs count="7">
     <dxf>
       <font>
+        <color rgb="FFE06666"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF783F04"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF0000FF"/>
       </font>
       <fill>
@@ -1879,30 +2014,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFF4CCCC"/>
           <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFE06666"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF783F04"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
         </patternFill>
       </fill>
       <border/>
@@ -3724,8 +3835,8 @@
       <c r="C38" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="D38" s="18" t="s">
-        <v>125</v>
+      <c r="D38" s="12" t="s">
+        <v>121</v>
       </c>
       <c r="E38" s="12" t="s">
         <v>26</v>
@@ -3763,13 +3874,13 @@
     </row>
     <row r="40">
       <c r="A40" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="C40" s="12" t="s">
         <v>126</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>127</v>
       </c>
       <c r="D40" s="12" t="s">
         <v>25</v>
@@ -3781,7 +3892,7 @@
       <c r="G40" s="11"/>
       <c r="H40" s="11"/>
       <c r="I40" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J40" s="11"/>
       <c r="K40" s="17">
@@ -3813,16 +3924,16 @@
     </row>
     <row r="41">
       <c r="A41" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B41" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="C41" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="D41" s="12" t="s">
         <v>131</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>132</v>
       </c>
       <c r="E41" s="12" t="s">
         <v>18</v>
@@ -3831,7 +3942,7 @@
       <c r="G41" s="11"/>
       <c r="H41" s="11"/>
       <c r="I41" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J41" s="11"/>
       <c r="K41" s="17">
@@ -3863,16 +3974,16 @@
     </row>
     <row r="42">
       <c r="A42" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="B42" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="C42" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="C42" s="12" t="s">
-        <v>136</v>
-      </c>
       <c r="D42" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E42" s="12" t="s">
         <v>18</v>
@@ -3881,7 +3992,7 @@
       <c r="G42" s="11"/>
       <c r="H42" s="11"/>
       <c r="I42" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J42" s="11"/>
       <c r="K42" s="17">
@@ -3913,16 +4024,16 @@
     </row>
     <row r="43">
       <c r="A43" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B43" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="B43" s="12" t="s">
+      <c r="C43" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="C43" s="12" t="s">
-        <v>140</v>
-      </c>
       <c r="D43" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E43" s="12" t="s">
         <v>18</v>
@@ -3931,7 +4042,7 @@
       <c r="G43" s="11"/>
       <c r="H43" s="11"/>
       <c r="I43" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J43" s="11"/>
       <c r="K43" s="17">
@@ -3966,13 +4077,13 @@
     </row>
     <row r="46">
       <c r="A46" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B46" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="B46" s="12" t="s">
+      <c r="C46" s="12" t="s">
         <v>143</v>
-      </c>
-      <c r="C46" s="12" t="s">
-        <v>144</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>25</v>
@@ -3987,6 +4098,9 @@
       <c r="M46" s="22" t="s">
         <v>20</v>
       </c>
+      <c r="N46" s="12" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="12" t="s">
@@ -4011,6 +4125,9 @@
       <c r="M47" s="22" t="s">
         <v>20</v>
       </c>
+      <c r="N47" s="12" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="12" t="s">
@@ -4035,6 +4152,229 @@
       <c r="M48" s="22" t="s">
         <v>20</v>
       </c>
+      <c r="N48" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I50" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="K50" s="17">
+        <v>45827.0</v>
+      </c>
+      <c r="M50" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N50" s="12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="I51" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="K51" s="17">
+        <v>45827.0</v>
+      </c>
+      <c r="M51" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N51" s="12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="I52" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="K52" s="17">
+        <v>45827.0</v>
+      </c>
+      <c r="M52" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N52" s="12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="I53" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="K53" s="17">
+        <v>45827.0</v>
+      </c>
+      <c r="M53" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="N53" s="12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="I54" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="K54" s="17">
+        <v>45827.0</v>
+      </c>
+      <c r="M54" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="N54" s="12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="I55" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="K55" s="17">
+        <v>45827.0</v>
+      </c>
+      <c r="M55" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="N55" s="12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="B56" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="I56" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="K56" s="17">
+        <v>45827.0</v>
+      </c>
+      <c r="M56" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="N56" s="12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="E57" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="K57" s="17">
+        <v>45827.0</v>
+      </c>
+      <c r="M57" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N57" s="12" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="70">
       <c r="B70" s="19"/>
@@ -6491,23 +6831,33 @@
       <c r="B887" s="19"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:AB44 A70:AB258">
+  <conditionalFormatting sqref="N46:N48 K50:K57 N50:N57">
     <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$M46="deprecated"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N46:N48 K50:K57 N50:N57">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$M46="changed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:AB44 N46:N48 K50:K57 N50:N57 A70:AB258">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$M2="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AD44 A70:AD278">
-    <cfRule type="expression" dxfId="1" priority="2">
+  <conditionalFormatting sqref="A2:AD44 N46:N48 K50:K57 N50:N57 A70:AD278">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$M2="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:AD44 A70:AD208">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>$M2="modified"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:AD44 A70:AD208">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>$M2="deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6568,13 +6918,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>152</v>
+        <v>186</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>153</v>
+        <v>187</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>154</v>
+        <v>188</v>
       </c>
       <c r="G1" s="23" t="s">
         <v>6</v>
@@ -6589,7 +6939,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="27" t="s">
-        <v>155</v>
+        <v>189</v>
       </c>
       <c r="L1" s="28" t="s">
         <v>11</v>
@@ -6606,13 +6956,13 @@
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>156</v>
+        <v>190</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>157</v>
+        <v>191</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>158</v>
+        <v>192</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>17</v>
@@ -6621,7 +6971,7 @@
         <v>25</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
@@ -6656,13 +7006,13 @@
     </row>
     <row r="3">
       <c r="A3" s="30" t="s">
-        <v>160</v>
+        <v>194</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>161</v>
+        <v>195</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>162</v>
+        <v>196</v>
       </c>
       <c r="D3" s="30" t="s">
         <v>17</v>
@@ -6671,13 +7021,13 @@
         <v>87</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="G3" s="32"/>
       <c r="H3" s="32"/>
       <c r="I3" s="32"/>
       <c r="J3" s="33" t="s">
-        <v>163</v>
+        <v>197</v>
       </c>
       <c r="K3" s="34">
         <v>43560.0</v>
@@ -6687,7 +7037,7 @@
         <v>20</v>
       </c>
       <c r="N3" s="36" t="s">
-        <v>164</v>
+        <v>198</v>
       </c>
       <c r="O3" s="37" t="s">
         <v>22</v>
@@ -6710,13 +7060,13 @@
     </row>
     <row r="4">
       <c r="A4" s="38" t="s">
-        <v>165</v>
+        <v>199</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>166</v>
+        <v>200</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>167</v>
+        <v>201</v>
       </c>
       <c r="D4" s="40" t="s">
         <v>17</v>
@@ -6725,7 +7075,7 @@
         <v>17</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="G4" s="41"/>
       <c r="H4" s="41"/>
@@ -6739,10 +7089,10 @@
         <v>20</v>
       </c>
       <c r="N4" s="44" t="s">
-        <v>168</v>
+        <v>202</v>
       </c>
       <c r="O4" s="45" t="s">
-        <v>169</v>
+        <v>203</v>
       </c>
       <c r="P4" s="46"/>
       <c r="Q4" s="46"/>
@@ -6762,13 +7112,13 @@
     </row>
     <row r="5">
       <c r="A5" s="12" t="s">
-        <v>170</v>
+        <v>204</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>171</v>
+        <v>205</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>172</v>
+        <v>206</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>17</v>
@@ -6777,7 +7127,7 @@
         <v>72</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -6794,7 +7144,7 @@
         <v>62</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>173</v>
+        <v>207</v>
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
@@ -6814,13 +7164,13 @@
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>174</v>
+        <v>208</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>175</v>
+        <v>209</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>176</v>
+        <v>210</v>
       </c>
       <c r="D6" s="47" t="s">
         <v>17</v>
@@ -6829,7 +7179,7 @@
         <v>17</v>
       </c>
       <c r="F6" s="47" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
@@ -6843,10 +7193,10 @@
         <v>20</v>
       </c>
       <c r="N6" s="12" t="s">
-        <v>177</v>
+        <v>211</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>178</v>
+        <v>212</v>
       </c>
       <c r="P6" s="11"/>
       <c r="Q6" s="11"/>
@@ -6866,13 +7216,13 @@
     </row>
     <row r="7">
       <c r="A7" s="12" t="s">
-        <v>179</v>
+        <v>213</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>180</v>
+        <v>214</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>181</v>
+        <v>215</v>
       </c>
       <c r="D7" s="47" t="s">
         <v>17</v>
@@ -6881,7 +7231,7 @@
         <v>17</v>
       </c>
       <c r="F7" s="47" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -6898,7 +7248,7 @@
         <v>62</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>182</v>
+        <v>216</v>
       </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
@@ -6918,13 +7268,13 @@
     </row>
     <row r="8">
       <c r="A8" s="12" t="s">
-        <v>183</v>
+        <v>217</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>184</v>
+        <v>218</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>185</v>
+        <v>219</v>
       </c>
       <c r="D8" s="47" t="s">
         <v>17</v>
@@ -6933,7 +7283,7 @@
         <v>17</v>
       </c>
       <c r="F8" s="47" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
@@ -6947,10 +7297,10 @@
         <v>20</v>
       </c>
       <c r="N8" s="18" t="s">
-        <v>177</v>
+        <v>211</v>
       </c>
       <c r="O8" s="16" t="s">
-        <v>178</v>
+        <v>212</v>
       </c>
       <c r="P8" s="11"/>
       <c r="Q8" s="11"/>
@@ -6970,22 +7320,22 @@
     </row>
     <row r="9">
       <c r="A9" s="12" t="s">
-        <v>186</v>
+        <v>220</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>187</v>
+        <v>221</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>188</v>
+        <v>222</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>189</v>
+        <v>223</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
@@ -7022,22 +7372,22 @@
     </row>
     <row r="10">
       <c r="A10" s="12" t="s">
-        <v>190</v>
+        <v>224</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>191</v>
+        <v>225</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>192</v>
+        <v>226</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="F10" s="12" t="s">
         <v>193</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>159</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
@@ -7074,13 +7424,13 @@
     </row>
     <row r="11">
       <c r="A11" s="12" t="s">
-        <v>194</v>
+        <v>228</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>195</v>
+        <v>229</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>196</v>
+        <v>230</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>17</v>
@@ -7089,7 +7439,7 @@
         <v>17</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -7106,7 +7456,7 @@
         <v>62</v>
       </c>
       <c r="O11" s="48" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="P11" s="11"/>
       <c r="Q11" s="11"/>
@@ -7126,22 +7476,22 @@
     </row>
     <row r="12">
       <c r="A12" s="12" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>199</v>
+        <v>233</v>
       </c>
       <c r="C12" s="49" t="s">
-        <v>200</v>
+        <v>234</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>189</v>
+        <v>223</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
@@ -7155,7 +7505,7 @@
         <v>20</v>
       </c>
       <c r="N12" s="12" t="s">
-        <v>201</v>
+        <v>235</v>
       </c>
       <c r="O12" s="11"/>
       <c r="P12" s="11"/>
@@ -7176,22 +7526,22 @@
     </row>
     <row r="13">
       <c r="A13" s="12" t="s">
-        <v>202</v>
+        <v>236</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>203</v>
+        <v>237</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>204</v>
+        <v>238</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>189</v>
+        <v>223</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
@@ -7205,7 +7555,7 @@
         <v>20</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>201</v>
+        <v>235</v>
       </c>
       <c r="O13" s="11"/>
       <c r="P13" s="11"/>
@@ -7226,13 +7576,13 @@
     </row>
     <row r="14">
       <c r="A14" s="12" t="s">
-        <v>205</v>
+        <v>239</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>206</v>
+        <v>240</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>207</v>
+        <v>241</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>17</v>
@@ -7241,7 +7591,7 @@
         <v>33</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
@@ -7276,13 +7626,13 @@
     </row>
     <row r="15">
       <c r="A15" s="50" t="s">
-        <v>208</v>
+        <v>242</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>209</v>
+        <v>243</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>210</v>
+        <v>244</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>17</v>
@@ -7291,7 +7641,7 @@
         <v>42</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
@@ -7326,22 +7676,22 @@
     </row>
     <row r="16">
       <c r="A16" s="50" t="s">
-        <v>211</v>
+        <v>245</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>212</v>
+        <v>246</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>213</v>
+        <v>247</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
@@ -7376,13 +7726,13 @@
     </row>
     <row r="17">
       <c r="A17" s="12" t="s">
-        <v>214</v>
+        <v>248</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>215</v>
+        <v>249</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>216</v>
+        <v>250</v>
       </c>
       <c r="D17" s="12" t="s">
         <v>17</v>
@@ -7391,7 +7741,7 @@
         <v>148</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
@@ -7404,7 +7754,9 @@
       <c r="M17" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="N17" s="11"/>
+      <c r="N17" s="12" t="s">
+        <v>144</v>
+      </c>
       <c r="O17" s="11"/>
       <c r="P17" s="11"/>
       <c r="Q17" s="11"/>
@@ -7423,7 +7775,54 @@
       <c r="AD17" s="11"/>
     </row>
     <row r="18">
-      <c r="B18" s="19"/>
+      <c r="A18" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="17">
+        <v>45827.0</v>
+      </c>
+      <c r="L18" s="11"/>
+      <c r="M18" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N18" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="11"/>
+      <c r="X18" s="11"/>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="11"/>
+      <c r="AB18" s="11"/>
+      <c r="AC18" s="11"/>
+      <c r="AD18" s="11"/>
     </row>
     <row r="19">
       <c r="B19" s="19"/>
@@ -10259,37 +10658,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:AD192">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$M2="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:AD192">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>$M2="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:AD192">
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>$M2="deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC12:AD13">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>$M12="changed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC12:AD13">
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>$M12="deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC12:AD13">
-    <cfRule type="expression" dxfId="1" priority="6">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>$M12="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:AD192">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="1" priority="7">
       <formula>$M2="changed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10386,7 +10785,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>217</v>
+        <v>254</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>25</v>
@@ -10410,7 +10809,7 @@
         <v>62</v>
       </c>
       <c r="O2" s="48" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
@@ -10442,16 +10841,16 @@
     </row>
     <row r="4">
       <c r="A4" s="15" t="s">
-        <v>218</v>
+        <v>255</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>219</v>
+        <v>256</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>220</v>
+        <v>257</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>221</v>
+        <v>258</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>26</v>
@@ -10472,7 +10871,7 @@
         <v>62</v>
       </c>
       <c r="O4" s="48" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
@@ -10492,17 +10891,17 @@
     </row>
     <row r="5">
       <c r="A5" s="12" t="s">
-        <v>222</v>
+        <v>259</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>223</v>
+        <v>260</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>224</v>
+        <v>261</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="12" t="s">
-        <v>225</v>
+        <v>262</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
@@ -10522,7 +10921,7 @@
         <v>62</v>
       </c>
       <c r="O5" s="48" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
@@ -10542,17 +10941,17 @@
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>226</v>
+        <v>263</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>227</v>
+        <v>264</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>228</v>
+        <v>265</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="12" t="s">
-        <v>225</v>
+        <v>262</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
@@ -10588,17 +10987,17 @@
     </row>
     <row r="7">
       <c r="A7" s="12" t="s">
-        <v>229</v>
+        <v>266</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>230</v>
+        <v>267</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>231</v>
+        <v>268</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="12" t="s">
-        <v>225</v>
+        <v>262</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
@@ -10616,7 +11015,7 @@
         <v>62</v>
       </c>
       <c r="O7" s="48" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
@@ -10636,17 +11035,17 @@
     </row>
     <row r="8">
       <c r="A8" s="12" t="s">
-        <v>232</v>
+        <v>269</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>233</v>
+        <v>270</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>234</v>
+        <v>271</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="12" t="s">
-        <v>225</v>
+        <v>262</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
@@ -10664,7 +11063,7 @@
         <v>62</v>
       </c>
       <c r="O8" s="48" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="P8" s="11"/>
       <c r="Q8" s="11"/>
@@ -10684,17 +11083,17 @@
     </row>
     <row r="9">
       <c r="A9" s="53" t="s">
-        <v>235</v>
+        <v>272</v>
       </c>
       <c r="B9" s="54" t="s">
-        <v>236</v>
+        <v>273</v>
       </c>
       <c r="C9" s="53" t="s">
-        <v>237</v>
+        <v>274</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="12" t="s">
-        <v>225</v>
+        <v>262</v>
       </c>
       <c r="F9" s="55"/>
       <c r="G9" s="55"/>
@@ -10712,7 +11111,7 @@
         <v>62</v>
       </c>
       <c r="O9" s="48" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="P9" s="55"/>
       <c r="Q9" s="55"/>
@@ -10732,23 +11131,23 @@
     </row>
     <row r="10">
       <c r="A10" s="12" t="s">
-        <v>238</v>
+        <v>275</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>239</v>
+        <v>276</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>240</v>
+        <v>277</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="18" t="s">
-        <v>225</v>
+        <v>262</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
       <c r="I10" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J10" s="11"/>
       <c r="K10" s="14">
@@ -10792,16 +11191,16 @@
     </row>
     <row r="12">
       <c r="A12" s="15" t="s">
-        <v>241</v>
+        <v>278</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>242</v>
+        <v>279</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>243</v>
+        <v>280</v>
       </c>
       <c r="D12" s="47" t="s">
-        <v>221</v>
+        <v>258</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>26</v>
@@ -10822,7 +11221,7 @@
         <v>62</v>
       </c>
       <c r="O12" s="48" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="P12" s="11"/>
       <c r="Q12" s="11"/>
@@ -10842,17 +11241,17 @@
     </row>
     <row r="13">
       <c r="A13" s="12" t="s">
-        <v>244</v>
+        <v>281</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>244</v>
+        <v>281</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>245</v>
+        <v>282</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="12" t="s">
-        <v>246</v>
+        <v>283</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
@@ -10870,7 +11269,7 @@
         <v>62</v>
       </c>
       <c r="O13" s="48" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="P13" s="11"/>
       <c r="Q13" s="11"/>
@@ -10890,46 +11289,46 @@
     </row>
     <row r="14">
       <c r="A14" s="12" t="s">
-        <v>247</v>
+        <v>284</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>247</v>
+        <v>284</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>248</v>
+        <v>285</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>246</v>
+        <v>283</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>249</v>
+        <v>286</v>
       </c>
       <c r="K14" s="17">
         <v>44699.0</v>
       </c>
       <c r="M14" s="12" t="s">
-        <v>250</v>
+        <v>287</v>
       </c>
       <c r="N14" s="12" t="s">
         <v>62</v>
       </c>
       <c r="O14" s="48" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="12" t="s">
-        <v>251</v>
+        <v>288</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>252</v>
+        <v>289</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>253</v>
+        <v>290</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="12" t="s">
-        <v>246</v>
+        <v>283</v>
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
@@ -10947,7 +11346,7 @@
         <v>62</v>
       </c>
       <c r="O15" s="48" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="P15" s="11"/>
       <c r="Q15" s="11"/>
@@ -10967,23 +11366,23 @@
     </row>
     <row r="16">
       <c r="A16" s="12" t="s">
-        <v>254</v>
+        <v>291</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>255</v>
+        <v>292</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>256</v>
+        <v>293</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="12" t="s">
-        <v>246</v>
+        <v>283</v>
       </c>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
       <c r="I16" s="12" t="s">
-        <v>257</v>
+        <v>294</v>
       </c>
       <c r="J16" s="11"/>
       <c r="K16" s="17">
@@ -10999,7 +11398,7 @@
         <v>62</v>
       </c>
       <c r="O16" s="48" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="P16" s="11"/>
       <c r="Q16" s="11"/>
@@ -11019,23 +11418,23 @@
     </row>
     <row r="17">
       <c r="A17" s="12" t="s">
-        <v>258</v>
+        <v>295</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>259</v>
+        <v>296</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>260</v>
+        <v>297</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="12" t="s">
-        <v>246</v>
+        <v>283</v>
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
       <c r="I17" s="12" t="s">
-        <v>261</v>
+        <v>298</v>
       </c>
       <c r="J17" s="11"/>
       <c r="K17" s="17">
@@ -11051,7 +11450,7 @@
         <v>62</v>
       </c>
       <c r="O17" s="48" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="P17" s="11"/>
       <c r="Q17" s="11"/>
@@ -11071,17 +11470,17 @@
     </row>
     <row r="18">
       <c r="A18" s="12" t="s">
-        <v>262</v>
+        <v>299</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>263</v>
+        <v>300</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>264</v>
+        <v>301</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="12" t="s">
-        <v>246</v>
+        <v>283</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
@@ -11117,17 +11516,17 @@
     </row>
     <row r="19">
       <c r="A19" s="12" t="s">
-        <v>265</v>
+        <v>302</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>266</v>
+        <v>303</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>267</v>
+        <v>304</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="12" t="s">
-        <v>246</v>
+        <v>283</v>
       </c>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
@@ -11170,16 +11569,16 @@
     </row>
     <row r="21">
       <c r="A21" s="15" t="s">
-        <v>268</v>
+        <v>305</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>268</v>
+        <v>305</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>269</v>
+        <v>306</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>246</v>
+        <v>283</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>26</v>
@@ -11200,7 +11599,7 @@
         <v>62</v>
       </c>
       <c r="O21" s="16" t="s">
-        <v>270</v>
+        <v>307</v>
       </c>
       <c r="P21" s="11"/>
       <c r="Q21" s="11"/>
@@ -11220,17 +11619,17 @@
     </row>
     <row r="22">
       <c r="A22" s="12" t="s">
-        <v>271</v>
+        <v>308</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>271</v>
+        <v>308</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>272</v>
+        <v>309</v>
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="12" t="s">
-        <v>273</v>
+        <v>310</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
@@ -11248,7 +11647,7 @@
         <v>62</v>
       </c>
       <c r="O22" s="16" t="s">
-        <v>270</v>
+        <v>307</v>
       </c>
       <c r="P22" s="11"/>
       <c r="Q22" s="11"/>
@@ -11268,17 +11667,17 @@
     </row>
     <row r="23">
       <c r="A23" s="12" t="s">
-        <v>274</v>
+        <v>311</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>274</v>
+        <v>311</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>275</v>
+        <v>312</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="12" t="s">
-        <v>273</v>
+        <v>310</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
@@ -11296,7 +11695,7 @@
         <v>62</v>
       </c>
       <c r="O23" s="16" t="s">
-        <v>270</v>
+        <v>307</v>
       </c>
       <c r="P23" s="11"/>
       <c r="Q23" s="11"/>
@@ -11316,17 +11715,17 @@
     </row>
     <row r="24">
       <c r="A24" s="13" t="s">
-        <v>276</v>
+        <v>313</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>277</v>
+        <v>314</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="12" t="s">
-        <v>273</v>
+        <v>310</v>
       </c>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
@@ -11344,7 +11743,7 @@
         <v>62</v>
       </c>
       <c r="O24" s="16" t="s">
-        <v>270</v>
+        <v>307</v>
       </c>
       <c r="P24" s="11"/>
       <c r="Q24" s="11"/>
@@ -11367,16 +11766,16 @@
     </row>
     <row r="26">
       <c r="A26" s="15" t="s">
-        <v>279</v>
+        <v>316</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>280</v>
+        <v>317</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>281</v>
+        <v>318</v>
       </c>
       <c r="D26" s="47" t="s">
-        <v>221</v>
+        <v>258</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>26</v>
@@ -11397,7 +11796,7 @@
         <v>62</v>
       </c>
       <c r="O26" s="48" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="P26" s="11"/>
       <c r="Q26" s="11"/>
@@ -11417,17 +11816,17 @@
     </row>
     <row r="27">
       <c r="A27" s="12" t="s">
-        <v>282</v>
+        <v>319</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>283</v>
+        <v>320</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>284</v>
+        <v>321</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="12" t="s">
-        <v>285</v>
+        <v>322</v>
       </c>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
@@ -11445,7 +11844,7 @@
         <v>62</v>
       </c>
       <c r="O27" s="48" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="P27" s="11"/>
       <c r="Q27" s="11"/>
@@ -11465,23 +11864,23 @@
     </row>
     <row r="28">
       <c r="A28" s="12" t="s">
-        <v>286</v>
+        <v>323</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>287</v>
+        <v>324</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>288</v>
+        <v>325</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="12" t="s">
-        <v>285</v>
+        <v>322</v>
       </c>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
       <c r="I28" s="12" t="s">
-        <v>289</v>
+        <v>326</v>
       </c>
       <c r="J28" s="11"/>
       <c r="K28" s="17">
@@ -11492,10 +11891,10 @@
         <v>20</v>
       </c>
       <c r="N28" s="12" t="s">
-        <v>290</v>
+        <v>327</v>
       </c>
       <c r="O28" s="48" t="s">
-        <v>291</v>
+        <v>328</v>
       </c>
       <c r="P28" s="11"/>
       <c r="Q28" s="11"/>
@@ -11515,17 +11914,17 @@
     </row>
     <row r="29">
       <c r="A29" s="12" t="s">
-        <v>292</v>
+        <v>329</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>293</v>
+        <v>330</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>294</v>
+        <v>331</v>
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="12" t="s">
-        <v>285</v>
+        <v>322</v>
       </c>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
@@ -11543,7 +11942,7 @@
         <v>62</v>
       </c>
       <c r="O29" s="48" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="P29" s="11"/>
       <c r="Q29" s="11"/>
@@ -11563,17 +11962,17 @@
     </row>
     <row r="30">
       <c r="A30" s="12" t="s">
-        <v>295</v>
+        <v>332</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>296</v>
+        <v>333</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>297</v>
+        <v>334</v>
       </c>
       <c r="D30" s="11"/>
       <c r="E30" s="12" t="s">
-        <v>285</v>
+        <v>322</v>
       </c>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
@@ -11591,7 +11990,7 @@
         <v>62</v>
       </c>
       <c r="O30" s="48" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="P30" s="11"/>
       <c r="Q30" s="11"/>
@@ -11611,17 +12010,17 @@
     </row>
     <row r="31">
       <c r="A31" s="12" t="s">
-        <v>298</v>
+        <v>335</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>299</v>
+        <v>336</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>300</v>
+        <v>337</v>
       </c>
       <c r="D31" s="11"/>
       <c r="E31" s="12" t="s">
-        <v>285</v>
+        <v>322</v>
       </c>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
@@ -11639,7 +12038,7 @@
         <v>62</v>
       </c>
       <c r="O31" s="48" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="P31" s="11"/>
       <c r="Q31" s="11"/>
@@ -11659,17 +12058,17 @@
     </row>
     <row r="32">
       <c r="A32" s="12" t="s">
-        <v>301</v>
+        <v>338</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>302</v>
+        <v>339</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>303</v>
+        <v>340</v>
       </c>
       <c r="D32" s="11"/>
       <c r="E32" s="12" t="s">
-        <v>285</v>
+        <v>322</v>
       </c>
       <c r="F32" s="11"/>
       <c r="G32" s="11"/>
@@ -11687,7 +12086,7 @@
         <v>62</v>
       </c>
       <c r="O32" s="48" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="P32" s="11"/>
       <c r="Q32" s="11"/>
@@ -11710,16 +12109,16 @@
     </row>
     <row r="34">
       <c r="A34" s="15" t="s">
-        <v>304</v>
+        <v>341</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>305</v>
+        <v>342</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>306</v>
+        <v>343</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>221</v>
+        <v>258</v>
       </c>
       <c r="E34" s="12" t="s">
         <v>26</v>
@@ -11758,17 +12157,17 @@
     </row>
     <row r="35">
       <c r="A35" s="12" t="s">
-        <v>307</v>
+        <v>344</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>307</v>
+        <v>344</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>308</v>
+        <v>345</v>
       </c>
       <c r="D35" s="11"/>
       <c r="E35" s="12" t="s">
-        <v>309</v>
+        <v>346</v>
       </c>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
@@ -11804,17 +12203,17 @@
     </row>
     <row r="36">
       <c r="A36" s="12" t="s">
-        <v>310</v>
+        <v>347</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>310</v>
+        <v>347</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>311</v>
+        <v>348</v>
       </c>
       <c r="D36" s="11"/>
       <c r="E36" s="12" t="s">
-        <v>309</v>
+        <v>346</v>
       </c>
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
@@ -11853,16 +12252,16 @@
     </row>
     <row r="38">
       <c r="A38" s="15" t="s">
-        <v>312</v>
+        <v>349</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>313</v>
+        <v>350</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>314</v>
+        <v>351</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>221</v>
+        <v>258</v>
       </c>
       <c r="E38" s="12" t="s">
         <v>26</v>
@@ -11901,17 +12300,17 @@
     </row>
     <row r="39">
       <c r="A39" s="12" t="s">
-        <v>315</v>
+        <v>352</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>316</v>
+        <v>353</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>317</v>
+        <v>354</v>
       </c>
       <c r="D39" s="11"/>
       <c r="E39" s="12" t="s">
-        <v>318</v>
+        <v>355</v>
       </c>
       <c r="F39" s="11"/>
       <c r="G39" s="11"/>
@@ -11947,17 +12346,17 @@
     </row>
     <row r="40">
       <c r="A40" s="12" t="s">
-        <v>319</v>
+        <v>356</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>320</v>
+        <v>357</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>321</v>
+        <v>358</v>
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="12" t="s">
-        <v>318</v>
+        <v>355</v>
       </c>
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
@@ -11993,17 +12392,17 @@
     </row>
     <row r="41">
       <c r="A41" s="12" t="s">
-        <v>322</v>
+        <v>359</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>323</v>
+        <v>360</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>324</v>
+        <v>361</v>
       </c>
       <c r="D41" s="11"/>
       <c r="E41" s="12" t="s">
-        <v>318</v>
+        <v>355</v>
       </c>
       <c r="F41" s="11"/>
       <c r="G41" s="11"/>
@@ -12039,17 +12438,17 @@
     </row>
     <row r="42">
       <c r="A42" s="12" t="s">
-        <v>325</v>
+        <v>362</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>326</v>
+        <v>363</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>327</v>
+        <v>364</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="12" t="s">
-        <v>318</v>
+        <v>355</v>
       </c>
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
@@ -12085,17 +12484,17 @@
     </row>
     <row r="43">
       <c r="A43" s="12" t="s">
-        <v>328</v>
+        <v>365</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>329</v>
+        <v>366</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>330</v>
+        <v>367</v>
       </c>
       <c r="D43" s="11"/>
       <c r="E43" s="12" t="s">
-        <v>318</v>
+        <v>355</v>
       </c>
       <c r="F43" s="11"/>
       <c r="G43" s="11"/>
@@ -12131,17 +12530,17 @@
     </row>
     <row r="44">
       <c r="A44" s="12" t="s">
-        <v>331</v>
+        <v>368</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>332</v>
+        <v>369</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>333</v>
+        <v>370</v>
       </c>
       <c r="D44" s="11"/>
       <c r="E44" s="12" t="s">
-        <v>318</v>
+        <v>355</v>
       </c>
       <c r="F44" s="11"/>
       <c r="G44" s="11"/>
@@ -12177,17 +12576,17 @@
     </row>
     <row r="45">
       <c r="A45" s="12" t="s">
-        <v>334</v>
+        <v>371</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>335</v>
+        <v>372</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>336</v>
+        <v>373</v>
       </c>
       <c r="D45" s="11"/>
       <c r="E45" s="12" t="s">
-        <v>318</v>
+        <v>355</v>
       </c>
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
@@ -12223,17 +12622,17 @@
     </row>
     <row r="46">
       <c r="A46" s="12" t="s">
-        <v>337</v>
+        <v>374</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>338</v>
+        <v>375</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>339</v>
+        <v>376</v>
       </c>
       <c r="D46" s="11"/>
       <c r="E46" s="12" t="s">
-        <v>318</v>
+        <v>355</v>
       </c>
       <c r="F46" s="11"/>
       <c r="G46" s="11"/>
@@ -12269,17 +12668,17 @@
     </row>
     <row r="47">
       <c r="A47" s="12" t="s">
-        <v>340</v>
+        <v>377</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>341</v>
+        <v>378</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>342</v>
+        <v>379</v>
       </c>
       <c r="D47" s="11"/>
       <c r="E47" s="12" t="s">
-        <v>318</v>
+        <v>355</v>
       </c>
       <c r="F47" s="11"/>
       <c r="G47" s="11"/>
@@ -12315,17 +12714,17 @@
     </row>
     <row r="48">
       <c r="A48" s="18" t="s">
-        <v>343</v>
+        <v>380</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>344</v>
+        <v>381</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>345</v>
+        <v>382</v>
       </c>
       <c r="D48" s="11"/>
       <c r="E48" s="12" t="s">
-        <v>318</v>
+        <v>355</v>
       </c>
       <c r="F48" s="11"/>
       <c r="G48" s="11"/>
@@ -12365,16 +12764,16 @@
     </row>
     <row r="50">
       <c r="A50" s="15" t="s">
-        <v>346</v>
+        <v>383</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>347</v>
+        <v>384</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>348</v>
+        <v>385</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>221</v>
+        <v>258</v>
       </c>
       <c r="E50" s="12" t="s">
         <v>26</v>
@@ -12392,7 +12791,7 @@
         <v>20</v>
       </c>
       <c r="N50" s="12" t="s">
-        <v>349</v>
+        <v>386</v>
       </c>
       <c r="O50" s="11"/>
       <c r="P50" s="11"/>
@@ -12413,16 +12812,16 @@
     </row>
     <row r="51">
       <c r="A51" s="15" t="s">
-        <v>350</v>
+        <v>387</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>351</v>
+        <v>388</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>352</v>
+        <v>389</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>353</v>
+        <v>390</v>
       </c>
       <c r="E51" s="12" t="s">
         <v>18</v>
@@ -12440,7 +12839,7 @@
         <v>20</v>
       </c>
       <c r="N51" s="12" t="s">
-        <v>349</v>
+        <v>386</v>
       </c>
       <c r="O51" s="11"/>
       <c r="P51" s="11"/>
@@ -12461,19 +12860,19 @@
     </row>
     <row r="52">
       <c r="A52" s="12" t="s">
-        <v>354</v>
+        <v>391</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>355</v>
+        <v>392</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>356</v>
+        <v>393</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>357</v>
+        <v>394</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>353</v>
+        <v>390</v>
       </c>
       <c r="F52" s="11"/>
       <c r="G52" s="11"/>
@@ -12488,7 +12887,7 @@
         <v>20</v>
       </c>
       <c r="N52" s="12" t="s">
-        <v>349</v>
+        <v>386</v>
       </c>
       <c r="O52" s="11"/>
       <c r="P52" s="11"/>
@@ -12509,19 +12908,19 @@
     </row>
     <row r="53">
       <c r="A53" s="12" t="s">
-        <v>358</v>
+        <v>395</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>359</v>
+        <v>396</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>360</v>
+        <v>397</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>357</v>
+        <v>394</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>353</v>
+        <v>390</v>
       </c>
       <c r="F53" s="11"/>
       <c r="G53" s="11"/>
@@ -12536,7 +12935,7 @@
         <v>20</v>
       </c>
       <c r="N53" s="12" t="s">
-        <v>349</v>
+        <v>386</v>
       </c>
       <c r="O53" s="11"/>
       <c r="P53" s="11"/>
@@ -12557,19 +12956,19 @@
     </row>
     <row r="54">
       <c r="A54" s="12" t="s">
-        <v>361</v>
+        <v>398</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>362</v>
+        <v>399</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>363</v>
+        <v>400</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>357</v>
+        <v>394</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>353</v>
+        <v>390</v>
       </c>
       <c r="F54" s="11"/>
       <c r="G54" s="11"/>
@@ -12584,7 +12983,7 @@
         <v>20</v>
       </c>
       <c r="N54" s="12" t="s">
-        <v>349</v>
+        <v>386</v>
       </c>
       <c r="O54" s="11"/>
       <c r="P54" s="11"/>
@@ -12605,19 +13004,19 @@
     </row>
     <row r="55">
       <c r="A55" s="12" t="s">
-        <v>364</v>
+        <v>401</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>365</v>
+        <v>402</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>366</v>
+        <v>403</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>357</v>
+        <v>394</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>353</v>
+        <v>390</v>
       </c>
       <c r="F55" s="11"/>
       <c r="G55" s="11"/>
@@ -12632,7 +13031,7 @@
         <v>20</v>
       </c>
       <c r="N55" s="12" t="s">
-        <v>349</v>
+        <v>386</v>
       </c>
       <c r="O55" s="11"/>
       <c r="P55" s="11"/>
@@ -12653,16 +13052,16 @@
     </row>
     <row r="56">
       <c r="A56" s="15" t="s">
-        <v>367</v>
+        <v>404</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>368</v>
+        <v>405</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>369</v>
+        <v>406</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>353</v>
+        <v>390</v>
       </c>
       <c r="E56" s="12" t="s">
         <v>26</v>
@@ -12680,7 +13079,7 @@
         <v>20</v>
       </c>
       <c r="N56" s="12" t="s">
-        <v>349</v>
+        <v>386</v>
       </c>
       <c r="O56" s="11"/>
       <c r="P56" s="11"/>
@@ -12701,19 +13100,19 @@
     </row>
     <row r="57">
       <c r="A57" s="12" t="s">
-        <v>370</v>
+        <v>407</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>371</v>
+        <v>408</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>372</v>
+        <v>409</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>373</v>
+        <v>410</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>353</v>
+        <v>390</v>
       </c>
       <c r="F57" s="11"/>
       <c r="G57" s="11"/>
@@ -12728,7 +13127,7 @@
         <v>20</v>
       </c>
       <c r="N57" s="12" t="s">
-        <v>349</v>
+        <v>386</v>
       </c>
       <c r="O57" s="11"/>
       <c r="P57" s="11"/>
@@ -12749,19 +13148,19 @@
     </row>
     <row r="58">
       <c r="A58" s="12" t="s">
-        <v>374</v>
+        <v>411</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>375</v>
+        <v>412</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>376</v>
+        <v>413</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>373</v>
+        <v>410</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>353</v>
+        <v>390</v>
       </c>
       <c r="F58" s="11"/>
       <c r="G58" s="11"/>
@@ -12776,7 +13175,7 @@
         <v>20</v>
       </c>
       <c r="N58" s="12" t="s">
-        <v>349</v>
+        <v>386</v>
       </c>
       <c r="O58" s="11"/>
       <c r="P58" s="11"/>
@@ -12797,19 +13196,19 @@
     </row>
     <row r="59">
       <c r="A59" s="12" t="s">
-        <v>377</v>
+        <v>414</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>378</v>
+        <v>415</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>379</v>
+        <v>416</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>373</v>
+        <v>410</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>353</v>
+        <v>390</v>
       </c>
       <c r="F59" s="11"/>
       <c r="G59" s="11"/>
@@ -12824,7 +13223,7 @@
         <v>20</v>
       </c>
       <c r="N59" s="12" t="s">
-        <v>349</v>
+        <v>386</v>
       </c>
       <c r="O59" s="11"/>
       <c r="P59" s="11"/>
@@ -12845,19 +13244,19 @@
     </row>
     <row r="60">
       <c r="A60" s="12" t="s">
-        <v>380</v>
+        <v>417</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>381</v>
+        <v>418</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>382</v>
+        <v>419</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>373</v>
+        <v>410</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>353</v>
+        <v>390</v>
       </c>
       <c r="F60" s="11"/>
       <c r="G60" s="11"/>
@@ -12872,7 +13271,7 @@
         <v>20</v>
       </c>
       <c r="N60" s="12" t="s">
-        <v>349</v>
+        <v>386</v>
       </c>
       <c r="O60" s="11"/>
       <c r="P60" s="11"/>
@@ -12897,16 +13296,16 @@
     </row>
     <row r="62">
       <c r="A62" s="15" t="s">
-        <v>383</v>
+        <v>420</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>384</v>
+        <v>421</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>385</v>
+        <v>422</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>221</v>
+        <v>258</v>
       </c>
       <c r="E62" s="12" t="s">
         <v>26</v>
@@ -12915,7 +13314,7 @@
       <c r="G62" s="11"/>
       <c r="H62" s="11"/>
       <c r="I62" s="12" t="s">
-        <v>386</v>
+        <v>423</v>
       </c>
       <c r="J62" s="11"/>
       <c r="K62" s="17">
@@ -12926,7 +13325,7 @@
         <v>20</v>
       </c>
       <c r="N62" s="12" t="s">
-        <v>349</v>
+        <v>386</v>
       </c>
       <c r="O62" s="11"/>
       <c r="P62" s="11"/>
@@ -12947,16 +13346,16 @@
     </row>
     <row r="63">
       <c r="A63" s="12" t="s">
-        <v>387</v>
+        <v>424</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>387</v>
+        <v>424</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>388</v>
+        <v>425</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>389</v>
+        <v>426</v>
       </c>
       <c r="E63" s="12" t="s">
         <v>18</v>
@@ -12974,7 +13373,7 @@
         <v>20</v>
       </c>
       <c r="N63" s="12" t="s">
-        <v>349</v>
+        <v>386</v>
       </c>
       <c r="O63" s="11"/>
       <c r="P63" s="11"/>
@@ -12995,16 +13394,16 @@
     </row>
     <row r="64">
       <c r="A64" s="12" t="s">
-        <v>390</v>
+        <v>427</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>390</v>
+        <v>427</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>391</v>
+        <v>428</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>389</v>
+        <v>426</v>
       </c>
       <c r="E64" s="12" t="s">
         <v>18</v>
@@ -13022,7 +13421,7 @@
         <v>20</v>
       </c>
       <c r="N64" s="12" t="s">
-        <v>349</v>
+        <v>386</v>
       </c>
       <c r="O64" s="11"/>
       <c r="P64" s="11"/>
@@ -13047,23 +13446,23 @@
     </row>
     <row r="66">
       <c r="A66" s="15" t="s">
-        <v>392</v>
+        <v>429</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>393</v>
+        <v>430</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>385</v>
+        <v>422</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>221</v>
+        <v>258</v>
       </c>
       <c r="E66" s="11"/>
       <c r="F66" s="11"/>
       <c r="G66" s="11"/>
       <c r="H66" s="11"/>
       <c r="I66" s="12" t="s">
-        <v>394</v>
+        <v>431</v>
       </c>
       <c r="J66" s="11"/>
       <c r="K66" s="17">
@@ -13074,7 +13473,7 @@
         <v>20</v>
       </c>
       <c r="N66" s="12" t="s">
-        <v>349</v>
+        <v>386</v>
       </c>
       <c r="O66" s="11"/>
       <c r="P66" s="11"/>
@@ -13095,16 +13494,16 @@
     </row>
     <row r="67">
       <c r="A67" s="12" t="s">
-        <v>395</v>
+        <v>432</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>395</v>
+        <v>432</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>396</v>
+        <v>433</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>397</v>
+        <v>434</v>
       </c>
       <c r="E67" s="12" t="s">
         <v>18</v>
@@ -13122,7 +13521,7 @@
         <v>20</v>
       </c>
       <c r="N67" s="12" t="s">
-        <v>349</v>
+        <v>386</v>
       </c>
       <c r="O67" s="11"/>
       <c r="P67" s="11"/>
@@ -13143,16 +13542,16 @@
     </row>
     <row r="68">
       <c r="A68" s="12" t="s">
-        <v>398</v>
+        <v>435</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>398</v>
+        <v>435</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>399</v>
+        <v>436</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>397</v>
+        <v>434</v>
       </c>
       <c r="E68" s="12" t="s">
         <v>18</v>
@@ -13170,7 +13569,7 @@
         <v>20</v>
       </c>
       <c r="N68" s="12" t="s">
-        <v>349</v>
+        <v>386</v>
       </c>
       <c r="O68" s="11"/>
       <c r="P68" s="11"/>
@@ -13195,16 +13594,16 @@
     </row>
     <row r="70">
       <c r="A70" s="15" t="s">
-        <v>400</v>
+        <v>437</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>401</v>
+        <v>438</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>402</v>
+        <v>439</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>221</v>
+        <v>258</v>
       </c>
       <c r="E70" s="12" t="s">
         <v>26</v>
@@ -13222,7 +13621,7 @@
         <v>20</v>
       </c>
       <c r="N70" s="12" t="s">
-        <v>349</v>
+        <v>386</v>
       </c>
       <c r="O70" s="11"/>
       <c r="P70" s="11"/>
@@ -13243,16 +13642,16 @@
     </row>
     <row r="71">
       <c r="A71" s="12" t="s">
-        <v>403</v>
+        <v>440</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>404</v>
+        <v>441</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>405</v>
+        <v>442</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>406</v>
+        <v>443</v>
       </c>
       <c r="E71" s="12" t="s">
         <v>18</v>
@@ -13261,7 +13660,7 @@
       <c r="G71" s="11"/>
       <c r="H71" s="11"/>
       <c r="I71" s="12" t="s">
-        <v>407</v>
+        <v>444</v>
       </c>
       <c r="J71" s="11"/>
       <c r="K71" s="17">
@@ -13272,7 +13671,7 @@
         <v>20</v>
       </c>
       <c r="N71" s="12" t="s">
-        <v>349</v>
+        <v>386</v>
       </c>
       <c r="O71" s="11"/>
       <c r="P71" s="11"/>
@@ -13293,16 +13692,16 @@
     </row>
     <row r="72">
       <c r="A72" s="12" t="s">
-        <v>408</v>
+        <v>445</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>409</v>
+        <v>446</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>410</v>
+        <v>447</v>
       </c>
       <c r="D72" s="12" t="s">
-        <v>406</v>
+        <v>443</v>
       </c>
       <c r="E72" s="12" t="s">
         <v>18</v>
@@ -13311,7 +13710,7 @@
       <c r="G72" s="11"/>
       <c r="H72" s="11"/>
       <c r="I72" s="12" t="s">
-        <v>411</v>
+        <v>448</v>
       </c>
       <c r="J72" s="11"/>
       <c r="K72" s="17">
@@ -13322,7 +13721,7 @@
         <v>20</v>
       </c>
       <c r="N72" s="12" t="s">
-        <v>349</v>
+        <v>386</v>
       </c>
       <c r="O72" s="11"/>
       <c r="P72" s="11"/>
@@ -13343,16 +13742,16 @@
     </row>
     <row r="73">
       <c r="A73" s="12" t="s">
-        <v>412</v>
+        <v>449</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>413</v>
+        <v>450</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>414</v>
+        <v>451</v>
       </c>
       <c r="D73" s="12" t="s">
-        <v>406</v>
+        <v>443</v>
       </c>
       <c r="E73" s="12" t="s">
         <v>18</v>
@@ -13370,7 +13769,7 @@
         <v>20</v>
       </c>
       <c r="N73" s="12" t="s">
-        <v>349</v>
+        <v>386</v>
       </c>
       <c r="O73" s="11"/>
       <c r="P73" s="11"/>
@@ -13394,16 +13793,16 @@
     </row>
     <row r="75">
       <c r="A75" s="15" t="s">
-        <v>415</v>
+        <v>452</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>416</v>
+        <v>453</v>
       </c>
       <c r="C75" s="12" t="s">
-        <v>417</v>
+        <v>454</v>
       </c>
       <c r="D75" s="12" t="s">
-        <v>221</v>
+        <v>258</v>
       </c>
       <c r="E75" s="12" t="s">
         <v>26</v>
@@ -13442,17 +13841,17 @@
     </row>
     <row r="76">
       <c r="A76" s="12" t="s">
-        <v>418</v>
+        <v>455</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>419</v>
+        <v>456</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>420</v>
+        <v>457</v>
       </c>
       <c r="D76" s="11"/>
       <c r="E76" s="12" t="s">
-        <v>421</v>
+        <v>458</v>
       </c>
       <c r="F76" s="11"/>
       <c r="G76" s="11"/>
@@ -13488,17 +13887,17 @@
     </row>
     <row r="77">
       <c r="A77" s="12" t="s">
-        <v>422</v>
+        <v>459</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>423</v>
+        <v>460</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>424</v>
+        <v>461</v>
       </c>
       <c r="D77" s="11"/>
       <c r="E77" s="12" t="s">
-        <v>421</v>
+        <v>458</v>
       </c>
       <c r="F77" s="11"/>
       <c r="G77" s="11"/>
@@ -13534,17 +13933,17 @@
     </row>
     <row r="78">
       <c r="A78" s="12" t="s">
-        <v>425</v>
+        <v>462</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>426</v>
+        <v>463</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>427</v>
+        <v>464</v>
       </c>
       <c r="D78" s="11"/>
       <c r="E78" s="12" t="s">
-        <v>421</v>
+        <v>458</v>
       </c>
       <c r="F78" s="11"/>
       <c r="G78" s="11"/>
@@ -13580,17 +13979,17 @@
     </row>
     <row r="79">
       <c r="A79" s="12" t="s">
-        <v>428</v>
+        <v>465</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>429</v>
+        <v>466</v>
       </c>
       <c r="C79" s="12" t="s">
-        <v>430</v>
+        <v>467</v>
       </c>
       <c r="D79" s="11"/>
       <c r="E79" s="12" t="s">
-        <v>421</v>
+        <v>458</v>
       </c>
       <c r="F79" s="11"/>
       <c r="G79" s="11"/>
@@ -13626,17 +14025,17 @@
     </row>
     <row r="80">
       <c r="A80" s="12" t="s">
-        <v>431</v>
+        <v>468</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>432</v>
+        <v>469</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>433</v>
+        <v>470</v>
       </c>
       <c r="D80" s="11"/>
       <c r="E80" s="12" t="s">
-        <v>421</v>
+        <v>458</v>
       </c>
       <c r="F80" s="11"/>
       <c r="G80" s="11"/>
@@ -16045,22 +16444,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A50:AD73">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$M50="modified"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:AD73">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>$M50="deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:AB73">
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$M50="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:AD200">
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$M1="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16123,13 +16522,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>152</v>
+        <v>186</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>153</v>
+        <v>187</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>154</v>
+        <v>188</v>
       </c>
       <c r="G1" s="23" t="s">
         <v>6</v>
@@ -16144,7 +16543,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="27" t="s">
-        <v>155</v>
+        <v>189</v>
       </c>
       <c r="L1" s="28" t="s">
         <v>11</v>
@@ -16161,22 +16560,22 @@
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>434</v>
+        <v>471</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>435</v>
+        <v>472</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>436</v>
+        <v>473</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>221</v>
+        <v>258</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
@@ -16193,7 +16592,7 @@
         <v>62</v>
       </c>
       <c r="O2" s="16" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
@@ -16213,22 +16612,22 @@
     </row>
     <row r="3">
       <c r="A3" s="12" t="s">
-        <v>437</v>
+        <v>474</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>438</v>
+        <v>475</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>439</v>
+        <v>476</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>246</v>
+        <v>283</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>440</v>
+        <v>477</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -16245,7 +16644,7 @@
         <v>62</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="P3" s="11"/>
       <c r="Q3" s="11"/>
@@ -16265,22 +16664,22 @@
     </row>
     <row r="4">
       <c r="A4" s="12" t="s">
-        <v>441</v>
+        <v>478</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>442</v>
+        <v>479</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>443</v>
+        <v>480</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>225</v>
+        <v>262</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>440</v>
+        <v>477</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
@@ -16297,7 +16696,7 @@
         <v>62</v>
       </c>
       <c r="O4" s="16" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
@@ -16317,22 +16716,22 @@
     </row>
     <row r="5">
       <c r="A5" s="12" t="s">
-        <v>444</v>
+        <v>481</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>445</v>
+        <v>482</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>446</v>
+        <v>483</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>285</v>
+        <v>322</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>440</v>
+        <v>477</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -16349,7 +16748,7 @@
         <v>62</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>447</v>
+        <v>484</v>
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
@@ -16369,22 +16768,22 @@
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>448</v>
+        <v>485</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>449</v>
+        <v>486</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>450</v>
+        <v>487</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>273</v>
+        <v>310</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>451</v>
+        <v>488</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
@@ -16419,22 +16818,22 @@
     </row>
     <row r="7">
       <c r="A7" s="12" t="s">
-        <v>452</v>
+        <v>489</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>453</v>
+        <v>490</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>454</v>
+        <v>491</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>353</v>
+        <v>390</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>440</v>
+        <v>477</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -16469,22 +16868,22 @@
     </row>
     <row r="8">
       <c r="A8" s="12" t="s">
-        <v>455</v>
+        <v>492</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>456</v>
+        <v>493</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>457</v>
+        <v>494</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>389</v>
+        <v>426</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>440</v>
+        <v>477</v>
       </c>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
@@ -16519,22 +16918,22 @@
     </row>
     <row r="9">
       <c r="A9" s="12" t="s">
-        <v>458</v>
+        <v>495</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>459</v>
+        <v>496</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>460</v>
+        <v>497</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>397</v>
+        <v>434</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>440</v>
+        <v>477</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
@@ -16571,22 +16970,22 @@
     </row>
     <row r="10">
       <c r="A10" s="12" t="s">
-        <v>461</v>
+        <v>498</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>462</v>
+        <v>499</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>463</v>
+        <v>500</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>406</v>
+        <v>443</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>440</v>
+        <v>477</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
@@ -16621,28 +17020,28 @@
     </row>
     <row r="11">
       <c r="A11" s="12" t="s">
-        <v>464</v>
+        <v>501</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>465</v>
+        <v>502</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>466</v>
+        <v>503</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>467</v>
+        <v>504</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="K11" s="14">
         <v>45422.0</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>468</v>
+        <v>505</v>
       </c>
       <c r="N11" s="12" t="s">
         <v>62</v>
@@ -16650,28 +17049,28 @@
     </row>
     <row r="12">
       <c r="A12" s="12" t="s">
-        <v>469</v>
+        <v>506</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>470</v>
+        <v>507</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>471</v>
+        <v>508</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>467</v>
+        <v>504</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="K12" s="14">
         <v>45422.0</v>
       </c>
       <c r="M12" s="12" t="s">
-        <v>468</v>
+        <v>505</v>
       </c>
       <c r="N12" s="12" t="s">
         <v>62</v>
@@ -16679,28 +17078,28 @@
     </row>
     <row r="13">
       <c r="A13" s="12" t="s">
-        <v>472</v>
+        <v>509</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>473</v>
+        <v>510</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>474</v>
+        <v>511</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>467</v>
+        <v>504</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="K13" s="14">
         <v>45422.0</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>468</v>
+        <v>505</v>
       </c>
       <c r="N13" s="12" t="s">
         <v>62</v>
@@ -16708,22 +17107,22 @@
     </row>
     <row r="14">
       <c r="A14" s="12" t="s">
-        <v>475</v>
+        <v>512</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>476</v>
+        <v>513</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>477</v>
+        <v>514</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>309</v>
+        <v>346</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="K14" s="17">
         <v>45453.0</v>
@@ -16737,22 +17136,22 @@
     </row>
     <row r="15">
       <c r="A15" s="12" t="s">
-        <v>478</v>
+        <v>515</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>479</v>
+        <v>516</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>480</v>
+        <v>517</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>318</v>
+        <v>355</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="K15" s="17">
         <v>45453.0</v>
@@ -16766,22 +17165,22 @@
     </row>
     <row r="16">
       <c r="A16" s="12" t="s">
-        <v>481</v>
+        <v>518</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>482</v>
+        <v>519</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>483</v>
+        <v>520</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>421</v>
+        <v>458</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="K16" s="17">
         <v>45453.0</v>
@@ -19636,52 +20035,52 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A11:AD13">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$M11="changed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:AD13">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$M11="deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:AD13">
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$M11="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:AD13">
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$M11="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:AD10">
-    <cfRule type="expression" dxfId="1" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>$M7="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:AD10">
-    <cfRule type="expression" dxfId="0" priority="6">
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>$M7="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:AD10">
-    <cfRule type="expression" dxfId="4" priority="7">
+    <cfRule type="expression" dxfId="0" priority="7">
       <formula>$M7="deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:AD10">
-    <cfRule type="expression" dxfId="5" priority="8">
+    <cfRule type="expression" dxfId="1" priority="8">
       <formula>$M7="changed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:AD6">
-    <cfRule type="expression" dxfId="1" priority="9">
+    <cfRule type="expression" dxfId="3" priority="9">
       <formula>$M2="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:AD6">
-    <cfRule type="expression" dxfId="0" priority="10">
+    <cfRule type="expression" dxfId="2" priority="10">
       <formula>$M2="proposed"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add ReuseCompatibility to SECTOR-HEALTH
- added `ReuseCompatibility` concepts to SECTOR-HEALTH by extending the
  DPV Context concepts
- changed definition of `dpv:ReuseCompatibility` concepts by replacing
  "Concept ..." with "Status ..." to indicate these are statuses
- added Status optional section to template for sectors
- fixes minor error in 300.py regarding printing which vocabs are params

Co-authored-by: Beatriz Esteves <beatriz.gc.esteves@gmail.com>
Co-authored-by: Julian Flake <flake@uni-koblenz.de>
</commit_message>
<xml_diff>
--- a/code/vocab_csv/context_status.xlsx
+++ b/code/vocab_csv/context_status.xlsx
@@ -3,10 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Context" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Context_properties" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Status" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Status_properties" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Context" sheetId="1" r:id="rId5"/>
+    <sheet state="visible" name="Context_properties" sheetId="2" r:id="rId6"/>
+    <sheet state="visible" name="Status" sheetId="3" r:id="rId7"/>
+    <sheet state="visible" name="Status_properties" sheetId="4" r:id="rId8"/>
+    <sheet state="visible" name="Sector_Health_Status" sheetId="5" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="528">
   <si>
     <t>Term</t>
   </si>
@@ -1338,7 +1339,7 @@
     <t>ReuseCompatibility</t>
   </si>
   <si>
-    <t>Concept indicating whether the specified context is compatible with another earlier context</t>
+    <t>Status indicating whether the specified context is compatible with another earlier context</t>
   </si>
   <si>
     <t>Compatibility refers to whether two contexts, such as dpv:Process instances, are compatible with each other based on a criteria which is not defined by the concept. This criteria can be based on requirements from law, such as GDPR's purpose compatibility or can be based on privacy norms such as contextual integrity. To express such interpretations, further concepts should be expanded from this base concept</t>
@@ -1353,7 +1354,7 @@
     <t>Primary Use</t>
   </si>
   <si>
-    <t>Concept indicating compatibility based on the use being either the original context or something that is compatible with it</t>
+    <t>Status indicating compatibility based on the use being either the original context or something that is compatible with it</t>
   </si>
   <si>
     <t>dpv:ReuseCompatibility</t>
@@ -1368,7 +1369,7 @@
     <t>Secondary Use</t>
   </si>
   <si>
-    <t>Concept indicating incompatibility based on the use not being compatible with an earlier context</t>
+    <t>Status indicating incompatibility based on the use not being compatible with an earlier context</t>
   </si>
   <si>
     <t>Secondary Use refers to an assessment where two contexts are found to be incompatible, e.g. if purpose is used to test compatibility, then for two activities the second activity is said be the secondary use if its purpose is incompatible with the first activity's purpose</t>
@@ -1380,7 +1381,7 @@
     <t>Primary Initial Use</t>
   </si>
   <si>
-    <t>Concept indicating this is the first or initial context which will be used for comparing compatibility with</t>
+    <t>Status indicating this is the first or initial context which will be used for comparing compatibility with</t>
   </si>
   <si>
     <t>dpv:PrimaryUse</t>
@@ -1395,7 +1396,7 @@
     <t>Primary Subsequent Reuse</t>
   </si>
   <si>
-    <t>Concept indicating this is a compatible reuse with a prior initial context</t>
+    <t>Status indicating this is a compatible reuse with a prior initial context</t>
   </si>
   <si>
     <t>Primary Subsequent Reuse indicates that this is not the original or initial context but another context which is compatible with it</t>
@@ -1407,7 +1408,7 @@
     <t>Secondary Contextual Reuse</t>
   </si>
   <si>
-    <t>Concept indicating incompatibility based on the use not being compatible with an earlier context but still being within the same broader context i.e. the degree of incompability does not violate or go beyond some established parameters or norms</t>
+    <t>Status indicating incompatibility based on the use not being compatible with an earlier context but still being within the same broader context i.e. the degree of incompability does not violate or go beyond some established parameters or norms</t>
   </si>
   <si>
     <t>dpv:SecondaryUse</t>
@@ -1422,7 +1423,7 @@
     <t>Tertiary Use</t>
   </si>
   <si>
-    <t>Concept indicating incompatibility that goes beyond some established parameters or norms to the extent that it is considered tertiary or completely removed or detached from the initial primary use</t>
+    <t>Status indicating incompatibility that goes beyond some established parameters or norms to the extent that it is considered tertiary or completely removed or detached from the initial primary use</t>
   </si>
   <si>
     <t>Tertiary Use is useful to indicate that the incompatibility is to such a degree that it should not be considered mere secondary use of the data and should be further distinguished from it. For example, in healthcare, reusing data from patients for medical research is considered secondary use, but if the same data is being used by external third parties who have no relation to the patients and are not using it for public good, then it can be considered as a Tertiary Use. This concept is intended to be analogous to "Third Party" in privacy contexts</t>
@@ -1434,7 +1435,7 @@
     <t>Compatibility Unknown</t>
   </si>
   <si>
-    <t>Concept indicating the compatibility of the context with an earlier context is currently unknown</t>
+    <t>Status indicating the compatibility of the context with an earlier context is currently unknown</t>
   </si>
   <si>
     <t>hasStatus</t>
@@ -1594,6 +1595,24 @@
   </si>
   <si>
     <t>Indicates the reuse compatibility for the specified context</t>
+  </si>
+  <si>
+    <t>Status indicating whether the reuse of health data is compatible for given context</t>
+  </si>
+  <si>
+    <t>Status indicating the reuse of health is compatible with the original purpose or use i.e. it can be considered as 'Primary Use'</t>
+  </si>
+  <si>
+    <t>sector-health:ReuseCompatibility</t>
+  </si>
+  <si>
+    <t>Status indicating the reuse of health is incompatible with the original purpose or use i.e. it is considered as 'Secondary Use'</t>
+  </si>
+  <si>
+    <t>Status indicating the compatibility for reuse of health data for the context is currently unknown</t>
+  </si>
+  <si>
+    <t>dpv:CompatibilityUnknown</t>
   </si>
 </sst>
 </file>
@@ -2051,6 +2070,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<x18tc:personList xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
@@ -13808,8 +13835,11 @@
       <c r="K82" s="17">
         <v>45827.0</v>
       </c>
+      <c r="L82" s="17">
+        <v>46060.0</v>
+      </c>
       <c r="M82" s="12" t="s">
-        <v>20</v>
+        <v>278</v>
       </c>
       <c r="N82" s="12" t="s">
         <v>438</v>
@@ -13834,8 +13864,11 @@
       <c r="K83" s="17">
         <v>45827.0</v>
       </c>
+      <c r="L83" s="17">
+        <v>46060.0</v>
+      </c>
       <c r="M83" s="12" t="s">
-        <v>20</v>
+        <v>278</v>
       </c>
       <c r="N83" s="12" t="s">
         <v>438</v>
@@ -13860,8 +13893,11 @@
       <c r="K84" s="17">
         <v>45827.0</v>
       </c>
+      <c r="L84" s="17">
+        <v>46060.0</v>
+      </c>
       <c r="M84" s="12" t="s">
-        <v>20</v>
+        <v>278</v>
       </c>
       <c r="N84" s="12" t="s">
         <v>438</v>
@@ -13999,8 +14035,11 @@
       <c r="K89" s="17">
         <v>45827.0</v>
       </c>
+      <c r="L89" s="17">
+        <v>46060.0</v>
+      </c>
       <c r="M89" s="12" t="s">
-        <v>20</v>
+        <v>278</v>
       </c>
       <c r="N89" s="12" t="s">
         <v>438</v>
@@ -20094,4 +20133,2561 @@
   </hyperlinks>
   <drawing r:id="rId5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1.0" ySplit="1.0" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B1" sqref="B1" pane="topRight"/>
+      <selection activeCell="A2" sqref="A2" pane="bottomLeft"/>
+      <selection activeCell="B2" sqref="B2" pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="29.88"/>
+    <col customWidth="1" min="2" max="2" width="31.88"/>
+    <col customWidth="1" min="3" max="3" width="60.88"/>
+    <col customWidth="1" min="9" max="9" width="43.13"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="28.5" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="12" t="s">
+        <v>435</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>435</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>522</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>437</v>
+      </c>
+      <c r="K2" s="17">
+        <v>45827.0</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="12" t="s">
+        <v>439</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>440</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>523</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>451</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>524</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="K3" s="17">
+        <v>45827.0</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="12" t="s">
+        <v>444</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>445</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>525</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>460</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>524</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>447</v>
+      </c>
+      <c r="K4" s="17">
+        <v>45827.0</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="12" t="s">
+        <v>466</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>467</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>526</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>527</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>524</v>
+      </c>
+      <c r="K5" s="17">
+        <v>45827.0</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="19"/>
+    </row>
+    <row r="7">
+      <c r="B7" s="19"/>
+    </row>
+    <row r="8">
+      <c r="B8" s="19"/>
+    </row>
+    <row r="9">
+      <c r="B9" s="19"/>
+    </row>
+    <row r="10">
+      <c r="B10" s="19"/>
+    </row>
+    <row r="11">
+      <c r="B11" s="19"/>
+    </row>
+    <row r="12">
+      <c r="B12" s="19"/>
+    </row>
+    <row r="13">
+      <c r="B13" s="19"/>
+    </row>
+    <row r="14">
+      <c r="B14" s="19"/>
+    </row>
+    <row r="15">
+      <c r="B15" s="19"/>
+    </row>
+    <row r="16">
+      <c r="B16" s="19"/>
+    </row>
+    <row r="17">
+      <c r="B17" s="19"/>
+    </row>
+    <row r="18">
+      <c r="B18" s="19"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="19"/>
+    </row>
+    <row r="20">
+      <c r="B20" s="19"/>
+    </row>
+    <row r="21">
+      <c r="B21" s="19"/>
+    </row>
+    <row r="22">
+      <c r="B22" s="19"/>
+    </row>
+    <row r="23">
+      <c r="B23" s="19"/>
+    </row>
+    <row r="24">
+      <c r="B24" s="19"/>
+    </row>
+    <row r="25">
+      <c r="B25" s="19"/>
+    </row>
+    <row r="26">
+      <c r="B26" s="19"/>
+    </row>
+    <row r="27">
+      <c r="B27" s="19"/>
+    </row>
+    <row r="28">
+      <c r="B28" s="19"/>
+    </row>
+    <row r="29">
+      <c r="B29" s="19"/>
+    </row>
+    <row r="30">
+      <c r="B30" s="19"/>
+    </row>
+    <row r="31">
+      <c r="B31" s="19"/>
+    </row>
+    <row r="32">
+      <c r="B32" s="19"/>
+    </row>
+    <row r="33">
+      <c r="B33" s="19"/>
+    </row>
+    <row r="34">
+      <c r="B34" s="19"/>
+    </row>
+    <row r="35">
+      <c r="B35" s="19"/>
+    </row>
+    <row r="36">
+      <c r="B36" s="19"/>
+    </row>
+    <row r="37">
+      <c r="B37" s="19"/>
+    </row>
+    <row r="38">
+      <c r="B38" s="19"/>
+    </row>
+    <row r="39">
+      <c r="B39" s="19"/>
+    </row>
+    <row r="40">
+      <c r="B40" s="19"/>
+    </row>
+    <row r="41">
+      <c r="B41" s="19"/>
+    </row>
+    <row r="42">
+      <c r="B42" s="19"/>
+    </row>
+    <row r="43">
+      <c r="B43" s="19"/>
+    </row>
+    <row r="44">
+      <c r="B44" s="19"/>
+    </row>
+    <row r="45">
+      <c r="B45" s="19"/>
+    </row>
+    <row r="46">
+      <c r="B46" s="19"/>
+    </row>
+    <row r="47">
+      <c r="B47" s="19"/>
+    </row>
+    <row r="48">
+      <c r="B48" s="19"/>
+    </row>
+    <row r="49">
+      <c r="B49" s="19"/>
+    </row>
+    <row r="50">
+      <c r="B50" s="19"/>
+    </row>
+    <row r="51">
+      <c r="B51" s="19"/>
+    </row>
+    <row r="52">
+      <c r="B52" s="19"/>
+    </row>
+    <row r="53">
+      <c r="B53" s="19"/>
+    </row>
+    <row r="54">
+      <c r="B54" s="19"/>
+    </row>
+    <row r="55">
+      <c r="B55" s="19"/>
+    </row>
+    <row r="56">
+      <c r="B56" s="19"/>
+    </row>
+    <row r="57">
+      <c r="B57" s="19"/>
+    </row>
+    <row r="58">
+      <c r="B58" s="19"/>
+    </row>
+    <row r="59">
+      <c r="B59" s="19"/>
+    </row>
+    <row r="60">
+      <c r="B60" s="19"/>
+    </row>
+    <row r="61">
+      <c r="B61" s="19"/>
+    </row>
+    <row r="62">
+      <c r="B62" s="19"/>
+    </row>
+    <row r="63">
+      <c r="B63" s="19"/>
+    </row>
+    <row r="64">
+      <c r="B64" s="19"/>
+    </row>
+    <row r="65">
+      <c r="B65" s="19"/>
+    </row>
+    <row r="66">
+      <c r="B66" s="19"/>
+    </row>
+    <row r="67">
+      <c r="B67" s="19"/>
+    </row>
+    <row r="68">
+      <c r="B68" s="19"/>
+    </row>
+    <row r="69">
+      <c r="B69" s="19"/>
+    </row>
+    <row r="70">
+      <c r="B70" s="19"/>
+    </row>
+    <row r="71">
+      <c r="B71" s="19"/>
+    </row>
+    <row r="72">
+      <c r="B72" s="19"/>
+    </row>
+    <row r="73">
+      <c r="B73" s="19"/>
+    </row>
+    <row r="74">
+      <c r="B74" s="19"/>
+    </row>
+    <row r="75">
+      <c r="B75" s="19"/>
+    </row>
+    <row r="76">
+      <c r="B76" s="19"/>
+    </row>
+    <row r="77">
+      <c r="B77" s="19"/>
+    </row>
+    <row r="78">
+      <c r="B78" s="19"/>
+    </row>
+    <row r="79">
+      <c r="B79" s="19"/>
+    </row>
+    <row r="80">
+      <c r="B80" s="19"/>
+    </row>
+    <row r="81">
+      <c r="B81" s="19"/>
+    </row>
+    <row r="82">
+      <c r="B82" s="19"/>
+    </row>
+    <row r="83">
+      <c r="B83" s="19"/>
+    </row>
+    <row r="84">
+      <c r="B84" s="19"/>
+    </row>
+    <row r="85">
+      <c r="B85" s="19"/>
+    </row>
+    <row r="86">
+      <c r="B86" s="19"/>
+    </row>
+    <row r="87">
+      <c r="B87" s="19"/>
+    </row>
+    <row r="88">
+      <c r="B88" s="19"/>
+    </row>
+    <row r="89">
+      <c r="B89" s="19"/>
+    </row>
+    <row r="90">
+      <c r="B90" s="19"/>
+    </row>
+    <row r="91">
+      <c r="B91" s="19"/>
+    </row>
+    <row r="92">
+      <c r="B92" s="19"/>
+    </row>
+    <row r="93">
+      <c r="B93" s="19"/>
+    </row>
+    <row r="94">
+      <c r="B94" s="19"/>
+    </row>
+    <row r="95">
+      <c r="B95" s="19"/>
+    </row>
+    <row r="96">
+      <c r="B96" s="19"/>
+    </row>
+    <row r="97">
+      <c r="B97" s="19"/>
+    </row>
+    <row r="98">
+      <c r="B98" s="19"/>
+    </row>
+    <row r="99">
+      <c r="B99" s="19"/>
+    </row>
+    <row r="100">
+      <c r="B100" s="19"/>
+    </row>
+    <row r="101">
+      <c r="B101" s="19"/>
+    </row>
+    <row r="102">
+      <c r="B102" s="19"/>
+    </row>
+    <row r="103">
+      <c r="B103" s="19"/>
+    </row>
+    <row r="104">
+      <c r="B104" s="19"/>
+    </row>
+    <row r="105">
+      <c r="B105" s="19"/>
+    </row>
+    <row r="106">
+      <c r="B106" s="19"/>
+    </row>
+    <row r="107">
+      <c r="B107" s="19"/>
+    </row>
+    <row r="108">
+      <c r="B108" s="19"/>
+    </row>
+    <row r="109">
+      <c r="B109" s="19"/>
+    </row>
+    <row r="110">
+      <c r="B110" s="19"/>
+    </row>
+    <row r="111">
+      <c r="B111" s="19"/>
+    </row>
+    <row r="112">
+      <c r="B112" s="19"/>
+    </row>
+    <row r="113">
+      <c r="B113" s="19"/>
+    </row>
+    <row r="114">
+      <c r="B114" s="19"/>
+    </row>
+    <row r="115">
+      <c r="B115" s="19"/>
+    </row>
+    <row r="116">
+      <c r="B116" s="19"/>
+    </row>
+    <row r="117">
+      <c r="B117" s="19"/>
+    </row>
+    <row r="118">
+      <c r="B118" s="19"/>
+    </row>
+    <row r="119">
+      <c r="B119" s="19"/>
+    </row>
+    <row r="120">
+      <c r="B120" s="19"/>
+    </row>
+    <row r="121">
+      <c r="B121" s="19"/>
+    </row>
+    <row r="122">
+      <c r="B122" s="19"/>
+    </row>
+    <row r="123">
+      <c r="B123" s="19"/>
+    </row>
+    <row r="124">
+      <c r="B124" s="19"/>
+    </row>
+    <row r="125">
+      <c r="B125" s="19"/>
+    </row>
+    <row r="126">
+      <c r="B126" s="19"/>
+    </row>
+    <row r="127">
+      <c r="B127" s="19"/>
+    </row>
+    <row r="128">
+      <c r="B128" s="19"/>
+    </row>
+    <row r="129">
+      <c r="B129" s="19"/>
+    </row>
+    <row r="130">
+      <c r="B130" s="19"/>
+    </row>
+    <row r="131">
+      <c r="B131" s="19"/>
+    </row>
+    <row r="132">
+      <c r="B132" s="19"/>
+    </row>
+    <row r="133">
+      <c r="B133" s="19"/>
+    </row>
+    <row r="134">
+      <c r="B134" s="19"/>
+    </row>
+    <row r="135">
+      <c r="B135" s="19"/>
+    </row>
+    <row r="136">
+      <c r="B136" s="19"/>
+    </row>
+    <row r="137">
+      <c r="B137" s="19"/>
+    </row>
+    <row r="138">
+      <c r="B138" s="19"/>
+    </row>
+    <row r="139">
+      <c r="B139" s="19"/>
+    </row>
+    <row r="140">
+      <c r="B140" s="19"/>
+    </row>
+    <row r="141">
+      <c r="B141" s="19"/>
+    </row>
+    <row r="142">
+      <c r="B142" s="19"/>
+    </row>
+    <row r="143">
+      <c r="B143" s="19"/>
+    </row>
+    <row r="144">
+      <c r="B144" s="19"/>
+    </row>
+    <row r="145">
+      <c r="B145" s="19"/>
+    </row>
+    <row r="146">
+      <c r="B146" s="19"/>
+    </row>
+    <row r="147">
+      <c r="B147" s="19"/>
+    </row>
+    <row r="148">
+      <c r="B148" s="19"/>
+    </row>
+    <row r="149">
+      <c r="B149" s="19"/>
+    </row>
+    <row r="150">
+      <c r="B150" s="19"/>
+    </row>
+    <row r="151">
+      <c r="B151" s="19"/>
+    </row>
+    <row r="152">
+      <c r="B152" s="19"/>
+    </row>
+    <row r="153">
+      <c r="B153" s="19"/>
+    </row>
+    <row r="154">
+      <c r="B154" s="19"/>
+    </row>
+    <row r="155">
+      <c r="B155" s="19"/>
+    </row>
+    <row r="156">
+      <c r="B156" s="19"/>
+    </row>
+    <row r="157">
+      <c r="B157" s="19"/>
+    </row>
+    <row r="158">
+      <c r="B158" s="19"/>
+    </row>
+    <row r="159">
+      <c r="B159" s="19"/>
+    </row>
+    <row r="160">
+      <c r="B160" s="19"/>
+    </row>
+    <row r="161">
+      <c r="B161" s="19"/>
+    </row>
+    <row r="162">
+      <c r="B162" s="19"/>
+    </row>
+    <row r="163">
+      <c r="B163" s="19"/>
+    </row>
+    <row r="164">
+      <c r="B164" s="19"/>
+    </row>
+    <row r="165">
+      <c r="B165" s="19"/>
+    </row>
+    <row r="166">
+      <c r="B166" s="19"/>
+    </row>
+    <row r="167">
+      <c r="B167" s="19"/>
+    </row>
+    <row r="168">
+      <c r="B168" s="19"/>
+    </row>
+    <row r="169">
+      <c r="B169" s="19"/>
+    </row>
+    <row r="170">
+      <c r="B170" s="19"/>
+    </row>
+    <row r="171">
+      <c r="B171" s="19"/>
+    </row>
+    <row r="172">
+      <c r="B172" s="19"/>
+    </row>
+    <row r="173">
+      <c r="B173" s="19"/>
+    </row>
+    <row r="174">
+      <c r="B174" s="19"/>
+    </row>
+    <row r="175">
+      <c r="B175" s="19"/>
+    </row>
+    <row r="176">
+      <c r="B176" s="19"/>
+    </row>
+    <row r="177">
+      <c r="B177" s="19"/>
+    </row>
+    <row r="178">
+      <c r="B178" s="19"/>
+    </row>
+    <row r="179">
+      <c r="B179" s="19"/>
+    </row>
+    <row r="180">
+      <c r="B180" s="19"/>
+    </row>
+    <row r="181">
+      <c r="B181" s="19"/>
+    </row>
+    <row r="182">
+      <c r="B182" s="19"/>
+    </row>
+    <row r="183">
+      <c r="B183" s="19"/>
+    </row>
+    <row r="184">
+      <c r="B184" s="19"/>
+    </row>
+    <row r="185">
+      <c r="B185" s="19"/>
+    </row>
+    <row r="186">
+      <c r="B186" s="19"/>
+    </row>
+    <row r="187">
+      <c r="B187" s="19"/>
+    </row>
+    <row r="188">
+      <c r="B188" s="19"/>
+    </row>
+    <row r="189">
+      <c r="B189" s="19"/>
+    </row>
+    <row r="190">
+      <c r="B190" s="19"/>
+    </row>
+    <row r="191">
+      <c r="B191" s="19"/>
+    </row>
+    <row r="192">
+      <c r="B192" s="19"/>
+    </row>
+    <row r="193">
+      <c r="B193" s="19"/>
+    </row>
+    <row r="194">
+      <c r="B194" s="19"/>
+    </row>
+    <row r="195">
+      <c r="B195" s="19"/>
+    </row>
+    <row r="196">
+      <c r="B196" s="19"/>
+    </row>
+    <row r="197">
+      <c r="B197" s="19"/>
+    </row>
+    <row r="198">
+      <c r="B198" s="19"/>
+    </row>
+    <row r="199">
+      <c r="B199" s="19"/>
+    </row>
+    <row r="200">
+      <c r="B200" s="19"/>
+    </row>
+    <row r="201">
+      <c r="B201" s="19"/>
+    </row>
+    <row r="202">
+      <c r="B202" s="19"/>
+    </row>
+    <row r="203">
+      <c r="B203" s="19"/>
+    </row>
+    <row r="204">
+      <c r="B204" s="19"/>
+    </row>
+    <row r="205">
+      <c r="B205" s="19"/>
+    </row>
+    <row r="206">
+      <c r="B206" s="19"/>
+    </row>
+    <row r="207">
+      <c r="B207" s="19"/>
+    </row>
+    <row r="208">
+      <c r="B208" s="19"/>
+    </row>
+    <row r="209">
+      <c r="B209" s="19"/>
+    </row>
+    <row r="210">
+      <c r="B210" s="19"/>
+    </row>
+    <row r="211">
+      <c r="B211" s="19"/>
+    </row>
+    <row r="212">
+      <c r="B212" s="19"/>
+    </row>
+    <row r="213">
+      <c r="B213" s="19"/>
+    </row>
+    <row r="214">
+      <c r="B214" s="19"/>
+    </row>
+    <row r="215">
+      <c r="B215" s="19"/>
+    </row>
+    <row r="216">
+      <c r="B216" s="19"/>
+    </row>
+    <row r="217">
+      <c r="B217" s="19"/>
+    </row>
+    <row r="218">
+      <c r="B218" s="19"/>
+    </row>
+    <row r="219">
+      <c r="B219" s="19"/>
+    </row>
+    <row r="220">
+      <c r="B220" s="19"/>
+    </row>
+    <row r="221">
+      <c r="B221" s="19"/>
+    </row>
+    <row r="222">
+      <c r="B222" s="19"/>
+    </row>
+    <row r="223">
+      <c r="B223" s="19"/>
+    </row>
+    <row r="224">
+      <c r="B224" s="19"/>
+    </row>
+    <row r="225">
+      <c r="B225" s="19"/>
+    </row>
+    <row r="226">
+      <c r="B226" s="19"/>
+    </row>
+    <row r="227">
+      <c r="B227" s="19"/>
+    </row>
+    <row r="228">
+      <c r="B228" s="19"/>
+    </row>
+    <row r="229">
+      <c r="B229" s="19"/>
+    </row>
+    <row r="230">
+      <c r="B230" s="19"/>
+    </row>
+    <row r="231">
+      <c r="B231" s="19"/>
+    </row>
+    <row r="232">
+      <c r="B232" s="19"/>
+    </row>
+    <row r="233">
+      <c r="B233" s="19"/>
+    </row>
+    <row r="234">
+      <c r="B234" s="19"/>
+    </row>
+    <row r="235">
+      <c r="B235" s="19"/>
+    </row>
+    <row r="236">
+      <c r="B236" s="19"/>
+    </row>
+    <row r="237">
+      <c r="B237" s="19"/>
+    </row>
+    <row r="238">
+      <c r="B238" s="19"/>
+    </row>
+    <row r="239">
+      <c r="B239" s="19"/>
+    </row>
+    <row r="240">
+      <c r="B240" s="19"/>
+    </row>
+    <row r="241">
+      <c r="B241" s="19"/>
+    </row>
+    <row r="242">
+      <c r="B242" s="19"/>
+    </row>
+    <row r="243">
+      <c r="B243" s="19"/>
+    </row>
+    <row r="244">
+      <c r="B244" s="19"/>
+    </row>
+    <row r="245">
+      <c r="B245" s="19"/>
+    </row>
+    <row r="246">
+      <c r="B246" s="19"/>
+    </row>
+    <row r="247">
+      <c r="B247" s="19"/>
+    </row>
+    <row r="248">
+      <c r="B248" s="19"/>
+    </row>
+    <row r="249">
+      <c r="B249" s="19"/>
+    </row>
+    <row r="250">
+      <c r="B250" s="19"/>
+    </row>
+    <row r="251">
+      <c r="B251" s="19"/>
+    </row>
+    <row r="252">
+      <c r="B252" s="19"/>
+    </row>
+    <row r="253">
+      <c r="B253" s="19"/>
+    </row>
+    <row r="254">
+      <c r="B254" s="19"/>
+    </row>
+    <row r="255">
+      <c r="B255" s="19"/>
+    </row>
+    <row r="256">
+      <c r="B256" s="19"/>
+    </row>
+    <row r="257">
+      <c r="B257" s="19"/>
+    </row>
+    <row r="258">
+      <c r="B258" s="19"/>
+    </row>
+    <row r="259">
+      <c r="B259" s="19"/>
+    </row>
+    <row r="260">
+      <c r="B260" s="19"/>
+    </row>
+    <row r="261">
+      <c r="B261" s="19"/>
+    </row>
+    <row r="262">
+      <c r="B262" s="19"/>
+    </row>
+    <row r="263">
+      <c r="B263" s="19"/>
+    </row>
+    <row r="264">
+      <c r="B264" s="19"/>
+    </row>
+    <row r="265">
+      <c r="B265" s="19"/>
+    </row>
+    <row r="266">
+      <c r="B266" s="19"/>
+    </row>
+    <row r="267">
+      <c r="B267" s="19"/>
+    </row>
+    <row r="268">
+      <c r="B268" s="19"/>
+    </row>
+    <row r="269">
+      <c r="B269" s="19"/>
+    </row>
+    <row r="270">
+      <c r="B270" s="19"/>
+    </row>
+    <row r="271">
+      <c r="B271" s="19"/>
+    </row>
+    <row r="272">
+      <c r="B272" s="19"/>
+    </row>
+    <row r="273">
+      <c r="B273" s="19"/>
+    </row>
+    <row r="274">
+      <c r="B274" s="19"/>
+    </row>
+    <row r="275">
+      <c r="B275" s="19"/>
+    </row>
+    <row r="276">
+      <c r="B276" s="19"/>
+    </row>
+    <row r="277">
+      <c r="B277" s="19"/>
+    </row>
+    <row r="278">
+      <c r="B278" s="19"/>
+    </row>
+    <row r="279">
+      <c r="B279" s="19"/>
+    </row>
+    <row r="280">
+      <c r="B280" s="19"/>
+    </row>
+    <row r="281">
+      <c r="B281" s="19"/>
+    </row>
+    <row r="282">
+      <c r="B282" s="19"/>
+    </row>
+    <row r="283">
+      <c r="B283" s="19"/>
+    </row>
+    <row r="284">
+      <c r="B284" s="19"/>
+    </row>
+    <row r="285">
+      <c r="B285" s="19"/>
+    </row>
+    <row r="286">
+      <c r="B286" s="19"/>
+    </row>
+    <row r="287">
+      <c r="B287" s="19"/>
+    </row>
+    <row r="288">
+      <c r="B288" s="19"/>
+    </row>
+    <row r="289">
+      <c r="B289" s="19"/>
+    </row>
+    <row r="290">
+      <c r="B290" s="19"/>
+    </row>
+    <row r="291">
+      <c r="B291" s="19"/>
+    </row>
+    <row r="292">
+      <c r="B292" s="19"/>
+    </row>
+    <row r="293">
+      <c r="B293" s="19"/>
+    </row>
+    <row r="294">
+      <c r="B294" s="19"/>
+    </row>
+    <row r="295">
+      <c r="B295" s="19"/>
+    </row>
+    <row r="296">
+      <c r="B296" s="19"/>
+    </row>
+    <row r="297">
+      <c r="B297" s="19"/>
+    </row>
+    <row r="298">
+      <c r="B298" s="19"/>
+    </row>
+    <row r="299">
+      <c r="B299" s="19"/>
+    </row>
+    <row r="300">
+      <c r="B300" s="19"/>
+    </row>
+    <row r="301">
+      <c r="B301" s="19"/>
+    </row>
+    <row r="302">
+      <c r="B302" s="19"/>
+    </row>
+    <row r="303">
+      <c r="B303" s="19"/>
+    </row>
+    <row r="304">
+      <c r="B304" s="19"/>
+    </row>
+    <row r="305">
+      <c r="B305" s="19"/>
+    </row>
+    <row r="306">
+      <c r="B306" s="19"/>
+    </row>
+    <row r="307">
+      <c r="B307" s="19"/>
+    </row>
+    <row r="308">
+      <c r="B308" s="19"/>
+    </row>
+    <row r="309">
+      <c r="B309" s="19"/>
+    </row>
+    <row r="310">
+      <c r="B310" s="19"/>
+    </row>
+    <row r="311">
+      <c r="B311" s="19"/>
+    </row>
+    <row r="312">
+      <c r="B312" s="19"/>
+    </row>
+    <row r="313">
+      <c r="B313" s="19"/>
+    </row>
+    <row r="314">
+      <c r="B314" s="19"/>
+    </row>
+    <row r="315">
+      <c r="B315" s="19"/>
+    </row>
+    <row r="316">
+      <c r="B316" s="19"/>
+    </row>
+    <row r="317">
+      <c r="B317" s="19"/>
+    </row>
+    <row r="318">
+      <c r="B318" s="19"/>
+    </row>
+    <row r="319">
+      <c r="B319" s="19"/>
+    </row>
+    <row r="320">
+      <c r="B320" s="19"/>
+    </row>
+    <row r="321">
+      <c r="B321" s="19"/>
+    </row>
+    <row r="322">
+      <c r="B322" s="19"/>
+    </row>
+    <row r="323">
+      <c r="B323" s="19"/>
+    </row>
+    <row r="324">
+      <c r="B324" s="19"/>
+    </row>
+    <row r="325">
+      <c r="B325" s="19"/>
+    </row>
+    <row r="326">
+      <c r="B326" s="19"/>
+    </row>
+    <row r="327">
+      <c r="B327" s="19"/>
+    </row>
+    <row r="328">
+      <c r="B328" s="19"/>
+    </row>
+    <row r="329">
+      <c r="B329" s="19"/>
+    </row>
+    <row r="330">
+      <c r="B330" s="19"/>
+    </row>
+    <row r="331">
+      <c r="B331" s="19"/>
+    </row>
+    <row r="332">
+      <c r="B332" s="19"/>
+    </row>
+    <row r="333">
+      <c r="B333" s="19"/>
+    </row>
+    <row r="334">
+      <c r="B334" s="19"/>
+    </row>
+    <row r="335">
+      <c r="B335" s="19"/>
+    </row>
+    <row r="336">
+      <c r="B336" s="19"/>
+    </row>
+    <row r="337">
+      <c r="B337" s="19"/>
+    </row>
+    <row r="338">
+      <c r="B338" s="19"/>
+    </row>
+    <row r="339">
+      <c r="B339" s="19"/>
+    </row>
+    <row r="340">
+      <c r="B340" s="19"/>
+    </row>
+    <row r="341">
+      <c r="B341" s="19"/>
+    </row>
+    <row r="342">
+      <c r="B342" s="19"/>
+    </row>
+    <row r="343">
+      <c r="B343" s="19"/>
+    </row>
+    <row r="344">
+      <c r="B344" s="19"/>
+    </row>
+    <row r="345">
+      <c r="B345" s="19"/>
+    </row>
+    <row r="346">
+      <c r="B346" s="19"/>
+    </row>
+    <row r="347">
+      <c r="B347" s="19"/>
+    </row>
+    <row r="348">
+      <c r="B348" s="19"/>
+    </row>
+    <row r="349">
+      <c r="B349" s="19"/>
+    </row>
+    <row r="350">
+      <c r="B350" s="19"/>
+    </row>
+    <row r="351">
+      <c r="B351" s="19"/>
+    </row>
+    <row r="352">
+      <c r="B352" s="19"/>
+    </row>
+    <row r="353">
+      <c r="B353" s="19"/>
+    </row>
+    <row r="354">
+      <c r="B354" s="19"/>
+    </row>
+    <row r="355">
+      <c r="B355" s="19"/>
+    </row>
+    <row r="356">
+      <c r="B356" s="19"/>
+    </row>
+    <row r="357">
+      <c r="B357" s="19"/>
+    </row>
+    <row r="358">
+      <c r="B358" s="19"/>
+    </row>
+    <row r="359">
+      <c r="B359" s="19"/>
+    </row>
+    <row r="360">
+      <c r="B360" s="19"/>
+    </row>
+    <row r="361">
+      <c r="B361" s="19"/>
+    </row>
+    <row r="362">
+      <c r="B362" s="19"/>
+    </row>
+    <row r="363">
+      <c r="B363" s="19"/>
+    </row>
+    <row r="364">
+      <c r="B364" s="19"/>
+    </row>
+    <row r="365">
+      <c r="B365" s="19"/>
+    </row>
+    <row r="366">
+      <c r="B366" s="19"/>
+    </row>
+    <row r="367">
+      <c r="B367" s="19"/>
+    </row>
+    <row r="368">
+      <c r="B368" s="19"/>
+    </row>
+    <row r="369">
+      <c r="B369" s="19"/>
+    </row>
+    <row r="370">
+      <c r="B370" s="19"/>
+    </row>
+    <row r="371">
+      <c r="B371" s="19"/>
+    </row>
+    <row r="372">
+      <c r="B372" s="19"/>
+    </row>
+    <row r="373">
+      <c r="B373" s="19"/>
+    </row>
+    <row r="374">
+      <c r="B374" s="19"/>
+    </row>
+    <row r="375">
+      <c r="B375" s="19"/>
+    </row>
+    <row r="376">
+      <c r="B376" s="19"/>
+    </row>
+    <row r="377">
+      <c r="B377" s="19"/>
+    </row>
+    <row r="378">
+      <c r="B378" s="19"/>
+    </row>
+    <row r="379">
+      <c r="B379" s="19"/>
+    </row>
+    <row r="380">
+      <c r="B380" s="19"/>
+    </row>
+    <row r="381">
+      <c r="B381" s="19"/>
+    </row>
+    <row r="382">
+      <c r="B382" s="19"/>
+    </row>
+    <row r="383">
+      <c r="B383" s="19"/>
+    </row>
+    <row r="384">
+      <c r="B384" s="19"/>
+    </row>
+    <row r="385">
+      <c r="B385" s="19"/>
+    </row>
+    <row r="386">
+      <c r="B386" s="19"/>
+    </row>
+    <row r="387">
+      <c r="B387" s="19"/>
+    </row>
+    <row r="388">
+      <c r="B388" s="19"/>
+    </row>
+    <row r="389">
+      <c r="B389" s="19"/>
+    </row>
+    <row r="390">
+      <c r="B390" s="19"/>
+    </row>
+    <row r="391">
+      <c r="B391" s="19"/>
+    </row>
+    <row r="392">
+      <c r="B392" s="19"/>
+    </row>
+    <row r="393">
+      <c r="B393" s="19"/>
+    </row>
+    <row r="394">
+      <c r="B394" s="19"/>
+    </row>
+    <row r="395">
+      <c r="B395" s="19"/>
+    </row>
+    <row r="396">
+      <c r="B396" s="19"/>
+    </row>
+    <row r="397">
+      <c r="B397" s="19"/>
+    </row>
+    <row r="398">
+      <c r="B398" s="19"/>
+    </row>
+    <row r="399">
+      <c r="B399" s="19"/>
+    </row>
+    <row r="400">
+      <c r="B400" s="19"/>
+    </row>
+    <row r="401">
+      <c r="B401" s="19"/>
+    </row>
+    <row r="402">
+      <c r="B402" s="19"/>
+    </row>
+    <row r="403">
+      <c r="B403" s="19"/>
+    </row>
+    <row r="404">
+      <c r="B404" s="19"/>
+    </row>
+    <row r="405">
+      <c r="B405" s="19"/>
+    </row>
+    <row r="406">
+      <c r="B406" s="19"/>
+    </row>
+    <row r="407">
+      <c r="B407" s="19"/>
+    </row>
+    <row r="408">
+      <c r="B408" s="19"/>
+    </row>
+    <row r="409">
+      <c r="B409" s="19"/>
+    </row>
+    <row r="410">
+      <c r="B410" s="19"/>
+    </row>
+    <row r="411">
+      <c r="B411" s="19"/>
+    </row>
+    <row r="412">
+      <c r="B412" s="19"/>
+    </row>
+    <row r="413">
+      <c r="B413" s="19"/>
+    </row>
+    <row r="414">
+      <c r="B414" s="19"/>
+    </row>
+    <row r="415">
+      <c r="B415" s="19"/>
+    </row>
+    <row r="416">
+      <c r="B416" s="19"/>
+    </row>
+    <row r="417">
+      <c r="B417" s="19"/>
+    </row>
+    <row r="418">
+      <c r="B418" s="19"/>
+    </row>
+    <row r="419">
+      <c r="B419" s="19"/>
+    </row>
+    <row r="420">
+      <c r="B420" s="19"/>
+    </row>
+    <row r="421">
+      <c r="B421" s="19"/>
+    </row>
+    <row r="422">
+      <c r="B422" s="19"/>
+    </row>
+    <row r="423">
+      <c r="B423" s="19"/>
+    </row>
+    <row r="424">
+      <c r="B424" s="19"/>
+    </row>
+    <row r="425">
+      <c r="B425" s="19"/>
+    </row>
+    <row r="426">
+      <c r="B426" s="19"/>
+    </row>
+    <row r="427">
+      <c r="B427" s="19"/>
+    </row>
+    <row r="428">
+      <c r="B428" s="19"/>
+    </row>
+    <row r="429">
+      <c r="B429" s="19"/>
+    </row>
+    <row r="430">
+      <c r="B430" s="19"/>
+    </row>
+    <row r="431">
+      <c r="B431" s="19"/>
+    </row>
+    <row r="432">
+      <c r="B432" s="19"/>
+    </row>
+    <row r="433">
+      <c r="B433" s="19"/>
+    </row>
+    <row r="434">
+      <c r="B434" s="19"/>
+    </row>
+    <row r="435">
+      <c r="B435" s="19"/>
+    </row>
+    <row r="436">
+      <c r="B436" s="19"/>
+    </row>
+    <row r="437">
+      <c r="B437" s="19"/>
+    </row>
+    <row r="438">
+      <c r="B438" s="19"/>
+    </row>
+    <row r="439">
+      <c r="B439" s="19"/>
+    </row>
+    <row r="440">
+      <c r="B440" s="19"/>
+    </row>
+    <row r="441">
+      <c r="B441" s="19"/>
+    </row>
+    <row r="442">
+      <c r="B442" s="19"/>
+    </row>
+    <row r="443">
+      <c r="B443" s="19"/>
+    </row>
+    <row r="444">
+      <c r="B444" s="19"/>
+    </row>
+    <row r="445">
+      <c r="B445" s="19"/>
+    </row>
+    <row r="446">
+      <c r="B446" s="19"/>
+    </row>
+    <row r="447">
+      <c r="B447" s="19"/>
+    </row>
+    <row r="448">
+      <c r="B448" s="19"/>
+    </row>
+    <row r="449">
+      <c r="B449" s="19"/>
+    </row>
+    <row r="450">
+      <c r="B450" s="19"/>
+    </row>
+    <row r="451">
+      <c r="B451" s="19"/>
+    </row>
+    <row r="452">
+      <c r="B452" s="19"/>
+    </row>
+    <row r="453">
+      <c r="B453" s="19"/>
+    </row>
+    <row r="454">
+      <c r="B454" s="19"/>
+    </row>
+    <row r="455">
+      <c r="B455" s="19"/>
+    </row>
+    <row r="456">
+      <c r="B456" s="19"/>
+    </row>
+    <row r="457">
+      <c r="B457" s="19"/>
+    </row>
+    <row r="458">
+      <c r="B458" s="19"/>
+    </row>
+    <row r="459">
+      <c r="B459" s="19"/>
+    </row>
+    <row r="460">
+      <c r="B460" s="19"/>
+    </row>
+    <row r="461">
+      <c r="B461" s="19"/>
+    </row>
+    <row r="462">
+      <c r="B462" s="19"/>
+    </row>
+    <row r="463">
+      <c r="B463" s="19"/>
+    </row>
+    <row r="464">
+      <c r="B464" s="19"/>
+    </row>
+    <row r="465">
+      <c r="B465" s="19"/>
+    </row>
+    <row r="466">
+      <c r="B466" s="19"/>
+    </row>
+    <row r="467">
+      <c r="B467" s="19"/>
+    </row>
+    <row r="468">
+      <c r="B468" s="19"/>
+    </row>
+    <row r="469">
+      <c r="B469" s="19"/>
+    </row>
+    <row r="470">
+      <c r="B470" s="19"/>
+    </row>
+    <row r="471">
+      <c r="B471" s="19"/>
+    </row>
+    <row r="472">
+      <c r="B472" s="19"/>
+    </row>
+    <row r="473">
+      <c r="B473" s="19"/>
+    </row>
+    <row r="474">
+      <c r="B474" s="19"/>
+    </row>
+    <row r="475">
+      <c r="B475" s="19"/>
+    </row>
+    <row r="476">
+      <c r="B476" s="19"/>
+    </row>
+    <row r="477">
+      <c r="B477" s="19"/>
+    </row>
+    <row r="478">
+      <c r="B478" s="19"/>
+    </row>
+    <row r="479">
+      <c r="B479" s="19"/>
+    </row>
+    <row r="480">
+      <c r="B480" s="19"/>
+    </row>
+    <row r="481">
+      <c r="B481" s="19"/>
+    </row>
+    <row r="482">
+      <c r="B482" s="19"/>
+    </row>
+    <row r="483">
+      <c r="B483" s="19"/>
+    </row>
+    <row r="484">
+      <c r="B484" s="19"/>
+    </row>
+    <row r="485">
+      <c r="B485" s="19"/>
+    </row>
+    <row r="486">
+      <c r="B486" s="19"/>
+    </row>
+    <row r="487">
+      <c r="B487" s="19"/>
+    </row>
+    <row r="488">
+      <c r="B488" s="19"/>
+    </row>
+    <row r="489">
+      <c r="B489" s="19"/>
+    </row>
+    <row r="490">
+      <c r="B490" s="19"/>
+    </row>
+    <row r="491">
+      <c r="B491" s="19"/>
+    </row>
+    <row r="492">
+      <c r="B492" s="19"/>
+    </row>
+    <row r="493">
+      <c r="B493" s="19"/>
+    </row>
+    <row r="494">
+      <c r="B494" s="19"/>
+    </row>
+    <row r="495">
+      <c r="B495" s="19"/>
+    </row>
+    <row r="496">
+      <c r="B496" s="19"/>
+    </row>
+    <row r="497">
+      <c r="B497" s="19"/>
+    </row>
+    <row r="498">
+      <c r="B498" s="19"/>
+    </row>
+    <row r="499">
+      <c r="B499" s="19"/>
+    </row>
+    <row r="500">
+      <c r="B500" s="19"/>
+    </row>
+    <row r="501">
+      <c r="B501" s="19"/>
+    </row>
+    <row r="502">
+      <c r="B502" s="19"/>
+    </row>
+    <row r="503">
+      <c r="B503" s="19"/>
+    </row>
+    <row r="504">
+      <c r="B504" s="19"/>
+    </row>
+    <row r="505">
+      <c r="B505" s="19"/>
+    </row>
+    <row r="506">
+      <c r="B506" s="19"/>
+    </row>
+    <row r="507">
+      <c r="B507" s="19"/>
+    </row>
+    <row r="508">
+      <c r="B508" s="19"/>
+    </row>
+    <row r="509">
+      <c r="B509" s="19"/>
+    </row>
+    <row r="510">
+      <c r="B510" s="19"/>
+    </row>
+    <row r="511">
+      <c r="B511" s="19"/>
+    </row>
+    <row r="512">
+      <c r="B512" s="19"/>
+    </row>
+    <row r="513">
+      <c r="B513" s="19"/>
+    </row>
+    <row r="514">
+      <c r="B514" s="19"/>
+    </row>
+    <row r="515">
+      <c r="B515" s="19"/>
+    </row>
+    <row r="516">
+      <c r="B516" s="19"/>
+    </row>
+    <row r="517">
+      <c r="B517" s="19"/>
+    </row>
+    <row r="518">
+      <c r="B518" s="19"/>
+    </row>
+    <row r="519">
+      <c r="B519" s="19"/>
+    </row>
+    <row r="520">
+      <c r="B520" s="19"/>
+    </row>
+    <row r="521">
+      <c r="B521" s="19"/>
+    </row>
+    <row r="522">
+      <c r="B522" s="19"/>
+    </row>
+    <row r="523">
+      <c r="B523" s="19"/>
+    </row>
+    <row r="524">
+      <c r="B524" s="19"/>
+    </row>
+    <row r="525">
+      <c r="B525" s="19"/>
+    </row>
+    <row r="526">
+      <c r="B526" s="19"/>
+    </row>
+    <row r="527">
+      <c r="B527" s="19"/>
+    </row>
+    <row r="528">
+      <c r="B528" s="19"/>
+    </row>
+    <row r="529">
+      <c r="B529" s="19"/>
+    </row>
+    <row r="530">
+      <c r="B530" s="19"/>
+    </row>
+    <row r="531">
+      <c r="B531" s="19"/>
+    </row>
+    <row r="532">
+      <c r="B532" s="19"/>
+    </row>
+    <row r="533">
+      <c r="B533" s="19"/>
+    </row>
+    <row r="534">
+      <c r="B534" s="19"/>
+    </row>
+    <row r="535">
+      <c r="B535" s="19"/>
+    </row>
+    <row r="536">
+      <c r="B536" s="19"/>
+    </row>
+    <row r="537">
+      <c r="B537" s="19"/>
+    </row>
+    <row r="538">
+      <c r="B538" s="19"/>
+    </row>
+    <row r="539">
+      <c r="B539" s="19"/>
+    </row>
+    <row r="540">
+      <c r="B540" s="19"/>
+    </row>
+    <row r="541">
+      <c r="B541" s="19"/>
+    </row>
+    <row r="542">
+      <c r="B542" s="19"/>
+    </row>
+    <row r="543">
+      <c r="B543" s="19"/>
+    </row>
+    <row r="544">
+      <c r="B544" s="19"/>
+    </row>
+    <row r="545">
+      <c r="B545" s="19"/>
+    </row>
+    <row r="546">
+      <c r="B546" s="19"/>
+    </row>
+    <row r="547">
+      <c r="B547" s="19"/>
+    </row>
+    <row r="548">
+      <c r="B548" s="19"/>
+    </row>
+    <row r="549">
+      <c r="B549" s="19"/>
+    </row>
+    <row r="550">
+      <c r="B550" s="19"/>
+    </row>
+    <row r="551">
+      <c r="B551" s="19"/>
+    </row>
+    <row r="552">
+      <c r="B552" s="19"/>
+    </row>
+    <row r="553">
+      <c r="B553" s="19"/>
+    </row>
+    <row r="554">
+      <c r="B554" s="19"/>
+    </row>
+    <row r="555">
+      <c r="B555" s="19"/>
+    </row>
+    <row r="556">
+      <c r="B556" s="19"/>
+    </row>
+    <row r="557">
+      <c r="B557" s="19"/>
+    </row>
+    <row r="558">
+      <c r="B558" s="19"/>
+    </row>
+    <row r="559">
+      <c r="B559" s="19"/>
+    </row>
+    <row r="560">
+      <c r="B560" s="19"/>
+    </row>
+    <row r="561">
+      <c r="B561" s="19"/>
+    </row>
+    <row r="562">
+      <c r="B562" s="19"/>
+    </row>
+    <row r="563">
+      <c r="B563" s="19"/>
+    </row>
+    <row r="564">
+      <c r="B564" s="19"/>
+    </row>
+    <row r="565">
+      <c r="B565" s="19"/>
+    </row>
+    <row r="566">
+      <c r="B566" s="19"/>
+    </row>
+    <row r="567">
+      <c r="B567" s="19"/>
+    </row>
+    <row r="568">
+      <c r="B568" s="19"/>
+    </row>
+    <row r="569">
+      <c r="B569" s="19"/>
+    </row>
+    <row r="570">
+      <c r="B570" s="19"/>
+    </row>
+    <row r="571">
+      <c r="B571" s="19"/>
+    </row>
+    <row r="572">
+      <c r="B572" s="19"/>
+    </row>
+    <row r="573">
+      <c r="B573" s="19"/>
+    </row>
+    <row r="574">
+      <c r="B574" s="19"/>
+    </row>
+    <row r="575">
+      <c r="B575" s="19"/>
+    </row>
+    <row r="576">
+      <c r="B576" s="19"/>
+    </row>
+    <row r="577">
+      <c r="B577" s="19"/>
+    </row>
+    <row r="578">
+      <c r="B578" s="19"/>
+    </row>
+    <row r="579">
+      <c r="B579" s="19"/>
+    </row>
+    <row r="580">
+      <c r="B580" s="19"/>
+    </row>
+    <row r="581">
+      <c r="B581" s="19"/>
+    </row>
+    <row r="582">
+      <c r="B582" s="19"/>
+    </row>
+    <row r="583">
+      <c r="B583" s="19"/>
+    </row>
+    <row r="584">
+      <c r="B584" s="19"/>
+    </row>
+    <row r="585">
+      <c r="B585" s="19"/>
+    </row>
+    <row r="586">
+      <c r="B586" s="19"/>
+    </row>
+    <row r="587">
+      <c r="B587" s="19"/>
+    </row>
+    <row r="588">
+      <c r="B588" s="19"/>
+    </row>
+    <row r="589">
+      <c r="B589" s="19"/>
+    </row>
+    <row r="590">
+      <c r="B590" s="19"/>
+    </row>
+    <row r="591">
+      <c r="B591" s="19"/>
+    </row>
+    <row r="592">
+      <c r="B592" s="19"/>
+    </row>
+    <row r="593">
+      <c r="B593" s="19"/>
+    </row>
+    <row r="594">
+      <c r="B594" s="19"/>
+    </row>
+    <row r="595">
+      <c r="B595" s="19"/>
+    </row>
+    <row r="596">
+      <c r="B596" s="19"/>
+    </row>
+    <row r="597">
+      <c r="B597" s="19"/>
+    </row>
+    <row r="598">
+      <c r="B598" s="19"/>
+    </row>
+    <row r="599">
+      <c r="B599" s="19"/>
+    </row>
+    <row r="600">
+      <c r="B600" s="19"/>
+    </row>
+    <row r="601">
+      <c r="B601" s="19"/>
+    </row>
+    <row r="602">
+      <c r="B602" s="19"/>
+    </row>
+    <row r="603">
+      <c r="B603" s="19"/>
+    </row>
+    <row r="604">
+      <c r="B604" s="19"/>
+    </row>
+    <row r="605">
+      <c r="B605" s="19"/>
+    </row>
+    <row r="606">
+      <c r="B606" s="19"/>
+    </row>
+    <row r="607">
+      <c r="B607" s="19"/>
+    </row>
+    <row r="608">
+      <c r="B608" s="19"/>
+    </row>
+    <row r="609">
+      <c r="B609" s="19"/>
+    </row>
+    <row r="610">
+      <c r="B610" s="19"/>
+    </row>
+    <row r="611">
+      <c r="B611" s="19"/>
+    </row>
+    <row r="612">
+      <c r="B612" s="19"/>
+    </row>
+    <row r="613">
+      <c r="B613" s="19"/>
+    </row>
+    <row r="614">
+      <c r="B614" s="19"/>
+    </row>
+    <row r="615">
+      <c r="B615" s="19"/>
+    </row>
+    <row r="616">
+      <c r="B616" s="19"/>
+    </row>
+    <row r="617">
+      <c r="B617" s="19"/>
+    </row>
+    <row r="618">
+      <c r="B618" s="19"/>
+    </row>
+    <row r="619">
+      <c r="B619" s="19"/>
+    </row>
+    <row r="620">
+      <c r="B620" s="19"/>
+    </row>
+    <row r="621">
+      <c r="B621" s="19"/>
+    </row>
+    <row r="622">
+      <c r="B622" s="19"/>
+    </row>
+    <row r="623">
+      <c r="B623" s="19"/>
+    </row>
+    <row r="624">
+      <c r="B624" s="19"/>
+    </row>
+    <row r="625">
+      <c r="B625" s="19"/>
+    </row>
+    <row r="626">
+      <c r="B626" s="19"/>
+    </row>
+    <row r="627">
+      <c r="B627" s="19"/>
+    </row>
+    <row r="628">
+      <c r="B628" s="19"/>
+    </row>
+    <row r="629">
+      <c r="B629" s="19"/>
+    </row>
+    <row r="630">
+      <c r="B630" s="19"/>
+    </row>
+    <row r="631">
+      <c r="B631" s="19"/>
+    </row>
+    <row r="632">
+      <c r="B632" s="19"/>
+    </row>
+    <row r="633">
+      <c r="B633" s="19"/>
+    </row>
+    <row r="634">
+      <c r="B634" s="19"/>
+    </row>
+    <row r="635">
+      <c r="B635" s="19"/>
+    </row>
+    <row r="636">
+      <c r="B636" s="19"/>
+    </row>
+    <row r="637">
+      <c r="B637" s="19"/>
+    </row>
+    <row r="638">
+      <c r="B638" s="19"/>
+    </row>
+    <row r="639">
+      <c r="B639" s="19"/>
+    </row>
+    <row r="640">
+      <c r="B640" s="19"/>
+    </row>
+    <row r="641">
+      <c r="B641" s="19"/>
+    </row>
+    <row r="642">
+      <c r="B642" s="19"/>
+    </row>
+    <row r="643">
+      <c r="B643" s="19"/>
+    </row>
+    <row r="644">
+      <c r="B644" s="19"/>
+    </row>
+    <row r="645">
+      <c r="B645" s="19"/>
+    </row>
+    <row r="646">
+      <c r="B646" s="19"/>
+    </row>
+    <row r="647">
+      <c r="B647" s="19"/>
+    </row>
+    <row r="648">
+      <c r="B648" s="19"/>
+    </row>
+    <row r="649">
+      <c r="B649" s="19"/>
+    </row>
+    <row r="650">
+      <c r="B650" s="19"/>
+    </row>
+    <row r="651">
+      <c r="B651" s="19"/>
+    </row>
+    <row r="652">
+      <c r="B652" s="19"/>
+    </row>
+    <row r="653">
+      <c r="B653" s="19"/>
+    </row>
+    <row r="654">
+      <c r="B654" s="19"/>
+    </row>
+    <row r="655">
+      <c r="B655" s="19"/>
+    </row>
+    <row r="656">
+      <c r="B656" s="19"/>
+    </row>
+    <row r="657">
+      <c r="B657" s="19"/>
+    </row>
+    <row r="658">
+      <c r="B658" s="19"/>
+    </row>
+    <row r="659">
+      <c r="B659" s="19"/>
+    </row>
+    <row r="660">
+      <c r="B660" s="19"/>
+    </row>
+    <row r="661">
+      <c r="B661" s="19"/>
+    </row>
+    <row r="662">
+      <c r="B662" s="19"/>
+    </row>
+    <row r="663">
+      <c r="B663" s="19"/>
+    </row>
+    <row r="664">
+      <c r="B664" s="19"/>
+    </row>
+    <row r="665">
+      <c r="B665" s="19"/>
+    </row>
+    <row r="666">
+      <c r="B666" s="19"/>
+    </row>
+    <row r="667">
+      <c r="B667" s="19"/>
+    </row>
+    <row r="668">
+      <c r="B668" s="19"/>
+    </row>
+    <row r="669">
+      <c r="B669" s="19"/>
+    </row>
+    <row r="670">
+      <c r="B670" s="19"/>
+    </row>
+    <row r="671">
+      <c r="B671" s="19"/>
+    </row>
+    <row r="672">
+      <c r="B672" s="19"/>
+    </row>
+    <row r="673">
+      <c r="B673" s="19"/>
+    </row>
+    <row r="674">
+      <c r="B674" s="19"/>
+    </row>
+    <row r="675">
+      <c r="B675" s="19"/>
+    </row>
+    <row r="676">
+      <c r="B676" s="19"/>
+    </row>
+    <row r="677">
+      <c r="B677" s="19"/>
+    </row>
+    <row r="678">
+      <c r="B678" s="19"/>
+    </row>
+    <row r="679">
+      <c r="B679" s="19"/>
+    </row>
+    <row r="680">
+      <c r="B680" s="19"/>
+    </row>
+    <row r="681">
+      <c r="B681" s="19"/>
+    </row>
+    <row r="682">
+      <c r="B682" s="19"/>
+    </row>
+    <row r="683">
+      <c r="B683" s="19"/>
+    </row>
+    <row r="684">
+      <c r="B684" s="19"/>
+    </row>
+    <row r="685">
+      <c r="B685" s="19"/>
+    </row>
+    <row r="686">
+      <c r="B686" s="19"/>
+    </row>
+    <row r="687">
+      <c r="B687" s="19"/>
+    </row>
+    <row r="688">
+      <c r="B688" s="19"/>
+    </row>
+    <row r="689">
+      <c r="B689" s="19"/>
+    </row>
+    <row r="690">
+      <c r="B690" s="19"/>
+    </row>
+    <row r="691">
+      <c r="B691" s="19"/>
+    </row>
+    <row r="692">
+      <c r="B692" s="19"/>
+    </row>
+    <row r="693">
+      <c r="B693" s="19"/>
+    </row>
+    <row r="694">
+      <c r="B694" s="19"/>
+    </row>
+    <row r="695">
+      <c r="B695" s="19"/>
+    </row>
+    <row r="696">
+      <c r="B696" s="19"/>
+    </row>
+    <row r="697">
+      <c r="B697" s="19"/>
+    </row>
+    <row r="698">
+      <c r="B698" s="19"/>
+    </row>
+    <row r="699">
+      <c r="B699" s="19"/>
+    </row>
+    <row r="700">
+      <c r="B700" s="19"/>
+    </row>
+    <row r="701">
+      <c r="B701" s="19"/>
+    </row>
+    <row r="702">
+      <c r="B702" s="19"/>
+    </row>
+    <row r="703">
+      <c r="B703" s="19"/>
+    </row>
+    <row r="704">
+      <c r="B704" s="19"/>
+    </row>
+    <row r="705">
+      <c r="B705" s="19"/>
+    </row>
+    <row r="706">
+      <c r="B706" s="19"/>
+    </row>
+    <row r="707">
+      <c r="B707" s="19"/>
+    </row>
+    <row r="708">
+      <c r="B708" s="19"/>
+    </row>
+    <row r="709">
+      <c r="B709" s="19"/>
+    </row>
+    <row r="710">
+      <c r="B710" s="19"/>
+    </row>
+    <row r="711">
+      <c r="B711" s="19"/>
+    </row>
+    <row r="712">
+      <c r="B712" s="19"/>
+    </row>
+    <row r="713">
+      <c r="B713" s="19"/>
+    </row>
+    <row r="714">
+      <c r="B714" s="19"/>
+    </row>
+    <row r="715">
+      <c r="B715" s="19"/>
+    </row>
+    <row r="716">
+      <c r="B716" s="19"/>
+    </row>
+    <row r="717">
+      <c r="B717" s="19"/>
+    </row>
+    <row r="718">
+      <c r="B718" s="19"/>
+    </row>
+    <row r="719">
+      <c r="B719" s="19"/>
+    </row>
+    <row r="720">
+      <c r="B720" s="19"/>
+    </row>
+    <row r="721">
+      <c r="B721" s="19"/>
+    </row>
+    <row r="722">
+      <c r="B722" s="19"/>
+    </row>
+    <row r="723">
+      <c r="B723" s="19"/>
+    </row>
+    <row r="724">
+      <c r="B724" s="19"/>
+    </row>
+    <row r="725">
+      <c r="B725" s="19"/>
+    </row>
+    <row r="726">
+      <c r="B726" s="19"/>
+    </row>
+    <row r="727">
+      <c r="B727" s="19"/>
+    </row>
+    <row r="728">
+      <c r="B728" s="19"/>
+    </row>
+    <row r="729">
+      <c r="B729" s="19"/>
+    </row>
+    <row r="730">
+      <c r="B730" s="19"/>
+    </row>
+    <row r="731">
+      <c r="B731" s="19"/>
+    </row>
+    <row r="732">
+      <c r="B732" s="19"/>
+    </row>
+    <row r="733">
+      <c r="B733" s="19"/>
+    </row>
+    <row r="734">
+      <c r="B734" s="19"/>
+    </row>
+    <row r="735">
+      <c r="B735" s="19"/>
+    </row>
+    <row r="736">
+      <c r="B736" s="19"/>
+    </row>
+    <row r="737">
+      <c r="B737" s="19"/>
+    </row>
+    <row r="738">
+      <c r="B738" s="19"/>
+    </row>
+    <row r="739">
+      <c r="B739" s="19"/>
+    </row>
+    <row r="740">
+      <c r="B740" s="19"/>
+    </row>
+    <row r="741">
+      <c r="B741" s="19"/>
+    </row>
+    <row r="742">
+      <c r="B742" s="19"/>
+    </row>
+    <row r="743">
+      <c r="B743" s="19"/>
+    </row>
+    <row r="744">
+      <c r="B744" s="19"/>
+    </row>
+    <row r="745">
+      <c r="B745" s="19"/>
+    </row>
+    <row r="746">
+      <c r="B746" s="19"/>
+    </row>
+    <row r="747">
+      <c r="B747" s="19"/>
+    </row>
+    <row r="748">
+      <c r="B748" s="19"/>
+    </row>
+    <row r="749">
+      <c r="B749" s="19"/>
+    </row>
+    <row r="750">
+      <c r="B750" s="19"/>
+    </row>
+    <row r="751">
+      <c r="B751" s="19"/>
+    </row>
+    <row r="752">
+      <c r="B752" s="19"/>
+    </row>
+    <row r="753">
+      <c r="B753" s="19"/>
+    </row>
+    <row r="754">
+      <c r="B754" s="19"/>
+    </row>
+    <row r="755">
+      <c r="B755" s="19"/>
+    </row>
+    <row r="756">
+      <c r="B756" s="19"/>
+    </row>
+    <row r="757">
+      <c r="B757" s="19"/>
+    </row>
+    <row r="758">
+      <c r="B758" s="19"/>
+    </row>
+    <row r="759">
+      <c r="B759" s="19"/>
+    </row>
+    <row r="760">
+      <c r="B760" s="19"/>
+    </row>
+    <row r="761">
+      <c r="B761" s="19"/>
+    </row>
+    <row r="762">
+      <c r="B762" s="19"/>
+    </row>
+    <row r="763">
+      <c r="B763" s="19"/>
+    </row>
+    <row r="764">
+      <c r="B764" s="19"/>
+    </row>
+    <row r="765">
+      <c r="B765" s="19"/>
+    </row>
+    <row r="766">
+      <c r="B766" s="19"/>
+    </row>
+    <row r="767">
+      <c r="B767" s="19"/>
+    </row>
+    <row r="768">
+      <c r="B768" s="19"/>
+    </row>
+    <row r="769">
+      <c r="B769" s="19"/>
+    </row>
+    <row r="770">
+      <c r="B770" s="19"/>
+    </row>
+    <row r="771">
+      <c r="B771" s="19"/>
+    </row>
+    <row r="772">
+      <c r="B772" s="19"/>
+    </row>
+    <row r="773">
+      <c r="B773" s="19"/>
+    </row>
+    <row r="774">
+      <c r="B774" s="19"/>
+    </row>
+    <row r="775">
+      <c r="B775" s="19"/>
+    </row>
+    <row r="776">
+      <c r="B776" s="19"/>
+    </row>
+    <row r="777">
+      <c r="B777" s="19"/>
+    </row>
+    <row r="778">
+      <c r="B778" s="19"/>
+    </row>
+    <row r="779">
+      <c r="B779" s="19"/>
+    </row>
+    <row r="780">
+      <c r="B780" s="19"/>
+    </row>
+    <row r="781">
+      <c r="B781" s="19"/>
+    </row>
+    <row r="782">
+      <c r="B782" s="19"/>
+    </row>
+    <row r="783">
+      <c r="B783" s="19"/>
+    </row>
+    <row r="784">
+      <c r="B784" s="19"/>
+    </row>
+    <row r="785">
+      <c r="B785" s="19"/>
+    </row>
+    <row r="786">
+      <c r="B786" s="19"/>
+    </row>
+    <row r="787">
+      <c r="B787" s="19"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="K2:K5 N2:N5">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$M2="deprecated"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K5 N2:N5">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$M2="changed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K5 N2:N5">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>$M2="proposed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K5 N2:N5">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>$M2="accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:AD1 A6:AD116">
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>$M1="accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>